<commit_message>
add screenshots of model
</commit_message>
<xml_diff>
--- a/Covid19_Germany_Estimates/Corona_Deutschland_Modellierung_08-03-2020.xlsx
+++ b/Covid19_Germany_Estimates/Corona_Deutschland_Modellierung_08-03-2020.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benni\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benni\Desktop\Covid19_Germany_Estimates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53A5385-F31A-4B3C-870B-B1687B8E7E66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABD1C6A-F24A-4493-952D-A488062A564B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{8F2FD530-AE1D-479B-B999-25EE25C3C974}"/>
   </bookViews>
@@ -6810,8 +6810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75855736-B2B6-4FFD-943C-E355D55A5C8E}">
   <dimension ref="A2:R39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AQ27" sqref="AQ27"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P39" sqref="P39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6945,7 +6945,7 @@
         <v>43889</v>
       </c>
       <c r="N15" s="5">
-        <f>H21</f>
+        <f t="shared" ref="N15:N33" si="0">H21</f>
         <v>344.26113175388667</v>
       </c>
     </row>
@@ -6960,18 +6960,18 @@
         <v>72</v>
       </c>
       <c r="H16" s="5">
-        <f t="shared" ref="H16:H39" si="0" xml:space="preserve"> $B$6* ((($B$6/$B$7)*C16+$B$8)^$B$7)^$B$9</f>
+        <f t="shared" ref="H16:H39" si="1" xml:space="preserve"> $B$6* ((($B$6/$B$7)*C16+$B$8)^$B$7)^$B$9</f>
         <v>72.830392953399539</v>
       </c>
       <c r="K16" s="5">
-        <f t="shared" ref="K16:K23" si="1">(H16 - F16) ^2</f>
+        <f t="shared" ref="K16:K23" si="2">(H16 - F16) ^2</f>
         <v>0.68955245705560841</v>
       </c>
       <c r="M16" s="1">
         <v>43890</v>
       </c>
       <c r="N16" s="5">
-        <f>H22</f>
+        <f t="shared" si="0"/>
         <v>468.53321368898429</v>
       </c>
     </row>
@@ -6986,18 +6986,18 @@
         <v>117</v>
       </c>
       <c r="H17" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>99.5273462880089</v>
       </c>
       <c r="K17" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>305.29362773915636</v>
       </c>
       <c r="M17" s="1">
         <v>43891</v>
       </c>
       <c r="N17" s="5">
-        <f>H23</f>
+        <f t="shared" si="0"/>
         <v>637.15173917596223</v>
       </c>
     </row>
@@ -7012,18 +7012,18 @@
         <v>130</v>
       </c>
       <c r="H18" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>135.89796505337185</v>
       </c>
       <c r="K18" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>34.78599177079559</v>
       </c>
       <c r="M18" s="1">
         <v>43892</v>
       </c>
       <c r="N18" s="5">
-        <f>H24</f>
+        <f t="shared" si="0"/>
         <v>865.75954196380235</v>
       </c>
     </row>
@@ -7038,18 +7038,18 @@
         <v>188</v>
       </c>
       <c r="H19" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>185.40700493350903</v>
       </c>
       <c r="K19" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.7236234148465153</v>
       </c>
       <c r="M19" s="1">
         <v>43893</v>
       </c>
       <c r="N19" s="5">
-        <f>H25</f>
+        <f t="shared" si="0"/>
         <v>1175.4534499539066</v>
       </c>
     </row>
@@ -7064,18 +7064,18 @@
         <v>240</v>
       </c>
       <c r="H20" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>252.74575017092192</v>
       </c>
       <c r="K20" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>162.45414741955622</v>
       </c>
       <c r="M20" s="1">
         <v>43894</v>
       </c>
       <c r="N20" s="5">
-        <f>H26</f>
+        <f t="shared" si="0"/>
         <v>1594.6637193547194</v>
       </c>
     </row>
@@ -7090,18 +7090,18 @@
         <v>351</v>
       </c>
       <c r="H21" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>344.26113175388667</v>
       </c>
       <c r="K21" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>45.412345238474508</v>
       </c>
       <c r="M21" s="1">
         <v>43895</v>
       </c>
       <c r="N21" s="5">
-        <f>H27</f>
+        <f t="shared" si="0"/>
         <v>2161.6735319038671</v>
       </c>
     </row>
@@ -7116,18 +7116,18 @@
         <v>670</v>
       </c>
       <c r="H22" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>468.53321368898429</v>
       </c>
       <c r="K22" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40588.865986488468</v>
       </c>
       <c r="M22" s="1">
         <v>43896</v>
       </c>
       <c r="N22" s="5">
-        <f>H28</f>
+        <f t="shared" si="0"/>
         <v>2927.9939677097495</v>
       </c>
     </row>
@@ -7142,18 +7142,18 @@
         <v>684</v>
       </c>
       <c r="H23" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>637.15173917596223</v>
       </c>
       <c r="K23" s="5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2194.7595422370719</v>
       </c>
       <c r="M23" s="1">
         <v>43897</v>
       </c>
       <c r="N23" s="5">
-        <f>H29</f>
+        <f t="shared" si="0"/>
         <v>3962.8815037882409</v>
       </c>
     </row>
@@ -7165,14 +7165,14 @@
         <v>9</v>
       </c>
       <c r="H24" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>865.75954196380235</v>
       </c>
       <c r="M24" s="1">
         <v>43898</v>
       </c>
       <c r="N24" s="5">
-        <f>H30</f>
+        <f t="shared" si="0"/>
         <v>5359.3802655189411</v>
       </c>
     </row>
@@ -7184,14 +7184,14 @@
         <v>10</v>
       </c>
       <c r="H25" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1175.4534499539066</v>
       </c>
       <c r="M25" s="1">
         <v>43899</v>
       </c>
       <c r="N25" s="5">
-        <f>H31</f>
+        <f t="shared" si="0"/>
         <v>7242.3976171645536</v>
       </c>
     </row>
@@ -7203,14 +7203,14 @@
         <v>11</v>
       </c>
       <c r="H26" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1594.6637193547194</v>
       </c>
       <c r="M26" s="1">
         <v>43900</v>
       </c>
       <c r="N26" s="5">
-        <f>H32</f>
+        <f t="shared" si="0"/>
         <v>9779.4893114971201</v>
       </c>
     </row>
@@ -7222,14 +7222,14 @@
         <v>12</v>
       </c>
       <c r="H27" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2161.6735319038671</v>
       </c>
       <c r="M27" s="1">
         <v>43901</v>
       </c>
       <c r="N27" s="5">
-        <f>H33</f>
+        <f t="shared" si="0"/>
         <v>13195.25264830535</v>
       </c>
     </row>
@@ -7241,14 +7241,14 @@
         <v>13</v>
       </c>
       <c r="H28" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2927.9939677097495</v>
       </c>
       <c r="M28" s="1">
         <v>43902</v>
       </c>
       <c r="N28" s="5">
-        <f>H34</f>
+        <f t="shared" si="0"/>
         <v>17790.520485216766</v>
       </c>
     </row>
@@ -7260,14 +7260,14 @@
         <v>14</v>
       </c>
       <c r="H29" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3962.8815037882409</v>
       </c>
       <c r="M29" s="1">
         <v>43903</v>
       </c>
       <c r="N29" s="5">
-        <f>H35</f>
+        <f t="shared" si="0"/>
         <v>23967.938654969657</v>
       </c>
     </row>
@@ -7279,14 +7279,14 @@
         <v>15</v>
       </c>
       <c r="H30" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5359.3802655189411</v>
       </c>
       <c r="M30" s="1">
         <v>43904</v>
       </c>
       <c r="N30" s="5">
-        <f>H36</f>
+        <f t="shared" si="0"/>
         <v>32266.024863121762</v>
       </c>
     </row>
@@ -7298,14 +7298,14 @@
         <v>16</v>
       </c>
       <c r="H31" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7242.3976171645536</v>
       </c>
       <c r="M31" s="1">
         <v>43905</v>
       </c>
       <c r="N31" s="5">
-        <f>H37</f>
+        <f t="shared" si="0"/>
         <v>43404.488598377131</v>
       </c>
     </row>
@@ -7317,14 +7317,14 @@
         <v>17</v>
       </c>
       <c r="H32" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>9779.4893114971201</v>
       </c>
       <c r="M32" s="1">
         <v>43906</v>
       </c>
       <c r="N32" s="5">
-        <f>H38</f>
+        <f t="shared" si="0"/>
         <v>58344.491759452074</v>
       </c>
     </row>
@@ -7336,14 +7336,14 @@
         <v>18</v>
       </c>
       <c r="H33" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>13195.25264830535</v>
       </c>
       <c r="M33" s="1">
         <v>43907</v>
       </c>
       <c r="N33" s="5">
-        <f>H39</f>
+        <f t="shared" si="0"/>
         <v>78368.717945830896</v>
       </c>
     </row>
@@ -7355,7 +7355,7 @@
         <v>19</v>
       </c>
       <c r="H34" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17790.520485216766</v>
       </c>
       <c r="N34" s="5"/>
@@ -7369,7 +7369,7 @@
         <v>20</v>
       </c>
       <c r="H35" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23967.938654969657</v>
       </c>
       <c r="N35" s="5"/>
@@ -7383,7 +7383,7 @@
         <v>21</v>
       </c>
       <c r="H36" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>32266.024863121762</v>
       </c>
       <c r="N36" s="5"/>
@@ -7397,7 +7397,7 @@
         <v>22</v>
       </c>
       <c r="H37" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>43404.488598377131</v>
       </c>
       <c r="N37" s="5"/>
@@ -7411,7 +7411,7 @@
         <v>23</v>
       </c>
       <c r="H38" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>58344.491759452074</v>
       </c>
       <c r="N38" s="5"/>
@@ -7425,7 +7425,7 @@
         <v>24</v>
       </c>
       <c r="H39" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>78368.717945830896</v>
       </c>
       <c r="N39" s="5"/>

</xml_diff>

<commit_message>
Update model with new data of 824 confirmed cases
</commit_message>
<xml_diff>
--- a/Covid19_Germany_Estimates/Corona_Deutschland_Modellierung_08-03-2020.xlsx
+++ b/Covid19_Germany_Estimates/Corona_Deutschland_Modellierung_08-03-2020.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benni\Desktop\Covid19_Germany_Estimates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8ABD1C6A-F24A-4493-952D-A488062A564B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8500F73D-D116-40EE-8332-68BE8183C8A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="4" xr2:uid="{8F2FD530-AE1D-479B-B999-25EE25C3C974}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{8F2FD530-AE1D-479B-B999-25EE25C3C974}"/>
   </bookViews>
   <sheets>
     <sheet name="Feasibility Report 1" sheetId="2" r:id="rId1"/>
@@ -547,31 +547,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="1">
-                  <c:v>48</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>117</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>130</c:v>
+                  <c:v>188</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>188</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>240</c:v>
+                  <c:v>351</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>351</c:v>
+                  <c:v>670</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>670</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>684</c:v>
+                  <c:v>824</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -672,37 +669,37 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="1">
-                  <c:v>53.250259223419413</c:v>
+                  <c:v>60.03665445359055</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72.830392953399539</c:v>
+                  <c:v>88.004346184969961</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>99.5273462880089</c:v>
+                  <c:v>128.84383413497102</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>135.89796505337185</c:v>
+                  <c:v>188.40758769140396</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>185.40700493350903</c:v>
+                  <c:v>275.1767162789738</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>252.74575017092192</c:v>
+                  <c:v>401.42721219784983</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>344.26113175388667</c:v>
+                  <c:v>584.90727019055851</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>468.53321368898429</c:v>
+                  <c:v>851.24688887121363</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>637.15173917596223</c:v>
+                  <c:v>1237.415514999318</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>865.75954196380235</c:v>
+                  <c:v>1796.677962523303</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1175.4534499539066</c:v>
+                  <c:v>2605.6898627877044</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1187,79 +1184,79 @@
               <c:strCache>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>28.02.2020</c:v>
+                  <c:v>2/28/2020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.02.2020</c:v>
+                  <c:v>2/29/2020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>01.03.2020</c:v>
+                  <c:v>3/1/2020</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>02.03.2020</c:v>
+                  <c:v>3/2/2020</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>03.03.2020</c:v>
+                  <c:v>3/3/2020</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>04.03.2020</c:v>
+                  <c:v>3/4/2020</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>05.03.2020</c:v>
+                  <c:v>3/5/2020</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>06.03.2020</c:v>
+                  <c:v>3/6/2020</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>07.03.2020</c:v>
+                  <c:v>3/7/2020</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>08.03.2020</c:v>
+                  <c:v>3/8/2020</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>09.03.2020</c:v>
+                  <c:v>3/9/2020</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10.03.2020</c:v>
+                  <c:v>3/10/2020</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.03.2020</c:v>
+                  <c:v>3/11/2020</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12.03.2020</c:v>
+                  <c:v>3/12/2020</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>13.03.2020</c:v>
+                  <c:v>3/13/2020</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14.03.2020</c:v>
+                  <c:v>3/14/2020</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.03.2020</c:v>
+                  <c:v>3/15/2020</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16.03.2020</c:v>
+                  <c:v>3/16/2020</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>17.03.2020</c:v>
+                  <c:v>3/17/2020</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>18.03.2020</c:v>
+                  <c:v>3/18/2020</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>19.03.2020</c:v>
+                  <c:v>3/19/2020</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>20.03.2020</c:v>
+                  <c:v>3/20/2020</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>21.03.2020</c:v>
+                  <c:v>3/21/2020</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>22.03.2020</c:v>
+                  <c:v>3/22/2020</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>23.03.2020</c:v>
+                  <c:v>3/23/2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1271,31 +1268,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>48</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>117</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>130</c:v>
+                  <c:v>188</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>188</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>240</c:v>
+                  <c:v>351</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>351</c:v>
+                  <c:v>670</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>670</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>684</c:v>
+                  <c:v>824</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1339,79 +1333,79 @@
               <c:strCache>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>28.02.2020</c:v>
+                  <c:v>2/28/2020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.02.2020</c:v>
+                  <c:v>2/29/2020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>01.03.2020</c:v>
+                  <c:v>3/1/2020</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>02.03.2020</c:v>
+                  <c:v>3/2/2020</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>03.03.2020</c:v>
+                  <c:v>3/3/2020</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>04.03.2020</c:v>
+                  <c:v>3/4/2020</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>05.03.2020</c:v>
+                  <c:v>3/5/2020</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>06.03.2020</c:v>
+                  <c:v>3/6/2020</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>07.03.2020</c:v>
+                  <c:v>3/7/2020</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>08.03.2020</c:v>
+                  <c:v>3/8/2020</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>09.03.2020</c:v>
+                  <c:v>3/9/2020</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10.03.2020</c:v>
+                  <c:v>3/10/2020</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.03.2020</c:v>
+                  <c:v>3/11/2020</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12.03.2020</c:v>
+                  <c:v>3/12/2020</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>13.03.2020</c:v>
+                  <c:v>3/13/2020</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14.03.2020</c:v>
+                  <c:v>3/14/2020</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.03.2020</c:v>
+                  <c:v>3/15/2020</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16.03.2020</c:v>
+                  <c:v>3/16/2020</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>17.03.2020</c:v>
+                  <c:v>3/17/2020</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>18.03.2020</c:v>
+                  <c:v>3/18/2020</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>19.03.2020</c:v>
+                  <c:v>3/19/2020</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>20.03.2020</c:v>
+                  <c:v>3/20/2020</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>21.03.2020</c:v>
+                  <c:v>3/21/2020</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>22.03.2020</c:v>
+                  <c:v>3/22/2020</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>23.03.2020</c:v>
+                  <c:v>3/23/2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1423,79 +1417,79 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>53.250259223419413</c:v>
+                  <c:v>60.03665445359055</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72.830392953399539</c:v>
+                  <c:v>88.004346184969961</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>99.5273462880089</c:v>
+                  <c:v>128.84383413497102</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>135.89796505337185</c:v>
+                  <c:v>188.40758769140396</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>185.40700493350903</c:v>
+                  <c:v>275.1767162789738</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>252.74575017092192</c:v>
+                  <c:v>401.42721219784983</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>344.26113175388667</c:v>
+                  <c:v>584.90727019055851</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>468.53321368898429</c:v>
+                  <c:v>851.24688887121363</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>637.15173917596223</c:v>
+                  <c:v>1237.415514999318</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>865.75954196380235</c:v>
+                  <c:v>1796.677962523303</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1175.4534499539066</c:v>
+                  <c:v>2605.6898627877044</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1594.6637193547194</c:v>
+                  <c:v>3774.6449670409188</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2161.6735319038671</c:v>
+                  <c:v>5461.7708455292295</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2927.9939677097495</c:v>
+                  <c:v>7894.0135581646546</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3962.8815037882409</c:v>
+                  <c:v>11396.521348685739</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5359.3802655189411</c:v>
+                  <c:v>16434.624598062568</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7242.3976171645536</c:v>
+                  <c:v>23673.543707643767</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9779.4893114971201</c:v>
+                  <c:v>34063.219972164021</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13195.25264830535</c:v>
+                  <c:v>48958.711448690585</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>17790.520485216766</c:v>
+                  <c:v>70290.88270668473</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>23967.938654969657</c:v>
+                  <c:v>100808.14248154381</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>32266.024863121762</c:v>
+                  <c:v>144418.44275233176</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43404.488598377131</c:v>
+                  <c:v>206672.61801561838</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>58344.491759452074</c:v>
+                  <c:v>295446.76871714654</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>78368.717945830896</c:v>
+                  <c:v>421904.66386981081</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1541,79 +1535,79 @@
               <c:strCache>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>28.02.2020</c:v>
+                  <c:v>2/28/2020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.02.2020</c:v>
+                  <c:v>2/29/2020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>01.03.2020</c:v>
+                  <c:v>3/1/2020</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>02.03.2020</c:v>
+                  <c:v>3/2/2020</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>03.03.2020</c:v>
+                  <c:v>3/3/2020</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>04.03.2020</c:v>
+                  <c:v>3/4/2020</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>05.03.2020</c:v>
+                  <c:v>3/5/2020</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>06.03.2020</c:v>
+                  <c:v>3/6/2020</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>07.03.2020</c:v>
+                  <c:v>3/7/2020</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>08.03.2020</c:v>
+                  <c:v>3/8/2020</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>09.03.2020</c:v>
+                  <c:v>3/9/2020</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10.03.2020</c:v>
+                  <c:v>3/10/2020</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.03.2020</c:v>
+                  <c:v>3/11/2020</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12.03.2020</c:v>
+                  <c:v>3/12/2020</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>13.03.2020</c:v>
+                  <c:v>3/13/2020</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14.03.2020</c:v>
+                  <c:v>3/14/2020</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.03.2020</c:v>
+                  <c:v>3/15/2020</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16.03.2020</c:v>
+                  <c:v>3/16/2020</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>17.03.2020</c:v>
+                  <c:v>3/17/2020</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>18.03.2020</c:v>
+                  <c:v>3/18/2020</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>19.03.2020</c:v>
+                  <c:v>3/19/2020</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>20.03.2020</c:v>
+                  <c:v>3/20/2020</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>21.03.2020</c:v>
+                  <c:v>3/21/2020</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>22.03.2020</c:v>
+                  <c:v>3/22/2020</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>23.03.2020</c:v>
+                  <c:v>3/23/2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1625,61 +1619,61 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>344.26113175388667</c:v>
+                  <c:v>584.90727019055851</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>468.53321368898429</c:v>
+                  <c:v>851.24688887121363</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>637.15173917596223</c:v>
+                  <c:v>1237.415514999318</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>865.75954196380235</c:v>
+                  <c:v>1796.677962523303</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1175.4534499539066</c:v>
+                  <c:v>2605.6898627877044</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1594.6637193547194</c:v>
+                  <c:v>3774.6449670409188</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2161.6735319038671</c:v>
+                  <c:v>5461.7708455292295</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2927.9939677097495</c:v>
+                  <c:v>7894.0135581646546</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3962.8815037882409</c:v>
+                  <c:v>11396.521348685739</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5359.3802655189411</c:v>
+                  <c:v>16434.624598062568</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7242.3976171645536</c:v>
+                  <c:v>23673.543707643767</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9779.4893114971201</c:v>
+                  <c:v>34063.219972164021</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13195.25264830535</c:v>
+                  <c:v>48958.711448690585</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>17790.520485216766</c:v>
+                  <c:v>70290.88270668473</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>23967.938654969657</c:v>
+                  <c:v>100808.14248154381</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>32266.024863121762</c:v>
+                  <c:v>144418.44275233176</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43404.488598377131</c:v>
+                  <c:v>206672.61801561838</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>58344.491759452074</c:v>
+                  <c:v>295446.76871714654</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>78368.717945830896</c:v>
+                  <c:v>421904.66386981081</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2272,31 +2266,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>48</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72</c:v>
+                  <c:v>117</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>117</c:v>
+                  <c:v>130</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>130</c:v>
+                  <c:v>188</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>188</c:v>
+                  <c:v>240</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>240</c:v>
+                  <c:v>351</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>351</c:v>
+                  <c:v>670</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>670</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>684</c:v>
+                  <c:v>824</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2462,79 +2453,79 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>53.250259223419413</c:v>
+                  <c:v>60.03665445359055</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72.830392953399539</c:v>
+                  <c:v>88.004346184969961</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>99.5273462880089</c:v>
+                  <c:v>128.84383413497102</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>135.89796505337185</c:v>
+                  <c:v>188.40758769140396</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>185.40700493350903</c:v>
+                  <c:v>275.1767162789738</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>252.74575017092192</c:v>
+                  <c:v>401.42721219784983</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>344.26113175388667</c:v>
+                  <c:v>584.90727019055851</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>468.53321368898429</c:v>
+                  <c:v>851.24688887121363</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>637.15173917596223</c:v>
+                  <c:v>1237.415514999318</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>865.75954196380235</c:v>
+                  <c:v>1796.677962523303</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1175.4534499539066</c:v>
+                  <c:v>2605.6898627877044</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1594.6637193547194</c:v>
+                  <c:v>3774.6449670409188</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2161.6735319038671</c:v>
+                  <c:v>5461.7708455292295</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2927.9939677097495</c:v>
+                  <c:v>7894.0135581646546</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3962.8815037882409</c:v>
+                  <c:v>11396.521348685739</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5359.3802655189411</c:v>
+                  <c:v>16434.624598062568</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7242.3976171645536</c:v>
+                  <c:v>23673.543707643767</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9779.4893114971201</c:v>
+                  <c:v>34063.219972164021</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>13195.25264830535</c:v>
+                  <c:v>48958.711448690585</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>17790.520485216766</c:v>
+                  <c:v>70290.88270668473</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>23967.938654969657</c:v>
+                  <c:v>100808.14248154381</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>32266.024863121762</c:v>
+                  <c:v>144418.44275233176</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>43404.488598377131</c:v>
+                  <c:v>206672.61801561838</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>58344.491759452074</c:v>
+                  <c:v>295446.76871714654</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>78368.717945830896</c:v>
+                  <c:v>421904.66386981081</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2702,61 +2693,61 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>344.26113175388667</c:v>
+                  <c:v>584.90727019055851</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>468.53321368898429</c:v>
+                  <c:v>851.24688887121363</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>637.15173917596223</c:v>
+                  <c:v>1237.415514999318</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>865.75954196380235</c:v>
+                  <c:v>1796.677962523303</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1175.4534499539066</c:v>
+                  <c:v>2605.6898627877044</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1594.6637193547194</c:v>
+                  <c:v>3774.6449670409188</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2161.6735319038671</c:v>
+                  <c:v>5461.7708455292295</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2927.9939677097495</c:v>
+                  <c:v>7894.0135581646546</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3962.8815037882409</c:v>
+                  <c:v>11396.521348685739</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5359.3802655189411</c:v>
+                  <c:v>16434.624598062568</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7242.3976171645536</c:v>
+                  <c:v>23673.543707643767</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>9779.4893114971201</c:v>
+                  <c:v>34063.219972164021</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13195.25264830535</c:v>
+                  <c:v>48958.711448690585</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>17790.520485216766</c:v>
+                  <c:v>70290.88270668473</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>23967.938654969657</c:v>
+                  <c:v>100808.14248154381</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>32266.024863121762</c:v>
+                  <c:v>144418.44275233176</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>43404.488598377131</c:v>
+                  <c:v>206672.61801561838</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>58344.491759452074</c:v>
+                  <c:v>295446.76871714654</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>78368.717945830896</c:v>
+                  <c:v>421904.66386981081</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3254,61 +3245,61 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>344.26113175388667</c:v>
+                  <c:v>584.90727019055851</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>468.53321368898429</c:v>
+                  <c:v>851.24688887121363</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>637.15173917596223</c:v>
+                  <c:v>1237.415514999318</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>865.75954196380235</c:v>
+                  <c:v>1796.677962523303</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1175.4534499539066</c:v>
+                  <c:v>2605.6898627877044</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1594.6637193547194</c:v>
+                  <c:v>3774.6449670409188</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2161.6735319038671</c:v>
+                  <c:v>5461.7708455292295</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2927.9939677097495</c:v>
+                  <c:v>7894.0135581646546</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3962.8815037882409</c:v>
+                  <c:v>11396.521348685739</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5359.3802655189411</c:v>
+                  <c:v>16434.624598062568</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7242.3976171645536</c:v>
+                  <c:v>23673.543707643767</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9779.4893114971201</c:v>
+                  <c:v>34063.219972164021</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>13195.25264830535</c:v>
+                  <c:v>48958.711448690585</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>17790.520485216766</c:v>
+                  <c:v>70290.88270668473</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>23967.938654969657</c:v>
+                  <c:v>100808.14248154381</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>32266.024863121762</c:v>
+                  <c:v>144418.44275233176</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>43404.488598377131</c:v>
+                  <c:v>206672.61801561838</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>58344.491759452074</c:v>
+                  <c:v>295446.76871714654</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>78368.717945830896</c:v>
+                  <c:v>421904.66386981081</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6811,14 +6802,17 @@
   <dimension ref="A2:R39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P39" sqref="P39"/>
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7109375" customWidth="1"/>
     <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.5703125" customWidth="1"/>
     <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6865,7 +6859,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="17">
-        <v>0.33070115162887759</v>
+        <v>0.58595469351715701</v>
       </c>
       <c r="D6" s="16" t="s">
         <v>5</v>
@@ -6878,11 +6872,11 @@
         <v>8</v>
       </c>
       <c r="B7" s="16">
-        <v>118.78222542515427</v>
-      </c>
-      <c r="D7" s="16">
-        <f>SUM(K15:K21)</f>
-        <v>582.92450995298543</v>
+        <v>176.4510567799318</v>
+      </c>
+      <c r="D7" s="17">
+        <f>SUM(K15:K22)</f>
+        <v>12748.843141858775</v>
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
@@ -6892,7 +6886,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="16">
-        <v>1.0441597081842038</v>
+        <v>1.0393701324990459</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -6900,7 +6894,7 @@
         <v>11</v>
       </c>
       <c r="B9" s="16">
-        <v>0.99</v>
+        <v>0.67944147424124168</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -6931,22 +6925,22 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>48</v>
+        <v>72</v>
       </c>
       <c r="H15" s="5">
         <f xml:space="preserve"> $B$6* ((($B$6/$B$7)*C15+$B$8)^$B$7)^$B$9</f>
-        <v>53.250259223419413</v>
+        <v>60.03665445359055</v>
       </c>
       <c r="K15" s="5">
-        <f>(H15 - F15) ^2</f>
-        <v>27.565221913100611</v>
+        <f>(H15 -F15) ^2</f>
+        <v>143.1216366627948</v>
       </c>
       <c r="M15" s="1">
         <v>43889</v>
       </c>
       <c r="N15" s="5">
         <f t="shared" ref="N15:N33" si="0">H21</f>
-        <v>344.26113175388667</v>
+        <v>584.90727019055851</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -6957,22 +6951,22 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <v>72</v>
+        <v>117</v>
       </c>
       <c r="H16" s="5">
         <f t="shared" ref="H16:H39" si="1" xml:space="preserve"> $B$6* ((($B$6/$B$7)*C16+$B$8)^$B$7)^$B$9</f>
-        <v>72.830392953399539</v>
+        <v>88.004346184969961</v>
       </c>
       <c r="K16" s="5">
-        <f t="shared" ref="K16:K23" si="2">(H16 - F16) ^2</f>
-        <v>0.68955245705560841</v>
+        <f>(H16 -F16) ^2</f>
+        <v>840.74794016106603</v>
       </c>
       <c r="M16" s="1">
         <v>43890</v>
       </c>
       <c r="N16" s="5">
         <f t="shared" si="0"/>
-        <v>468.53321368898429</v>
+        <v>851.24688887121363</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
@@ -6983,22 +6977,22 @@
         <v>2</v>
       </c>
       <c r="F17">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="H17" s="5">
         <f t="shared" si="1"/>
-        <v>99.5273462880089</v>
+        <v>128.84383413497102</v>
       </c>
       <c r="K17" s="5">
-        <f t="shared" si="2"/>
-        <v>305.29362773915636</v>
+        <f>(H17 -F17) ^2</f>
+        <v>1.336719507458213</v>
       </c>
       <c r="M17" s="1">
         <v>43891</v>
       </c>
       <c r="N17" s="5">
         <f t="shared" si="0"/>
-        <v>637.15173917596223</v>
+        <v>1237.415514999318</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
@@ -7009,22 +7003,22 @@
         <v>3</v>
       </c>
       <c r="F18">
-        <v>130</v>
+        <v>188</v>
       </c>
       <c r="H18" s="5">
         <f t="shared" si="1"/>
-        <v>135.89796505337185</v>
+        <v>188.40758769140396</v>
       </c>
       <c r="K18" s="5">
-        <f t="shared" si="2"/>
-        <v>34.78599177079559</v>
+        <f>(H18 -F18) ^2</f>
+        <v>0.16612772618401064</v>
       </c>
       <c r="M18" s="1">
         <v>43892</v>
       </c>
       <c r="N18" s="5">
         <f t="shared" si="0"/>
-        <v>865.75954196380235</v>
+        <v>1796.677962523303</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
@@ -7035,22 +7029,22 @@
         <v>4</v>
       </c>
       <c r="F19">
-        <v>188</v>
+        <v>240</v>
       </c>
       <c r="H19" s="5">
         <f t="shared" si="1"/>
-        <v>185.40700493350903</v>
+        <v>275.1767162789738</v>
       </c>
       <c r="K19" s="5">
-        <f t="shared" si="2"/>
-        <v>6.7236234148465153</v>
+        <f>(H19 -F19) ^2</f>
+        <v>1237.4013681714202</v>
       </c>
       <c r="M19" s="1">
         <v>43893</v>
       </c>
       <c r="N19" s="5">
         <f t="shared" si="0"/>
-        <v>1175.4534499539066</v>
+        <v>2605.6898627877044</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -7061,22 +7055,22 @@
         <v>5</v>
       </c>
       <c r="F20">
-        <v>240</v>
+        <v>351</v>
       </c>
       <c r="H20" s="5">
         <f t="shared" si="1"/>
-        <v>252.74575017092192</v>
+        <v>401.42721219784983</v>
       </c>
       <c r="K20" s="5">
-        <f t="shared" si="2"/>
-        <v>162.45414741955622</v>
+        <f>(H20 -F20) ^2</f>
+        <v>2542.9037300469745</v>
       </c>
       <c r="M20" s="1">
         <v>43894</v>
       </c>
       <c r="N20" s="5">
         <f t="shared" si="0"/>
-        <v>1594.6637193547194</v>
+        <v>3774.6449670409188</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -7087,22 +7081,22 @@
         <v>6</v>
       </c>
       <c r="F21">
-        <v>351</v>
+        <v>670</v>
       </c>
       <c r="H21" s="5">
         <f t="shared" si="1"/>
-        <v>344.26113175388667</v>
+        <v>584.90727019055851</v>
       </c>
       <c r="K21" s="5">
-        <f t="shared" si="2"/>
-        <v>45.412345238474508</v>
+        <f>(H21 -F21) ^2</f>
+        <v>7240.7726664226129</v>
       </c>
       <c r="M21" s="1">
         <v>43895</v>
       </c>
       <c r="N21" s="5">
         <f t="shared" si="0"/>
-        <v>2161.6735319038671</v>
+        <v>5461.7708455292295</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -7113,22 +7107,22 @@
         <v>7</v>
       </c>
       <c r="F22">
-        <v>670</v>
+        <v>824</v>
       </c>
       <c r="H22" s="5">
         <f t="shared" si="1"/>
-        <v>468.53321368898429</v>
+        <v>851.24688887121363</v>
       </c>
       <c r="K22" s="5">
-        <f t="shared" si="2"/>
-        <v>40588.865986488468</v>
+        <f>(H22 -F22) ^2</f>
+        <v>742.39295316026505</v>
       </c>
       <c r="M22" s="1">
         <v>43896</v>
       </c>
       <c r="N22" s="5">
         <f t="shared" si="0"/>
-        <v>2927.9939677097495</v>
+        <v>7894.0135581646546</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -7138,23 +7132,17 @@
       <c r="C23">
         <v>8</v>
       </c>
-      <c r="F23">
-        <v>684</v>
-      </c>
       <c r="H23" s="5">
         <f t="shared" si="1"/>
-        <v>637.15173917596223</v>
-      </c>
-      <c r="K23" s="5">
-        <f t="shared" si="2"/>
-        <v>2194.7595422370719</v>
-      </c>
+        <v>1237.415514999318</v>
+      </c>
+      <c r="K23" s="5"/>
       <c r="M23" s="1">
         <v>43897</v>
       </c>
       <c r="N23" s="5">
         <f t="shared" si="0"/>
-        <v>3962.8815037882409</v>
+        <v>11396.521348685739</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -7166,14 +7154,14 @@
       </c>
       <c r="H24" s="5">
         <f t="shared" si="1"/>
-        <v>865.75954196380235</v>
+        <v>1796.677962523303</v>
       </c>
       <c r="M24" s="1">
         <v>43898</v>
       </c>
       <c r="N24" s="5">
         <f t="shared" si="0"/>
-        <v>5359.3802655189411</v>
+        <v>16434.624598062568</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -7185,14 +7173,14 @@
       </c>
       <c r="H25" s="5">
         <f t="shared" si="1"/>
-        <v>1175.4534499539066</v>
+        <v>2605.6898627877044</v>
       </c>
       <c r="M25" s="1">
         <v>43899</v>
       </c>
       <c r="N25" s="5">
         <f t="shared" si="0"/>
-        <v>7242.3976171645536</v>
+        <v>23673.543707643767</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -7204,14 +7192,14 @@
       </c>
       <c r="H26" s="5">
         <f t="shared" si="1"/>
-        <v>1594.6637193547194</v>
+        <v>3774.6449670409188</v>
       </c>
       <c r="M26" s="1">
         <v>43900</v>
       </c>
       <c r="N26" s="5">
         <f t="shared" si="0"/>
-        <v>9779.4893114971201</v>
+        <v>34063.219972164021</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -7223,14 +7211,14 @@
       </c>
       <c r="H27" s="5">
         <f t="shared" si="1"/>
-        <v>2161.6735319038671</v>
+        <v>5461.7708455292295</v>
       </c>
       <c r="M27" s="1">
         <v>43901</v>
       </c>
       <c r="N27" s="5">
         <f t="shared" si="0"/>
-        <v>13195.25264830535</v>
+        <v>48958.711448690585</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -7242,14 +7230,14 @@
       </c>
       <c r="H28" s="5">
         <f t="shared" si="1"/>
-        <v>2927.9939677097495</v>
+        <v>7894.0135581646546</v>
       </c>
       <c r="M28" s="1">
         <v>43902</v>
       </c>
       <c r="N28" s="5">
         <f t="shared" si="0"/>
-        <v>17790.520485216766</v>
+        <v>70290.88270668473</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -7261,14 +7249,14 @@
       </c>
       <c r="H29" s="5">
         <f t="shared" si="1"/>
-        <v>3962.8815037882409</v>
+        <v>11396.521348685739</v>
       </c>
       <c r="M29" s="1">
         <v>43903</v>
       </c>
       <c r="N29" s="5">
         <f t="shared" si="0"/>
-        <v>23967.938654969657</v>
+        <v>100808.14248154381</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -7280,14 +7268,14 @@
       </c>
       <c r="H30" s="5">
         <f t="shared" si="1"/>
-        <v>5359.3802655189411</v>
+        <v>16434.624598062568</v>
       </c>
       <c r="M30" s="1">
         <v>43904</v>
       </c>
       <c r="N30" s="5">
         <f t="shared" si="0"/>
-        <v>32266.024863121762</v>
+        <v>144418.44275233176</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -7299,14 +7287,14 @@
       </c>
       <c r="H31" s="5">
         <f t="shared" si="1"/>
-        <v>7242.3976171645536</v>
+        <v>23673.543707643767</v>
       </c>
       <c r="M31" s="1">
         <v>43905</v>
       </c>
       <c r="N31" s="5">
         <f t="shared" si="0"/>
-        <v>43404.488598377131</v>
+        <v>206672.61801561838</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -7318,14 +7306,14 @@
       </c>
       <c r="H32" s="5">
         <f t="shared" si="1"/>
-        <v>9779.4893114971201</v>
+        <v>34063.219972164021</v>
       </c>
       <c r="M32" s="1">
         <v>43906</v>
       </c>
       <c r="N32" s="5">
         <f t="shared" si="0"/>
-        <v>58344.491759452074</v>
+        <v>295446.76871714654</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -7337,14 +7325,14 @@
       </c>
       <c r="H33" s="5">
         <f t="shared" si="1"/>
-        <v>13195.25264830535</v>
+        <v>48958.711448690585</v>
       </c>
       <c r="M33" s="1">
         <v>43907</v>
       </c>
       <c r="N33" s="5">
         <f t="shared" si="0"/>
-        <v>78368.717945830896</v>
+        <v>421904.66386981081</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -7356,7 +7344,7 @@
       </c>
       <c r="H34" s="5">
         <f t="shared" si="1"/>
-        <v>17790.520485216766</v>
+        <v>70290.88270668473</v>
       </c>
       <c r="N34" s="5"/>
       <c r="O34" s="1"/>
@@ -7370,7 +7358,7 @@
       </c>
       <c r="H35" s="5">
         <f t="shared" si="1"/>
-        <v>23967.938654969657</v>
+        <v>100808.14248154381</v>
       </c>
       <c r="N35" s="5"/>
       <c r="O35" s="1"/>
@@ -7384,7 +7372,7 @@
       </c>
       <c r="H36" s="5">
         <f t="shared" si="1"/>
-        <v>32266.024863121762</v>
+        <v>144418.44275233176</v>
       </c>
       <c r="N36" s="5"/>
       <c r="O36" s="1"/>
@@ -7398,7 +7386,7 @@
       </c>
       <c r="H37" s="5">
         <f t="shared" si="1"/>
-        <v>43404.488598377131</v>
+        <v>206672.61801561838</v>
       </c>
       <c r="N37" s="5"/>
       <c r="O37" s="1"/>
@@ -7412,7 +7400,7 @@
       </c>
       <c r="H38" s="5">
         <f t="shared" si="1"/>
-        <v>58344.491759452074</v>
+        <v>295446.76871714654</v>
       </c>
       <c r="N38" s="5"/>
       <c r="O38" s="1"/>
@@ -7426,7 +7414,7 @@
       </c>
       <c r="H39" s="5">
         <f t="shared" si="1"/>
-        <v>78368.717945830896</v>
+        <v>421904.66386981081</v>
       </c>
       <c r="N39" s="5"/>
       <c r="O39" s="1"/>

</xml_diff>

<commit_message>
Update Model with more sane estimates on case doubling rate
</commit_message>
<xml_diff>
--- a/Covid19_Germany_Estimates/Corona_Deutschland_Modellierung_08-03-2020.xlsx
+++ b/Covid19_Germany_Estimates/Corona_Deutschland_Modellierung_08-03-2020.xlsx
@@ -8,69 +8,65 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benni\Desktop\Covid19_Germany_Estimates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8500F73D-D116-40EE-8332-68BE8183C8A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAAC4FD-B895-4771-953F-7ACBB7457B00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="4" xr2:uid="{8F2FD530-AE1D-479B-B999-25EE25C3C974}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8F2FD530-AE1D-479B-B999-25EE25C3C974}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feasibility Report 1" sheetId="2" r:id="rId1"/>
-    <sheet name="Feasibility Report 2" sheetId="3" r:id="rId2"/>
-    <sheet name="Answer Report 1" sheetId="4" r:id="rId3"/>
-    <sheet name="Sensitivity Report 1" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId5"/>
+    <sheet name="Polynomial-Exponential Growth" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="4" hidden="1">Sheet1!$B$6:$B$9</definedName>
-    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
-    <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_eng" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="4" hidden="1">Sheet1!$B$6</definedName>
-    <definedName name="solver_lhs2" localSheetId="4" hidden="1">Sheet1!$B$6</definedName>
-    <definedName name="solver_lhs3" localSheetId="4" hidden="1">Sheet1!$B$7</definedName>
-    <definedName name="solver_lhs4" localSheetId="4" hidden="1">Sheet1!$B$7</definedName>
-    <definedName name="solver_lhs5" localSheetId="4" hidden="1">Sheet1!$B$8</definedName>
-    <definedName name="solver_lhs6" localSheetId="4" hidden="1">Sheet1!$B$8</definedName>
-    <definedName name="solver_lhs7" localSheetId="4" hidden="1">Sheet1!$B$9</definedName>
-    <definedName name="solver_lhs8" localSheetId="4" hidden="1">Sheet1!$B$9</definedName>
-    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
-    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
-    <definedName name="solver_msl" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="4" hidden="1">8</definedName>
-    <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="4" hidden="1">Sheet1!$D$7</definedName>
-    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
-    <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="4" hidden="1">3</definedName>
-    <definedName name="solver_rel3" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_rel4" localSheetId="4" hidden="1">3</definedName>
-    <definedName name="solver_rel5" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_rel6" localSheetId="4" hidden="1">3</definedName>
-    <definedName name="solver_rel7" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_rel8" localSheetId="4" hidden="1">3</definedName>
-    <definedName name="solver_rhs1" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_rhs2" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_rhs3" localSheetId="4" hidden="1">200</definedName>
-    <definedName name="solver_rhs4" localSheetId="4" hidden="1">90</definedName>
-    <definedName name="solver_rhs5" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_rhs6" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_rhs7" localSheetId="4" hidden="1">0.99</definedName>
-    <definedName name="solver_rhs8" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
-    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
-    <definedName name="solver_typ" localSheetId="4" hidden="1">2</definedName>
-    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
-    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$6:$B$9</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$6</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$6</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$7</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$7</definedName>
+    <definedName name="solver_lhs5" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$8</definedName>
+    <definedName name="solver_lhs6" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$8</definedName>
+    <definedName name="solver_lhs7" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$9</definedName>
+    <definedName name="solver_lhs8" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$9</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">8</definedName>
+    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$D$7</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel6" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel7" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel8" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">40</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">20</definedName>
+    <definedName name="solver_rhs5" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rhs6" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs7" localSheetId="0" hidden="1">0.35</definedName>
+    <definedName name="solver_rhs8" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -90,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Bestätigte Fälle</t>
   </si>
@@ -128,155 +124,20 @@
     <t>p</t>
   </si>
   <si>
-    <t>Microsoft Excel 16.0 Feasibility Report</t>
+    <t>Modellierung einer Vorhersage des Covid19 Verlaufs in Deutschland durch GRG Nonlinear mit Multistart Global Minimum Suche</t>
   </si>
   <si>
-    <t>Worksheet: [Corona_Deutschland_Modellierung.xlsx]Sheet1</t>
+    <t>Wirkliche Fälle mit Lag = 3 Tage zwischen Infektiösität und Bestätigung</t>
   </si>
   <si>
-    <t>Report Created: 07.03.2020 13:13:34</t>
-  </si>
-  <si>
-    <t>Constraints Which Make the Problem Infeasible</t>
-  </si>
-  <si>
-    <t>Cell</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Cell Value</t>
-  </si>
-  <si>
-    <t>Formula</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Slack</t>
-  </si>
-  <si>
-    <t>Constraints (not including Variable Bounds) Which Make the Problem Infeasible</t>
-  </si>
-  <si>
-    <t>Microsoft Excel 16.0 Answer Report</t>
-  </si>
-  <si>
-    <t>Report Created: 07.03.2020 13:52:22</t>
-  </si>
-  <si>
-    <t>Result: Solver found a solution.  All Constraints and optimality conditions are satisfied.</t>
-  </si>
-  <si>
-    <t>Solver Engine</t>
-  </si>
-  <si>
-    <t>Engine: GRG Nonlinear</t>
-  </si>
-  <si>
-    <t>Solution Time: 0,015 Seconds.</t>
-  </si>
-  <si>
-    <t>Iterations: 1 Subproblems: 0</t>
-  </si>
-  <si>
-    <t>Solver Options</t>
-  </si>
-  <si>
-    <t>Max Time Unlimited,  Iterations Unlimited, Precision 0,000001</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Convergence 0,0001, Population Size 100, Random Seed 0, Derivatives Forward, Require Bounds</t>
-  </si>
-  <si>
-    <t>Max Subproblems Unlimited, Max Integer Sols Unlimited, Integer Tolerance 1%, Assume NonNegative</t>
-  </si>
-  <si>
-    <t>Objective Cell (Min)</t>
-  </si>
-  <si>
-    <t>Original Value</t>
-  </si>
-  <si>
-    <t>Final Value</t>
-  </si>
-  <si>
-    <t>Variable Cells</t>
-  </si>
-  <si>
-    <t>Integer</t>
-  </si>
-  <si>
-    <t>Constraints</t>
-  </si>
-  <si>
-    <t>$D$7</t>
-  </si>
-  <si>
-    <t>m Summe Quadratischer Fehler</t>
-  </si>
-  <si>
-    <t>$B$6</t>
-  </si>
-  <si>
-    <t>r Fallzahl = r(((r/m)*t + A)^m ) ^p</t>
-  </si>
-  <si>
-    <t>Contin</t>
-  </si>
-  <si>
-    <t>$B$7</t>
-  </si>
-  <si>
-    <t>m Fallzahl = r(((r/m)*t + A)^m ) ^p</t>
-  </si>
-  <si>
-    <t>$B$8</t>
-  </si>
-  <si>
-    <t>a Fallzahl = r(((r/m)*t + A)^m ) ^p</t>
-  </si>
-  <si>
-    <t>$B$9</t>
-  </si>
-  <si>
-    <t>p Fallzahl = r(((r/m)*t + A)^m ) ^p</t>
-  </si>
-  <si>
-    <t>Binding</t>
-  </si>
-  <si>
-    <t>Microsoft Excel 16.0 Sensitivity Report</t>
-  </si>
-  <si>
-    <t>Final</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Reduced</t>
-  </si>
-  <si>
-    <t>Gradient</t>
-  </si>
-  <si>
-    <t>NONE</t>
-  </si>
-  <si>
-    <t>Wirkliche Fälle mit Lag = 7 Tage zwischen Infektion und Bestätigung</t>
-  </si>
-  <si>
-    <t>Modellierung einer Vorhersage des Covid19 Verlaufs in Deutschland durch GRG Nonlinear mit Multistart Global Minimum Suche</t>
+    <t>Wirkliche Fälle mit Lag = 4 Tage zwischen Infektiösität und Bestätigung</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -296,14 +157,6 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="18"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -335,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -343,81 +196,17 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="23"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="23"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="23"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="23"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="23"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="23"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="23"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -463,7 +252,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$13</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$F$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -500,7 +289,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$14:$C$25</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$C$14:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -542,7 +331,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$14:$F$25</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$F$14:$F$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -569,6 +358,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>824</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -585,7 +377,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$13</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$H$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -622,7 +414,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$14:$C$25</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$C$14:$C$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
@@ -664,42 +456,42 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$14:$H$25</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$H$14:$H$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="1">
-                  <c:v>60.03665445359055</c:v>
+                  <c:v>136.35317742460342</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88.004346184969961</c:v>
+                  <c:v>174.07356974954914</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128.84383413497102</c:v>
+                  <c:v>221.30016805303734</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>188.40758769140396</c:v>
+                  <c:v>280.20333763126752</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>275.1767162789738</c:v>
+                  <c:v>353.39938038393734</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>401.42721219784983</c:v>
+                  <c:v>444.03233708280101</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>584.90727019055851</c:v>
+                  <c:v>555.86905690020535</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>851.24688887121363</c:v>
+                  <c:v>693.40941376396938</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1237.415514999318</c:v>
+                  <c:v>862.01377812993894</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1796.677962523303</c:v>
+                  <c:v>1068.0501053077762</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2605.6898627877044</c:v>
+                  <c:v>1319.0632795186532</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1157,7 +949,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$13</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$F$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1180,90 +972,90 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Sheet1!$A$14:$B$39</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$A$14:$B$39</c:f>
               <c:strCache>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>2/28/2020</c:v>
+                  <c:v>28.02.2020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2/29/2020</c:v>
+                  <c:v>29.02.2020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3/1/2020</c:v>
+                  <c:v>01.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3/2/2020</c:v>
+                  <c:v>02.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3/3/2020</c:v>
+                  <c:v>03.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3/4/2020</c:v>
+                  <c:v>04.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3/5/2020</c:v>
+                  <c:v>05.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3/6/2020</c:v>
+                  <c:v>06.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3/7/2020</c:v>
+                  <c:v>07.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3/8/2020</c:v>
+                  <c:v>08.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3/9/2020</c:v>
+                  <c:v>09.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3/10/2020</c:v>
+                  <c:v>10.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3/11/2020</c:v>
+                  <c:v>11.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3/12/2020</c:v>
+                  <c:v>12.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3/13/2020</c:v>
+                  <c:v>13.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3/14/2020</c:v>
+                  <c:v>14.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3/15/2020</c:v>
+                  <c:v>15.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3/16/2020</c:v>
+                  <c:v>16.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3/17/2020</c:v>
+                  <c:v>17.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3/18/2020</c:v>
+                  <c:v>18.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3/19/2020</c:v>
+                  <c:v>19.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3/20/2020</c:v>
+                  <c:v>20.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3/21/2020</c:v>
+                  <c:v>21.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3/22/2020</c:v>
+                  <c:v>22.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3/23/2020</c:v>
+                  <c:v>23.03.2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$14:$F$39</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$F$14:$F$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -1290,6 +1082,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>824</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1306,7 +1101,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$13</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$H$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1329,167 +1124,167 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Sheet1!$A$14:$B$39</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$A$14:$B$39</c:f>
               <c:strCache>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>2/28/2020</c:v>
+                  <c:v>28.02.2020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2/29/2020</c:v>
+                  <c:v>29.02.2020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3/1/2020</c:v>
+                  <c:v>01.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3/2/2020</c:v>
+                  <c:v>02.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3/3/2020</c:v>
+                  <c:v>03.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3/4/2020</c:v>
+                  <c:v>04.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3/5/2020</c:v>
+                  <c:v>05.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3/6/2020</c:v>
+                  <c:v>06.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3/7/2020</c:v>
+                  <c:v>07.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3/8/2020</c:v>
+                  <c:v>08.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3/9/2020</c:v>
+                  <c:v>09.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3/10/2020</c:v>
+                  <c:v>10.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3/11/2020</c:v>
+                  <c:v>11.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3/12/2020</c:v>
+                  <c:v>12.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3/13/2020</c:v>
+                  <c:v>13.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3/14/2020</c:v>
+                  <c:v>14.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3/15/2020</c:v>
+                  <c:v>15.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3/16/2020</c:v>
+                  <c:v>16.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3/17/2020</c:v>
+                  <c:v>17.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3/18/2020</c:v>
+                  <c:v>18.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3/19/2020</c:v>
+                  <c:v>19.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3/20/2020</c:v>
+                  <c:v>20.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3/21/2020</c:v>
+                  <c:v>21.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3/22/2020</c:v>
+                  <c:v>22.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3/23/2020</c:v>
+                  <c:v>23.03.2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$14:$H$39</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$H$14:$H$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>60.03665445359055</c:v>
+                  <c:v>136.35317742460342</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88.004346184969961</c:v>
+                  <c:v>174.07356974954914</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128.84383413497102</c:v>
+                  <c:v>221.30016805303734</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>188.40758769140396</c:v>
+                  <c:v>280.20333763126752</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>275.1767162789738</c:v>
+                  <c:v>353.39938038393734</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>401.42721219784983</c:v>
+                  <c:v>444.03233708280101</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>584.90727019055851</c:v>
+                  <c:v>555.86905690020535</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>851.24688887121363</c:v>
+                  <c:v>693.40941376396938</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1237.415514999318</c:v>
+                  <c:v>862.01377812993894</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1796.677962523303</c:v>
+                  <c:v>1068.0501053077762</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2605.6898627877044</c:v>
+                  <c:v>1319.0632795186532</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3774.6449670409188</c:v>
+                  <c:v>1623.9696585163392</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5461.7708455292295</c:v>
+                  <c:v>1993.2800991135582</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7894.0135581646546</c:v>
+                  <c:v>2439.3551117163765</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11396.521348685739</c:v>
+                  <c:v>2976.6961945237013</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16434.624598062568</c:v>
+                  <c:v>3622.277838098089</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>23673.543707643767</c:v>
+                  <c:v>4395.9251714253242</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>34063.219972164021</c:v>
+                  <c:v>5320.7427443918887</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>48958.711448690585</c:v>
+                  <c:v>6423.600512042467</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>70290.88270668473</c:v>
+                  <c:v>7735.6837064417305</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>100808.14248154381</c:v>
+                  <c:v>9293.1139560602078</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>144418.44275233176</c:v>
+                  <c:v>11137.64974414328</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>206672.61801561838</c:v>
+                  <c:v>13317.475090528151</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>295446.76871714654</c:v>
+                  <c:v>15888.086200090984</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>421904.66386981081</c:v>
+                  <c:v>18913.286749912746</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1506,11 +1301,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$13</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$N$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Wirkliche Fälle mit Lag = 7 Tage zwischen Infektion und Bestätigung</c:v>
+                  <c:v>Wirkliche Fälle mit Lag = 3 Tage zwischen Infektiösität und Bestätigung</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1531,149 +1326,161 @@
           </c:marker>
           <c:xVal>
             <c:strRef>
-              <c:f>Sheet1!$A$14:$B$39</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$A$14:$B$39</c:f>
               <c:strCache>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>2/28/2020</c:v>
+                  <c:v>28.02.2020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2/29/2020</c:v>
+                  <c:v>29.02.2020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3/1/2020</c:v>
+                  <c:v>01.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3/2/2020</c:v>
+                  <c:v>02.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3/3/2020</c:v>
+                  <c:v>03.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3/4/2020</c:v>
+                  <c:v>04.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3/5/2020</c:v>
+                  <c:v>05.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3/6/2020</c:v>
+                  <c:v>06.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3/7/2020</c:v>
+                  <c:v>07.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3/8/2020</c:v>
+                  <c:v>08.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3/9/2020</c:v>
+                  <c:v>09.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3/10/2020</c:v>
+                  <c:v>10.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3/11/2020</c:v>
+                  <c:v>11.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3/12/2020</c:v>
+                  <c:v>12.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3/13/2020</c:v>
+                  <c:v>13.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3/14/2020</c:v>
+                  <c:v>14.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3/15/2020</c:v>
+                  <c:v>15.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3/16/2020</c:v>
+                  <c:v>16.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3/17/2020</c:v>
+                  <c:v>17.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3/18/2020</c:v>
+                  <c:v>18.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3/19/2020</c:v>
+                  <c:v>19.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3/20/2020</c:v>
+                  <c:v>20.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3/21/2020</c:v>
+                  <c:v>21.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3/22/2020</c:v>
+                  <c:v>22.03.2020</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3/23/2020</c:v>
+                  <c:v>23.03.2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$14:$N$39</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$N$14:$N$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>584.90727019055851</c:v>
+                  <c:v>221.30016805303734</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>851.24688887121363</c:v>
+                  <c:v>280.20333763126752</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1237.415514999318</c:v>
+                  <c:v>353.39938038393734</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1796.677962523303</c:v>
+                  <c:v>444.03233708280101</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2605.6898627877044</c:v>
+                  <c:v>555.86905690020535</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3774.6449670409188</c:v>
+                  <c:v>693.40941376396938</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5461.7708455292295</c:v>
+                  <c:v>862.01377812993894</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7894.0135581646546</c:v>
+                  <c:v>1068.0501053077762</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11396.521348685739</c:v>
+                  <c:v>1319.0632795186532</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16434.624598062568</c:v>
+                  <c:v>1623.9696585163392</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23673.543707643767</c:v>
+                  <c:v>1993.2800991135582</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34063.219972164021</c:v>
+                  <c:v>2439.3551117163765</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>48958.711448690585</c:v>
+                  <c:v>2976.6961945237013</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70290.88270668473</c:v>
+                  <c:v>3622.277838098089</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>100808.14248154381</c:v>
+                  <c:v>4395.9251714253242</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>144418.44275233176</c:v>
+                  <c:v>5320.7427443918887</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>206672.61801561838</c:v>
+                  <c:v>6423.600512042467</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>295446.76871714654</c:v>
+                  <c:v>7735.6837064417305</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>421904.66386981081</c:v>
+                  <c:v>9293.1139560602078</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11137.64974414328</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13317.475090528151</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>15888.086200090984</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>18913.286749912746</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1682,6 +1489,171 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000000B-2A83-4D4C-8CF1-81651205BB7D}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Polynomial-Exponential Growth'!$P$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Wirkliche Fälle mit Lag = 4 Tage zwischen Infektiösität und Bestätigung</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Polynomial-Exponential Growth'!$C$15:$C$33</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Polynomial-Exponential Growth'!$P$15:$P$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="19"/>
+                <c:pt idx="0">
+                  <c:v>353.39938038393734</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>444.03233708280101</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>555.86905690020535</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>693.40941376396938</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>862.01377812993894</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1068.0501053077762</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1319.0632795186532</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1623.9696585163392</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1993.2800991135582</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2439.3551117163765</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2976.6961945237013</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3622.277838098089</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4395.9251714253242</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>5320.7427443918887</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6423.600512042467</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7735.6837064417305</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9293.1139560602078</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>11137.64974414328</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13317.475090528151</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C23C-44F8-BA14-4DD24DD7FB91}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1839,6 +1811,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1944,7 +1930,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2015,6 +2001,7 @@
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -2117,7 +2104,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$F$13</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$F$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2178,7 +2165,7 @@
           </c:errBars>
           <c:xVal>
             <c:strRef>
-              <c:f>Sheet1!$A$14:$B$39</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$A$14:$B$39</c:f>
               <c:strCache>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
@@ -2261,7 +2248,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$14:$F$39</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$F$14:$F$39</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -2288,6 +2275,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>824</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2304,7 +2294,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$H$13</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$H$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2365,7 +2355,7 @@
           </c:errBars>
           <c:xVal>
             <c:strRef>
-              <c:f>Sheet1!$A$14:$B$39</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$A$14:$B$39</c:f>
               <c:strCache>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
@@ -2448,84 +2438,84 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$H$14:$H$39</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$H$14:$H$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>60.03665445359055</c:v>
+                  <c:v>136.35317742460342</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>88.004346184969961</c:v>
+                  <c:v>174.07356974954914</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>128.84383413497102</c:v>
+                  <c:v>221.30016805303734</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>188.40758769140396</c:v>
+                  <c:v>280.20333763126752</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>275.1767162789738</c:v>
+                  <c:v>353.39938038393734</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>401.42721219784983</c:v>
+                  <c:v>444.03233708280101</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>584.90727019055851</c:v>
+                  <c:v>555.86905690020535</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>851.24688887121363</c:v>
+                  <c:v>693.40941376396938</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1237.415514999318</c:v>
+                  <c:v>862.01377812993894</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1796.677962523303</c:v>
+                  <c:v>1068.0501053077762</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2605.6898627877044</c:v>
+                  <c:v>1319.0632795186532</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3774.6449670409188</c:v>
+                  <c:v>1623.9696585163392</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5461.7708455292295</c:v>
+                  <c:v>1993.2800991135582</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7894.0135581646546</c:v>
+                  <c:v>2439.3551117163765</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11396.521348685739</c:v>
+                  <c:v>2976.6961945237013</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16434.624598062568</c:v>
+                  <c:v>3622.277838098089</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>23673.543707643767</c:v>
+                  <c:v>4395.9251714253242</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>34063.219972164021</c:v>
+                  <c:v>5320.7427443918887</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>48958.711448690585</c:v>
+                  <c:v>6423.600512042467</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>70290.88270668473</c:v>
+                  <c:v>7735.6837064417305</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>100808.14248154381</c:v>
+                  <c:v>9293.1139560602078</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>144418.44275233176</c:v>
+                  <c:v>11137.64974414328</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>206672.61801561838</c:v>
+                  <c:v>13317.475090528151</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>295446.76871714654</c:v>
+                  <c:v>15888.086200090984</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>421904.66386981081</c:v>
+                  <c:v>18913.286749912746</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2542,11 +2532,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$N$13</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$N$13</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Wirkliche Fälle mit Lag = 7 Tage zwischen Infektion und Bestätigung</c:v>
+                  <c:v>Wirkliche Fälle mit Lag = 3 Tage zwischen Infektiösität und Bestätigung</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2605,7 +2595,7 @@
           </c:errBars>
           <c:xVal>
             <c:strRef>
-              <c:f>Sheet1!$A$14:$B$39</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$A$14:$B$39</c:f>
               <c:strCache>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
@@ -2688,66 +2678,78 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$14:$N$39</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$N$14:$N$39</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>584.90727019055851</c:v>
+                  <c:v>221.30016805303734</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>851.24688887121363</c:v>
+                  <c:v>280.20333763126752</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1237.415514999318</c:v>
+                  <c:v>353.39938038393734</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1796.677962523303</c:v>
+                  <c:v>444.03233708280101</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2605.6898627877044</c:v>
+                  <c:v>555.86905690020535</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3774.6449670409188</c:v>
+                  <c:v>693.40941376396938</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5461.7708455292295</c:v>
+                  <c:v>862.01377812993894</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7894.0135581646546</c:v>
+                  <c:v>1068.0501053077762</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>11396.521348685739</c:v>
+                  <c:v>1319.0632795186532</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16434.624598062568</c:v>
+                  <c:v>1623.9696585163392</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23673.543707643767</c:v>
+                  <c:v>1993.2800991135582</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34063.219972164021</c:v>
+                  <c:v>2439.3551117163765</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>48958.711448690585</c:v>
+                  <c:v>2976.6961945237013</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>70290.88270668473</c:v>
+                  <c:v>3622.277838098089</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>100808.14248154381</c:v>
+                  <c:v>4395.9251714253242</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>144418.44275233176</c:v>
+                  <c:v>5320.7427443918887</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>206672.61801561838</c:v>
+                  <c:v>6423.600512042467</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>295446.76871714654</c:v>
+                  <c:v>7735.6837064417305</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>421904.66386981081</c:v>
+                  <c:v>9293.1139560602078</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11137.64974414328</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13317.475090528151</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>15888.086200090984</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>18913.286749912746</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3117,7 +3119,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="de-DE" baseline="0"/>
-              <a:t> mit Lag = 7 Tage vs Kalendertag</a:t>
+              <a:t> mit Lag = 3 Tage vs Kalendertag</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -3174,7 +3176,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$M$15:$M$33</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$M$15:$M$33</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="19"/>
@@ -3240,66 +3242,66 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$N$15:$N$33</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$N$15:$N$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>584.90727019055851</c:v>
+                  <c:v>221.30016805303734</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>851.24688887121363</c:v>
+                  <c:v>280.20333763126752</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1237.415514999318</c:v>
+                  <c:v>353.39938038393734</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1796.677962523303</c:v>
+                  <c:v>444.03233708280101</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2605.6898627877044</c:v>
+                  <c:v>555.86905690020535</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3774.6449670409188</c:v>
+                  <c:v>693.40941376396938</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5461.7708455292295</c:v>
+                  <c:v>862.01377812993894</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7894.0135581646546</c:v>
+                  <c:v>1068.0501053077762</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>11396.521348685739</c:v>
+                  <c:v>1319.0632795186532</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16434.624598062568</c:v>
+                  <c:v>1623.9696585163392</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23673.543707643767</c:v>
+                  <c:v>1993.2800991135582</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34063.219972164021</c:v>
+                  <c:v>2439.3551117163765</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>48958.711448690585</c:v>
+                  <c:v>2976.6961945237013</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>70290.88270668473</c:v>
+                  <c:v>3622.277838098089</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>100808.14248154381</c:v>
+                  <c:v>4395.9251714253242</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>144418.44275233176</c:v>
+                  <c:v>5320.7427443918887</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>206672.61801561838</c:v>
+                  <c:v>6423.600512042467</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>295446.76871714654</c:v>
+                  <c:v>7735.6837064417305</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>421904.66386981081</c:v>
+                  <c:v>9293.1139560602078</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5992,7 +5994,116 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>29</xdr:col>
+      <xdr:colOff>172973</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>75471</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="937629"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rectangle 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4517D686-DABE-47E7-859E-55F182EBEDD3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19603973" y="7205614"/>
+          <a:ext cx="184731" cy="937629"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="5400" b="1" cap="none" spc="0">
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent5"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="12700" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="accent5">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.45942</cdr:x>
+      <cdr:y>0.8185</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.54928</cdr:x>
+      <cdr:y>1</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93DAED7F-9C14-4E24-BB05-73080E68948D}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4674816" y="4123645"/>
+          <a:ext cx="914400" cy="914400"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="de-DE" sz="1100"/>
+            <a:t>^Freitag 13.03.2020</a:t>
+          </a:r>
+        </a:p>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:endParaRPr lang="de-DE" sz="1100"/>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6291,518 +6402,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DFB9B1F-ABB8-4C4B-A9D6-9C0D0321C67F}">
-  <dimension ref="A1:G7"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81BE3287-B94E-481D-B084-9DC06C4AC873}">
-  <dimension ref="A1:G7"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
-    <col min="2" max="2" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54E288C6-5E20-4548-A122-00FE2E61328E}">
-  <dimension ref="A1:G29"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D16" s="10">
-        <v>1517.8940327961509</v>
-      </c>
-      <c r="E16" s="10">
-        <v>1517.8940327961509</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="11">
-        <v>0.31987547649785281</v>
-      </c>
-      <c r="E21" s="11">
-        <v>0.31987547649785281</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="12">
-        <v>103.41782520856621</v>
-      </c>
-      <c r="E22" s="12">
-        <v>103.41782520856621</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D23" s="12">
-        <v>1.0395259515324491</v>
-      </c>
-      <c r="E23" s="12">
-        <v>1.0395259515324491</v>
-      </c>
-      <c r="F23" s="9" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="10">
-        <v>0.98999999901110602</v>
-      </c>
-      <c r="E24" s="10">
-        <v>0.98999999901110602</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="10">
-        <v>0.98999999901110602</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="G29" s="8">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB1B8F6E-23B8-45D2-AC17-398C4DCB4A0D}">
-  <dimension ref="A1:E15"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.28515625" customWidth="1"/>
-    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D9" s="9">
-        <v>0.31987547649785281</v>
-      </c>
-      <c r="E9" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="9">
-        <v>103.41782520856621</v>
-      </c>
-      <c r="E10" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="9">
-        <v>1.0395259515324491</v>
-      </c>
-      <c r="E11" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" s="8">
-        <v>0.98999999901110602</v>
-      </c>
-      <c r="E12" s="8">
-        <v>-4217.4931640625</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75855736-B2B6-4FFD-943C-E355D55A5C8E}">
   <dimension ref="A2:R39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P7" sqref="P7"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AM43" sqref="AM43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6818,7 +6422,7 @@
   <sheetData>
     <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -6839,62 +6443,62 @@
       <c r="R2" s="2"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15" t="s">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="17">
-        <v>0.58595469351715701</v>
-      </c>
-      <c r="D6" s="16" t="s">
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="16">
-        <v>176.4510567799318</v>
-      </c>
-      <c r="D7" s="17">
+      <c r="B7" s="7">
+        <v>40</v>
+      </c>
+      <c r="D7" s="8">
         <f>SUM(K15:K22)</f>
-        <v>12748.843141858775</v>
-      </c>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
+        <v>75830.108566325041</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="16">
-        <v>1.0393701324990459</v>
+      <c r="B8" s="7">
+        <v>1.4206139997087863</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+      <c r="A9" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="16">
-        <v>0.67944147424124168</v>
+      <c r="B9" s="7">
+        <v>0.35</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -6914,7 +6518,10 @@
         <v>4</v>
       </c>
       <c r="N13" t="s">
-        <v>58</v>
+        <v>13</v>
+      </c>
+      <c r="P13" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -6929,18 +6536,22 @@
       </c>
       <c r="H15" s="5">
         <f xml:space="preserve"> $B$6* ((($B$6/$B$7)*C15+$B$8)^$B$7)^$B$9</f>
-        <v>60.03665445359055</v>
+        <v>136.35317742460342</v>
       </c>
       <c r="K15" s="5">
-        <f>(H15 -F15) ^2</f>
-        <v>143.1216366627948</v>
+        <f t="shared" ref="K15:K23" si="0">(H15 -F15) ^2</f>
+        <v>4141.3314446424865</v>
       </c>
       <c r="M15" s="1">
         <v>43889</v>
       </c>
       <c r="N15" s="5">
-        <f t="shared" ref="N15:N33" si="0">H21</f>
-        <v>584.90727019055851</v>
+        <f>H17</f>
+        <v>221.30016805303734</v>
+      </c>
+      <c r="P15" s="5">
+        <f>H19</f>
+        <v>353.39938038393734</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -6955,21 +6566,25 @@
       </c>
       <c r="H16" s="5">
         <f t="shared" ref="H16:H39" si="1" xml:space="preserve"> $B$6* ((($B$6/$B$7)*C16+$B$8)^$B$7)^$B$9</f>
-        <v>88.004346184969961</v>
+        <v>174.07356974954914</v>
       </c>
       <c r="K16" s="5">
-        <f>(H16 -F16) ^2</f>
-        <v>840.74794016106603</v>
+        <f t="shared" si="0"/>
+        <v>3257.3923639566501</v>
       </c>
       <c r="M16" s="1">
         <v>43890</v>
       </c>
       <c r="N16" s="5">
-        <f t="shared" si="0"/>
-        <v>851.24688887121363</v>
+        <f t="shared" ref="N16:N39" si="2">H18</f>
+        <v>280.20333763126752</v>
+      </c>
+      <c r="P16" s="5">
+        <f t="shared" ref="P16:P37" si="3">H20</f>
+        <v>444.03233708280101</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43891</v>
       </c>
@@ -6981,21 +6596,25 @@
       </c>
       <c r="H17" s="5">
         <f t="shared" si="1"/>
-        <v>128.84383413497102</v>
+        <v>221.30016805303734</v>
       </c>
       <c r="K17" s="5">
-        <f>(H17 -F17) ^2</f>
-        <v>1.336719507458213</v>
+        <f t="shared" si="0"/>
+        <v>8335.7206865128592</v>
       </c>
       <c r="M17" s="1">
         <v>43891</v>
       </c>
       <c r="N17" s="5">
-        <f t="shared" si="0"/>
-        <v>1237.415514999318</v>
+        <f t="shared" si="2"/>
+        <v>353.39938038393734</v>
+      </c>
+      <c r="P17" s="5">
+        <f t="shared" si="3"/>
+        <v>555.86905690020535</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43892</v>
       </c>
@@ -7007,21 +6626,25 @@
       </c>
       <c r="H18" s="5">
         <f t="shared" si="1"/>
-        <v>188.40758769140396</v>
+        <v>280.20333763126752</v>
       </c>
       <c r="K18" s="5">
-        <f>(H18 -F18) ^2</f>
-        <v>0.16612772618401064</v>
+        <f t="shared" si="0"/>
+        <v>8501.4554703455124</v>
       </c>
       <c r="M18" s="1">
         <v>43892</v>
       </c>
       <c r="N18" s="5">
-        <f t="shared" si="0"/>
-        <v>1796.677962523303</v>
+        <f t="shared" si="2"/>
+        <v>444.03233708280101</v>
+      </c>
+      <c r="P18" s="5">
+        <f t="shared" si="3"/>
+        <v>693.40941376396938</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43893</v>
       </c>
@@ -7033,21 +6656,25 @@
       </c>
       <c r="H19" s="5">
         <f t="shared" si="1"/>
-        <v>275.1767162789738</v>
+        <v>353.39938038393734</v>
       </c>
       <c r="K19" s="5">
-        <f>(H19 -F19) ^2</f>
-        <v>1237.4013681714202</v>
+        <f t="shared" si="0"/>
+        <v>12859.419471460913</v>
       </c>
       <c r="M19" s="1">
         <v>43893</v>
       </c>
       <c r="N19" s="5">
-        <f t="shared" si="0"/>
-        <v>2605.6898627877044</v>
+        <f t="shared" si="2"/>
+        <v>555.86905690020535</v>
+      </c>
+      <c r="P19" s="5">
+        <f t="shared" si="3"/>
+        <v>862.01377812993894</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43894</v>
       </c>
@@ -7059,21 +6686,25 @@
       </c>
       <c r="H20" s="5">
         <f t="shared" si="1"/>
-        <v>401.42721219784983</v>
+        <v>444.03233708280101</v>
       </c>
       <c r="K20" s="5">
-        <f>(H20 -F20) ^2</f>
-        <v>2542.9037300469745</v>
+        <f t="shared" si="0"/>
+        <v>8655.0157430879117</v>
       </c>
       <c r="M20" s="1">
         <v>43894</v>
       </c>
       <c r="N20" s="5">
-        <f t="shared" si="0"/>
-        <v>3774.6449670409188</v>
+        <f t="shared" si="2"/>
+        <v>693.40941376396938</v>
+      </c>
+      <c r="P20" s="5">
+        <f t="shared" si="3"/>
+        <v>1068.0501053077762</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43895</v>
       </c>
@@ -7085,21 +6716,25 @@
       </c>
       <c r="H21" s="5">
         <f t="shared" si="1"/>
-        <v>584.90727019055851</v>
+        <v>555.86905690020535</v>
       </c>
       <c r="K21" s="5">
-        <f>(H21 -F21) ^2</f>
-        <v>7240.7726664226129</v>
+        <f t="shared" si="0"/>
+        <v>13025.872172848563</v>
       </c>
       <c r="M21" s="1">
         <v>43895</v>
       </c>
       <c r="N21" s="5">
-        <f t="shared" si="0"/>
-        <v>5461.7708455292295</v>
+        <f t="shared" si="2"/>
+        <v>862.01377812993894</v>
+      </c>
+      <c r="P21" s="5">
+        <f t="shared" si="3"/>
+        <v>1319.0632795186532</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43896</v>
       </c>
@@ -7111,41 +6746,55 @@
       </c>
       <c r="H22" s="5">
         <f t="shared" si="1"/>
-        <v>851.24688887121363</v>
+        <v>693.40941376396938</v>
       </c>
       <c r="K22" s="5">
-        <f>(H22 -F22) ^2</f>
-        <v>742.39295316026505</v>
+        <f t="shared" si="0"/>
+        <v>17053.901213470148</v>
       </c>
       <c r="M22" s="1">
         <v>43896</v>
       </c>
       <c r="N22" s="5">
-        <f t="shared" si="0"/>
-        <v>7894.0135581646546</v>
+        <f t="shared" si="2"/>
+        <v>1068.0501053077762</v>
+      </c>
+      <c r="P22" s="5">
+        <f t="shared" si="3"/>
+        <v>1623.9696585163392</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43897</v>
       </c>
       <c r="C23">
         <v>8</v>
       </c>
+      <c r="F23">
+        <v>900</v>
+      </c>
       <c r="H23" s="5">
         <f t="shared" si="1"/>
-        <v>1237.415514999318</v>
-      </c>
-      <c r="K23" s="5"/>
+        <v>862.01377812993894</v>
+      </c>
+      <c r="K23" s="5">
+        <f t="shared" si="0"/>
+        <v>1442.953051961505</v>
+      </c>
       <c r="M23" s="1">
         <v>43897</v>
       </c>
       <c r="N23" s="5">
-        <f t="shared" si="0"/>
-        <v>11396.521348685739</v>
+        <f t="shared" si="2"/>
+        <v>1319.0632795186532</v>
+      </c>
+      <c r="P23" s="5">
+        <f t="shared" si="3"/>
+        <v>1993.2800991135582</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43898</v>
       </c>
@@ -7154,17 +6803,21 @@
       </c>
       <c r="H24" s="5">
         <f t="shared" si="1"/>
-        <v>1796.677962523303</v>
+        <v>1068.0501053077762</v>
       </c>
       <c r="M24" s="1">
         <v>43898</v>
       </c>
       <c r="N24" s="5">
-        <f t="shared" si="0"/>
-        <v>16434.624598062568</v>
+        <f t="shared" si="2"/>
+        <v>1623.9696585163392</v>
+      </c>
+      <c r="P24" s="5">
+        <f t="shared" si="3"/>
+        <v>2439.3551117163765</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43899</v>
       </c>
@@ -7173,17 +6826,21 @@
       </c>
       <c r="H25" s="5">
         <f t="shared" si="1"/>
-        <v>2605.6898627877044</v>
+        <v>1319.0632795186532</v>
       </c>
       <c r="M25" s="1">
         <v>43899</v>
       </c>
       <c r="N25" s="5">
-        <f t="shared" si="0"/>
-        <v>23673.543707643767</v>
+        <f t="shared" si="2"/>
+        <v>1993.2800991135582</v>
+      </c>
+      <c r="P25" s="5">
+        <f t="shared" si="3"/>
+        <v>2976.6961945237013</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43900</v>
       </c>
@@ -7192,17 +6849,21 @@
       </c>
       <c r="H26" s="5">
         <f t="shared" si="1"/>
-        <v>3774.6449670409188</v>
+        <v>1623.9696585163392</v>
       </c>
       <c r="M26" s="1">
         <v>43900</v>
       </c>
       <c r="N26" s="5">
-        <f t="shared" si="0"/>
-        <v>34063.219972164021</v>
+        <f t="shared" si="2"/>
+        <v>2439.3551117163765</v>
+      </c>
+      <c r="P26" s="5">
+        <f t="shared" si="3"/>
+        <v>3622.277838098089</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43901</v>
       </c>
@@ -7211,17 +6872,21 @@
       </c>
       <c r="H27" s="5">
         <f t="shared" si="1"/>
-        <v>5461.7708455292295</v>
+        <v>1993.2800991135582</v>
       </c>
       <c r="M27" s="1">
         <v>43901</v>
       </c>
       <c r="N27" s="5">
-        <f t="shared" si="0"/>
-        <v>48958.711448690585</v>
+        <f t="shared" si="2"/>
+        <v>2976.6961945237013</v>
+      </c>
+      <c r="P27" s="5">
+        <f t="shared" si="3"/>
+        <v>4395.9251714253242</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43902</v>
       </c>
@@ -7230,17 +6895,21 @@
       </c>
       <c r="H28" s="5">
         <f t="shared" si="1"/>
-        <v>7894.0135581646546</v>
+        <v>2439.3551117163765</v>
       </c>
       <c r="M28" s="1">
         <v>43902</v>
       </c>
       <c r="N28" s="5">
-        <f t="shared" si="0"/>
-        <v>70290.88270668473</v>
+        <f t="shared" si="2"/>
+        <v>3622.277838098089</v>
+      </c>
+      <c r="P28" s="5">
+        <f t="shared" si="3"/>
+        <v>5320.7427443918887</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43903</v>
       </c>
@@ -7249,17 +6918,21 @@
       </c>
       <c r="H29" s="5">
         <f t="shared" si="1"/>
-        <v>11396.521348685739</v>
+        <v>2976.6961945237013</v>
       </c>
       <c r="M29" s="1">
         <v>43903</v>
       </c>
       <c r="N29" s="5">
-        <f t="shared" si="0"/>
-        <v>100808.14248154381</v>
+        <f t="shared" si="2"/>
+        <v>4395.9251714253242</v>
+      </c>
+      <c r="P29" s="5">
+        <f t="shared" si="3"/>
+        <v>6423.600512042467</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43904</v>
       </c>
@@ -7268,17 +6941,21 @@
       </c>
       <c r="H30" s="5">
         <f t="shared" si="1"/>
-        <v>16434.624598062568</v>
+        <v>3622.277838098089</v>
       </c>
       <c r="M30" s="1">
         <v>43904</v>
       </c>
       <c r="N30" s="5">
-        <f t="shared" si="0"/>
-        <v>144418.44275233176</v>
+        <f t="shared" si="2"/>
+        <v>5320.7427443918887</v>
+      </c>
+      <c r="P30" s="5">
+        <f t="shared" si="3"/>
+        <v>7735.6837064417305</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43905</v>
       </c>
@@ -7287,17 +6964,21 @@
       </c>
       <c r="H31" s="5">
         <f t="shared" si="1"/>
-        <v>23673.543707643767</v>
+        <v>4395.9251714253242</v>
       </c>
       <c r="M31" s="1">
         <v>43905</v>
       </c>
       <c r="N31" s="5">
-        <f t="shared" si="0"/>
-        <v>206672.61801561838</v>
+        <f t="shared" si="2"/>
+        <v>6423.600512042467</v>
+      </c>
+      <c r="P31" s="5">
+        <f t="shared" si="3"/>
+        <v>9293.1139560602078</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43906</v>
       </c>
@@ -7306,17 +6987,21 @@
       </c>
       <c r="H32" s="5">
         <f t="shared" si="1"/>
-        <v>34063.219972164021</v>
+        <v>5320.7427443918887</v>
       </c>
       <c r="M32" s="1">
         <v>43906</v>
       </c>
       <c r="N32" s="5">
-        <f t="shared" si="0"/>
-        <v>295446.76871714654</v>
+        <f t="shared" si="2"/>
+        <v>7735.6837064417305</v>
+      </c>
+      <c r="P32" s="5">
+        <f t="shared" si="3"/>
+        <v>11137.64974414328</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43907</v>
       </c>
@@ -7325,17 +7010,21 @@
       </c>
       <c r="H33" s="5">
         <f t="shared" si="1"/>
-        <v>48958.711448690585</v>
+        <v>6423.600512042467</v>
       </c>
       <c r="M33" s="1">
         <v>43907</v>
       </c>
       <c r="N33" s="5">
-        <f t="shared" si="0"/>
-        <v>421904.66386981081</v>
+        <f t="shared" si="2"/>
+        <v>9293.1139560602078</v>
+      </c>
+      <c r="P33" s="5">
+        <f t="shared" si="3"/>
+        <v>13317.475090528151</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43908</v>
       </c>
@@ -7344,12 +7033,19 @@
       </c>
       <c r="H34" s="5">
         <f t="shared" si="1"/>
-        <v>70290.88270668473</v>
-      </c>
-      <c r="N34" s="5"/>
+        <v>7735.6837064417305</v>
+      </c>
+      <c r="N34" s="5">
+        <f t="shared" si="2"/>
+        <v>11137.64974414328</v>
+      </c>
       <c r="O34" s="1"/>
+      <c r="P34" s="5">
+        <f t="shared" si="3"/>
+        <v>15888.086200090984</v>
+      </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43909</v>
       </c>
@@ -7358,12 +7054,19 @@
       </c>
       <c r="H35" s="5">
         <f t="shared" si="1"/>
-        <v>100808.14248154381</v>
-      </c>
-      <c r="N35" s="5"/>
+        <v>9293.1139560602078</v>
+      </c>
+      <c r="N35" s="5">
+        <f t="shared" si="2"/>
+        <v>13317.475090528151</v>
+      </c>
       <c r="O35" s="1"/>
+      <c r="P35" s="5">
+        <f t="shared" si="3"/>
+        <v>18913.286749912746</v>
+      </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43910</v>
       </c>
@@ -7372,12 +7075,16 @@
       </c>
       <c r="H36" s="5">
         <f t="shared" si="1"/>
-        <v>144418.44275233176</v>
-      </c>
-      <c r="N36" s="5"/>
+        <v>11137.64974414328</v>
+      </c>
+      <c r="N36" s="5">
+        <f t="shared" si="2"/>
+        <v>15888.086200090984</v>
+      </c>
       <c r="O36" s="1"/>
+      <c r="P36" s="5"/>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43911</v>
       </c>
@@ -7386,12 +7093,16 @@
       </c>
       <c r="H37" s="5">
         <f t="shared" si="1"/>
-        <v>206672.61801561838</v>
-      </c>
-      <c r="N37" s="5"/>
+        <v>13317.475090528151</v>
+      </c>
+      <c r="N37" s="5">
+        <f t="shared" si="2"/>
+        <v>18913.286749912746</v>
+      </c>
       <c r="O37" s="1"/>
+      <c r="P37" s="5"/>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43912</v>
       </c>
@@ -7400,12 +7111,12 @@
       </c>
       <c r="H38" s="5">
         <f t="shared" si="1"/>
-        <v>295446.76871714654</v>
+        <v>15888.086200090984</v>
       </c>
       <c r="N38" s="5"/>
       <c r="O38" s="1"/>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43913</v>
       </c>
@@ -7414,7 +7125,7 @@
       </c>
       <c r="H39" s="5">
         <f t="shared" si="1"/>
-        <v>421904.66386981081</v>
+        <v>18913.286749912746</v>
       </c>
       <c r="N39" s="5"/>
       <c r="O39" s="1"/>

</xml_diff>

<commit_message>
Adjusted real data with proper source from RKI
Original data source was incorrect. However estimates did not change much for the close future.
</commit_message>
<xml_diff>
--- a/Covid19_Germany_Estimates/Corona_Deutschland_Modellierung_08-03-2020.xlsx
+++ b/Covid19_Germany_Estimates/Corona_Deutschland_Modellierung_08-03-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benni\Desktop\Covid19_Germany_Estimates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BAAC4FD-B895-4771-953F-7ACBB7457B00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0F2F1E-456E-41F8-8C22-8D77FD738FA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8F2FD530-AE1D-479B-B999-25EE25C3C974}"/>
   </bookViews>
@@ -16,32 +16,35 @@
     <sheet name="Polynomial-Exponential Growth" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$6:$B$9</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$6:$B$10</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$6</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$6</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$7</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$7</definedName>
-    <definedName name="solver_lhs5" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$8</definedName>
-    <definedName name="solver_lhs6" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$8</definedName>
-    <definedName name="solver_lhs7" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$9</definedName>
-    <definedName name="solver_lhs8" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$9</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$10</definedName>
+    <definedName name="solver_lhs10" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$9</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$10</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$6</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$6</definedName>
+    <definedName name="solver_lhs5" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$7</definedName>
+    <definedName name="solver_lhs6" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$7</definedName>
+    <definedName name="solver_lhs7" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$8</definedName>
+    <definedName name="solver_lhs8" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$8</definedName>
+    <definedName name="solver_lhs9" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$9</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_num" localSheetId="0" hidden="1">8</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">10</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$D$7</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel10" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
@@ -49,14 +52,17 @@
     <definedName name="solver_rel6" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel7" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel8" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">0</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">40</definedName>
-    <definedName name="solver_rhs4" localSheetId="0" hidden="1">20</definedName>
-    <definedName name="solver_rhs5" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_rhs6" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_rhs7" localSheetId="0" hidden="1">0.35</definedName>
-    <definedName name="solver_rhs8" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rel9" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_rhs10" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">-100</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs5" localSheetId="0" hidden="1">40</definedName>
+    <definedName name="solver_rhs6" localSheetId="0" hidden="1">20</definedName>
+    <definedName name="solver_rhs7" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rhs8" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs9" localSheetId="0" hidden="1">0.35</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
@@ -100,9 +106,6 @@
     <t>Vorhergesagte Fälle</t>
   </si>
   <si>
-    <t>Quadratischer Fehler</t>
-  </si>
-  <si>
     <t>Summe Quadratischer Fehler</t>
   </si>
   <si>
@@ -130,7 +133,10 @@
     <t>Wirkliche Fälle mit Lag = 3 Tage zwischen Infektiösität und Bestätigung</t>
   </si>
   <si>
-    <t>Wirkliche Fälle mit Lag = 4 Tage zwischen Infektiösität und Bestätigung</t>
+    <t>Wirkliche Fälle mit Lag = 5 Tage zwischen Infektiösität und Bestätigung</t>
+  </si>
+  <si>
+    <t>^2 Error Scaled by #</t>
   </si>
 </sst>
 </file>
@@ -241,7 +247,62 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Model vs Actual Data</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -336,31 +397,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="1">
-                  <c:v>72</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>117</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>130</c:v>
-                </c:pt>
                 <c:pt idx="4">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>188</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>351</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>670</c:v>
+                  <c:v>349</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>824</c:v>
+                  <c:v>534</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>900</c:v>
+                  <c:v>684</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>847</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1194</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -461,37 +528,37 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="1">
-                  <c:v>136.35317742460342</c:v>
+                  <c:v>27.673769115073469</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>174.07356974954914</c:v>
+                  <c:v>63.179036358768613</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>221.30016805303734</c:v>
+                  <c:v>107.67848749967958</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>280.20333763126752</c:v>
+                  <c:v>163.23600350324494</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>353.39938038393734</c:v>
+                  <c:v>232.34163540313443</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>444.03233708280101</c:v>
+                  <c:v>317.99016318318394</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>555.86905690020535</c:v>
+                  <c:v>423.77245715724291</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>693.40941376396938</c:v>
+                  <c:v>553.9814641445513</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>862.01377812993894</c:v>
+                  <c:v>713.73486381707357</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1068.0501053077762</c:v>
+                  <c:v>909.11668668752702</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1319.0632795186532</c:v>
+                  <c:v>1147.3404562581306</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1060,31 +1127,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>72</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>117</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>130</c:v>
-                </c:pt>
                 <c:pt idx="4">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>188</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>351</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>670</c:v>
+                  <c:v>349</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>824</c:v>
+                  <c:v>534</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>900</c:v>
+                  <c:v>684</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>847</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1194</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1212,79 +1285,79 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>136.35317742460342</c:v>
+                  <c:v>27.673769115073469</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>174.07356974954914</c:v>
+                  <c:v>63.179036358768613</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>221.30016805303734</c:v>
+                  <c:v>107.67848749967958</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>280.20333763126752</c:v>
+                  <c:v>163.23600350324494</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>353.39938038393734</c:v>
+                  <c:v>232.34163540313443</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>444.03233708280101</c:v>
+                  <c:v>317.99016318318394</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>555.86905690020535</c:v>
+                  <c:v>423.77245715724291</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>693.40941376396938</c:v>
+                  <c:v>553.9814641445513</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>862.01377812993894</c:v>
+                  <c:v>713.73486381707357</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1068.0501053077762</c:v>
+                  <c:v>909.11668668752702</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1319.0632795186532</c:v>
+                  <c:v>1147.3404562581306</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1623.9696585163392</c:v>
+                  <c:v>1436.9367159358608</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1993.2800991135582</c:v>
+                  <c:v>1787.9681286508344</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2439.3551117163765</c:v>
+                  <c:v>2212.275696043906</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2976.6961945237013</c:v>
+                  <c:v>2723.7600371202593</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3622.277838098089</c:v>
+                  <c:v>3338.7020960557197</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4395.9251714253242</c:v>
+                  <c:v>4076.1281182146959</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5320.7427443918887</c:v>
+                  <c:v>4958.2242453843637</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6423.600512042467</c:v>
+                  <c:v>6010.8066389213163</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7735.6837064417305</c:v>
+                  <c:v>7263.8536463009505</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9293.1139560602078</c:v>
+                  <c:v>8752.1071860071224</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11137.64974414328</c:v>
+                  <c:v>10515.751241557307</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>13317.475090528151</c:v>
+                  <c:v>12601.176131686761</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>15888.086200090984</c:v>
+                  <c:v>15061.838064505604</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>18913.286749912746</c:v>
+                  <c:v>17959.224393204116</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1414,73 +1487,73 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>221.30016805303734</c:v>
+                  <c:v>107.67848749967958</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>280.20333763126752</c:v>
+                  <c:v>163.23600350324494</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>353.39938038393734</c:v>
+                  <c:v>232.34163540313443</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>444.03233708280101</c:v>
+                  <c:v>317.99016318318394</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>555.86905690020535</c:v>
+                  <c:v>423.77245715724291</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>693.40941376396938</c:v>
+                  <c:v>553.9814641445513</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>862.01377812993894</c:v>
+                  <c:v>713.73486381707357</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1068.0501053077762</c:v>
+                  <c:v>909.11668668752702</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1319.0632795186532</c:v>
+                  <c:v>1147.3404562581306</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1623.9696585163392</c:v>
+                  <c:v>1436.9367159358608</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1993.2800991135582</c:v>
+                  <c:v>1787.9681286508344</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2439.3551117163765</c:v>
+                  <c:v>2212.275696043906</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2976.6961945237013</c:v>
+                  <c:v>2723.7600371202593</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3622.277838098089</c:v>
+                  <c:v>3338.7020960557197</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4395.9251714253242</c:v>
+                  <c:v>4076.1281182146959</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5320.7427443918887</c:v>
+                  <c:v>4958.2242453843637</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6423.600512042467</c:v>
+                  <c:v>6010.8066389213163</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7735.6837064417305</c:v>
+                  <c:v>7263.8536463009505</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9293.1139560602078</c:v>
+                  <c:v>8752.1071860071224</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11137.64974414328</c:v>
+                  <c:v>10515.751241557307</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>13317.475090528151</c:v>
+                  <c:v>12601.176131686761</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>15888.086200090984</c:v>
+                  <c:v>15061.838064505604</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>18913.286749912746</c:v>
+                  <c:v>17959.224393204116</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1501,7 +1574,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Wirkliche Fälle mit Lag = 4 Tage zwischen Infektiösität und Bestätigung</c:v>
+                  <c:v>Wirkliche Fälle mit Lag = 5 Tage zwischen Infektiösität und Bestätigung</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1591,61 +1664,61 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>353.39938038393734</c:v>
+                  <c:v>232.34163540313443</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>444.03233708280101</c:v>
+                  <c:v>317.99016318318394</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>555.86905690020535</c:v>
+                  <c:v>423.77245715724291</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>693.40941376396938</c:v>
+                  <c:v>553.9814641445513</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>862.01377812993894</c:v>
+                  <c:v>713.73486381707357</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1068.0501053077762</c:v>
+                  <c:v>909.11668668752702</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1319.0632795186532</c:v>
+                  <c:v>1147.3404562581306</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1623.9696585163392</c:v>
+                  <c:v>1436.9367159358608</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1993.2800991135582</c:v>
+                  <c:v>1787.9681286508344</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2439.3551117163765</c:v>
+                  <c:v>2212.275696043906</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2976.6961945237013</c:v>
+                  <c:v>2723.7600371202593</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3622.277838098089</c:v>
+                  <c:v>3338.7020960557197</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4395.9251714253242</c:v>
+                  <c:v>4076.1281182146959</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5320.7427443918887</c:v>
+                  <c:v>4958.2242453843637</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6423.600512042467</c:v>
+                  <c:v>6010.8066389213163</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7735.6837064417305</c:v>
+                  <c:v>7263.8536463009505</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9293.1139560602078</c:v>
+                  <c:v>8752.1071860071224</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11137.64974414328</c:v>
+                  <c:v>10515.751241557307</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>13317.475090528151</c:v>
+                  <c:v>12601.176131686761</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2253,31 +2326,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>72</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>117</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>130</c:v>
-                </c:pt>
                 <c:pt idx="4">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>188</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="6">
                   <c:v>240</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>351</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>670</c:v>
+                  <c:v>349</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>824</c:v>
+                  <c:v>534</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>900</c:v>
+                  <c:v>684</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>847</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1194</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2443,79 +2522,79 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>136.35317742460342</c:v>
+                  <c:v>27.673769115073469</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>174.07356974954914</c:v>
+                  <c:v>63.179036358768613</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>221.30016805303734</c:v>
+                  <c:v>107.67848749967958</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>280.20333763126752</c:v>
+                  <c:v>163.23600350324494</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>353.39938038393734</c:v>
+                  <c:v>232.34163540313443</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>444.03233708280101</c:v>
+                  <c:v>317.99016318318394</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>555.86905690020535</c:v>
+                  <c:v>423.77245715724291</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>693.40941376396938</c:v>
+                  <c:v>553.9814641445513</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>862.01377812993894</c:v>
+                  <c:v>713.73486381707357</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1068.0501053077762</c:v>
+                  <c:v>909.11668668752702</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1319.0632795186532</c:v>
+                  <c:v>1147.3404562581306</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1623.9696585163392</c:v>
+                  <c:v>1436.9367159358608</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1993.2800991135582</c:v>
+                  <c:v>1787.9681286508344</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2439.3551117163765</c:v>
+                  <c:v>2212.275696043906</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2976.6961945237013</c:v>
+                  <c:v>2723.7600371202593</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3622.277838098089</c:v>
+                  <c:v>3338.7020960557197</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4395.9251714253242</c:v>
+                  <c:v>4076.1281182146959</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5320.7427443918887</c:v>
+                  <c:v>4958.2242453843637</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6423.600512042467</c:v>
+                  <c:v>6010.8066389213163</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7735.6837064417305</c:v>
+                  <c:v>7263.8536463009505</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9293.1139560602078</c:v>
+                  <c:v>8752.1071860071224</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>11137.64974414328</c:v>
+                  <c:v>10515.751241557307</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>13317.475090528151</c:v>
+                  <c:v>12601.176131686761</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>15888.086200090984</c:v>
+                  <c:v>15061.838064505604</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>18913.286749912746</c:v>
+                  <c:v>17959.224393204116</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2683,73 +2762,73 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>221.30016805303734</c:v>
+                  <c:v>107.67848749967958</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>280.20333763126752</c:v>
+                  <c:v>163.23600350324494</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>353.39938038393734</c:v>
+                  <c:v>232.34163540313443</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>444.03233708280101</c:v>
+                  <c:v>317.99016318318394</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>555.86905690020535</c:v>
+                  <c:v>423.77245715724291</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>693.40941376396938</c:v>
+                  <c:v>553.9814641445513</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>862.01377812993894</c:v>
+                  <c:v>713.73486381707357</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1068.0501053077762</c:v>
+                  <c:v>909.11668668752702</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1319.0632795186532</c:v>
+                  <c:v>1147.3404562581306</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1623.9696585163392</c:v>
+                  <c:v>1436.9367159358608</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1993.2800991135582</c:v>
+                  <c:v>1787.9681286508344</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2439.3551117163765</c:v>
+                  <c:v>2212.275696043906</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2976.6961945237013</c:v>
+                  <c:v>2723.7600371202593</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3622.277838098089</c:v>
+                  <c:v>3338.7020960557197</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4395.9251714253242</c:v>
+                  <c:v>4076.1281182146959</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5320.7427443918887</c:v>
+                  <c:v>4958.2242453843637</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6423.600512042467</c:v>
+                  <c:v>6010.8066389213163</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7735.6837064417305</c:v>
+                  <c:v>7263.8536463009505</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9293.1139560602078</c:v>
+                  <c:v>8752.1071860071224</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11137.64974414328</c:v>
+                  <c:v>10515.751241557307</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>13317.475090528151</c:v>
+                  <c:v>12601.176131686761</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>15888.086200090984</c:v>
+                  <c:v>15061.838064505604</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>18913.286749912746</c:v>
+                  <c:v>17959.224393204116</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3247,61 +3326,61 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>221.30016805303734</c:v>
+                  <c:v>107.67848749967958</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>280.20333763126752</c:v>
+                  <c:v>163.23600350324494</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>353.39938038393734</c:v>
+                  <c:v>232.34163540313443</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>444.03233708280101</c:v>
+                  <c:v>317.99016318318394</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>555.86905690020535</c:v>
+                  <c:v>423.77245715724291</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>693.40941376396938</c:v>
+                  <c:v>553.9814641445513</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>862.01377812993894</c:v>
+                  <c:v>713.73486381707357</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1068.0501053077762</c:v>
+                  <c:v>909.11668668752702</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1319.0632795186532</c:v>
+                  <c:v>1147.3404562581306</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1623.9696585163392</c:v>
+                  <c:v>1436.9367159358608</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1993.2800991135582</c:v>
+                  <c:v>1787.9681286508344</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2439.3551117163765</c:v>
+                  <c:v>2212.275696043906</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2976.6961945237013</c:v>
+                  <c:v>2723.7600371202593</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3622.277838098089</c:v>
+                  <c:v>3338.7020960557197</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4395.9251714253242</c:v>
+                  <c:v>4076.1281182146959</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5320.7427443918887</c:v>
+                  <c:v>4958.2242453843637</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6423.600512042467</c:v>
+                  <c:v>6010.8066389213163</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7735.6837064417305</c:v>
+                  <c:v>7263.8536463009505</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9293.1139560602078</c:v>
+                  <c:v>8752.1071860071224</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6061,12 +6140,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.45942</cdr:x>
-      <cdr:y>0.8185</cdr:y>
+      <cdr:x>0.55082</cdr:x>
+      <cdr:y>0.76067</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.54928</cdr:x>
-      <cdr:y>1</cdr:y>
+      <cdr:x>0.64068</cdr:x>
+      <cdr:y>0.94217</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -6081,8 +6160,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="4674816" y="4123645"/>
-          <a:ext cx="914400" cy="914400"/>
+          <a:off x="5537450" y="3832287"/>
+          <a:ext cx="903366" cy="914405"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -6405,8 +6484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75855736-B2B6-4FFD-943C-E355D55A5C8E}">
   <dimension ref="A2:R39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AM43" sqref="AM43"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6422,7 +6501,7 @@
   <sheetData>
     <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -6444,13 +6523,13 @@
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
       <c r="F4" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
@@ -6460,45 +6539,51 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="8">
         <v>1</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="7">
         <v>40</v>
       </c>
       <c r="D7" s="8">
-        <f>SUM(K15:K22)</f>
-        <v>75830.108566325041</v>
+        <f>SUM(K15:K25)</f>
+        <v>31637413238.285164</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="7">
-        <v>1.4206139997087863</v>
+        <v>1.4139558017857481</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" s="7">
         <v>0.35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7">
+        <v>-99.999999999999986</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
@@ -6515,13 +6600,13 @@
         <v>3</v>
       </c>
       <c r="K13" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="N13" t="s">
+        <v>12</v>
+      </c>
+      <c r="P13" t="s">
         <v>13</v>
-      </c>
-      <c r="P13" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
@@ -6532,26 +6617,26 @@
         <v>0</v>
       </c>
       <c r="F15">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="H15" s="5">
-        <f xml:space="preserve"> $B$6* ((($B$6/$B$7)*C15+$B$8)^$B$7)^$B$9</f>
-        <v>136.35317742460342</v>
+        <f xml:space="preserve"> $B$6* ((($B$6/$B$7)*C15+$B$8)^$B$7)^$B$9 + $B$10</f>
+        <v>27.673769115073469</v>
       </c>
       <c r="K15" s="5">
-        <f t="shared" ref="K15:K23" si="0">(H15 -F15) ^2</f>
-        <v>4141.3314446424865</v>
+        <f>(H15 ^2   -F15 ^2) ^2</f>
+        <v>4174513.0135246785</v>
       </c>
       <c r="M15" s="1">
         <v>43889</v>
       </c>
       <c r="N15" s="5">
         <f>H17</f>
-        <v>221.30016805303734</v>
+        <v>107.67848749967958</v>
       </c>
       <c r="P15" s="5">
         <f>H19</f>
-        <v>353.39938038393734</v>
+        <v>232.34163540313443</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
@@ -6562,26 +6647,26 @@
         <v>1</v>
       </c>
       <c r="F16">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="H16" s="5">
-        <f t="shared" ref="H16:H39" si="1" xml:space="preserve"> $B$6* ((($B$6/$B$7)*C16+$B$8)^$B$7)^$B$9</f>
-        <v>174.07356974954914</v>
+        <f t="shared" ref="H16:H39" si="0" xml:space="preserve"> $B$6* ((($B$6/$B$7)*C16+$B$8)^$B$7)^$B$9 + $B$10</f>
+        <v>63.179036358768613</v>
       </c>
       <c r="K16" s="5">
-        <f t="shared" si="0"/>
-        <v>3257.3923639566501</v>
+        <f t="shared" ref="K16:K25" si="1">(H16 ^2   -F16 ^2) ^2</f>
+        <v>132794.18513746338</v>
       </c>
       <c r="M16" s="1">
         <v>43890</v>
       </c>
       <c r="N16" s="5">
-        <f t="shared" ref="N16:N39" si="2">H18</f>
-        <v>280.20333763126752</v>
+        <f t="shared" ref="N16:N37" si="2">H18</f>
+        <v>163.23600350324494</v>
       </c>
       <c r="P16" s="5">
-        <f t="shared" ref="P16:P37" si="3">H20</f>
-        <v>444.03233708280101</v>
+        <f t="shared" ref="P16:P35" si="3">H20</f>
+        <v>317.99016318318394</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -6592,26 +6677,26 @@
         <v>2</v>
       </c>
       <c r="F17">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="H17" s="5">
+        <f t="shared" si="0"/>
+        <v>107.67848749967958</v>
+      </c>
+      <c r="K17" s="5">
         <f t="shared" si="1"/>
-        <v>221.30016805303734</v>
-      </c>
-      <c r="K17" s="5">
-        <f t="shared" si="0"/>
-        <v>8335.7206865128592</v>
+        <v>4386273.9829996321</v>
       </c>
       <c r="M17" s="1">
         <v>43891</v>
       </c>
       <c r="N17" s="5">
         <f t="shared" si="2"/>
-        <v>353.39938038393734</v>
+        <v>232.34163540313443</v>
       </c>
       <c r="P17" s="5">
         <f t="shared" si="3"/>
-        <v>555.86905690020535</v>
+        <v>423.77245715724291</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -6622,26 +6707,26 @@
         <v>3</v>
       </c>
       <c r="F18">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="H18" s="5">
+        <f t="shared" si="0"/>
+        <v>163.23600350324494</v>
+      </c>
+      <c r="K18" s="5">
         <f t="shared" si="1"/>
-        <v>280.20333763126752</v>
-      </c>
-      <c r="K18" s="5">
-        <f t="shared" si="0"/>
-        <v>8501.4554703455124</v>
+        <v>14783969.937431892</v>
       </c>
       <c r="M18" s="1">
         <v>43892</v>
       </c>
       <c r="N18" s="5">
         <f t="shared" si="2"/>
-        <v>444.03233708280101</v>
+        <v>317.99016318318394</v>
       </c>
       <c r="P18" s="5">
         <f t="shared" si="3"/>
-        <v>693.40941376396938</v>
+        <v>553.9814641445513</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -6652,26 +6737,26 @@
         <v>4</v>
       </c>
       <c r="F19">
-        <v>240</v>
+        <v>188</v>
       </c>
       <c r="H19" s="5">
+        <f t="shared" si="0"/>
+        <v>232.34163540313443</v>
+      </c>
+      <c r="K19" s="5">
         <f t="shared" si="1"/>
-        <v>353.39938038393734</v>
-      </c>
-      <c r="K19" s="5">
-        <f t="shared" si="0"/>
-        <v>12859.419471460913</v>
+        <v>347398734.86016393</v>
       </c>
       <c r="M19" s="1">
         <v>43893</v>
       </c>
       <c r="N19" s="5">
         <f t="shared" si="2"/>
-        <v>555.86905690020535</v>
+        <v>423.77245715724291</v>
       </c>
       <c r="P19" s="5">
         <f t="shared" si="3"/>
-        <v>862.01377812993894</v>
+        <v>713.73486381707357</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -6682,26 +6767,26 @@
         <v>5</v>
       </c>
       <c r="F20">
-        <v>351</v>
+        <v>240</v>
       </c>
       <c r="H20" s="5">
+        <f t="shared" si="0"/>
+        <v>317.99016318318394</v>
+      </c>
+      <c r="K20" s="5">
         <f t="shared" si="1"/>
-        <v>444.03233708280101</v>
-      </c>
-      <c r="K20" s="5">
-        <f t="shared" si="0"/>
-        <v>8655.0157430879117</v>
+        <v>1893794032.5156338</v>
       </c>
       <c r="M20" s="1">
         <v>43894</v>
       </c>
       <c r="N20" s="5">
         <f t="shared" si="2"/>
-        <v>693.40941376396938</v>
+        <v>553.9814641445513</v>
       </c>
       <c r="P20" s="5">
         <f t="shared" si="3"/>
-        <v>1068.0501053077762</v>
+        <v>909.11668668752702</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -6712,26 +6797,26 @@
         <v>6</v>
       </c>
       <c r="F21">
-        <v>670</v>
+        <v>349</v>
       </c>
       <c r="H21" s="5">
+        <f t="shared" si="0"/>
+        <v>423.77245715724291</v>
+      </c>
+      <c r="K21" s="5">
         <f t="shared" si="1"/>
-        <v>555.86905690020535</v>
-      </c>
-      <c r="K21" s="5">
-        <f t="shared" si="0"/>
-        <v>13025.872172848563</v>
+        <v>3338770554.0251746</v>
       </c>
       <c r="M21" s="1">
         <v>43895</v>
       </c>
       <c r="N21" s="5">
         <f t="shared" si="2"/>
-        <v>862.01377812993894</v>
+        <v>713.73486381707357</v>
       </c>
       <c r="P21" s="5">
         <f t="shared" si="3"/>
-        <v>1319.0632795186532</v>
+        <v>1147.3404562581306</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -6742,26 +6827,26 @@
         <v>7</v>
       </c>
       <c r="F22">
-        <v>824</v>
+        <v>534</v>
       </c>
       <c r="H22" s="5">
+        <f t="shared" si="0"/>
+        <v>553.9814641445513</v>
+      </c>
+      <c r="K22" s="5">
         <f t="shared" si="1"/>
-        <v>693.40941376396938</v>
-      </c>
-      <c r="K22" s="5">
-        <f t="shared" si="0"/>
-        <v>17053.901213470148</v>
+        <v>472604234.82119083</v>
       </c>
       <c r="M22" s="1">
         <v>43896</v>
       </c>
       <c r="N22" s="5">
         <f t="shared" si="2"/>
-        <v>1068.0501053077762</v>
+        <v>909.11668668752702</v>
       </c>
       <c r="P22" s="5">
         <f t="shared" si="3"/>
-        <v>1623.9696585163392</v>
+        <v>1436.9367159358608</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -6772,26 +6857,26 @@
         <v>8</v>
       </c>
       <c r="F23">
-        <v>900</v>
+        <v>684</v>
       </c>
       <c r="H23" s="5">
+        <f t="shared" si="0"/>
+        <v>713.73486381707357</v>
+      </c>
+      <c r="K23" s="5">
         <f t="shared" si="1"/>
-        <v>862.01377812993894</v>
-      </c>
-      <c r="K23" s="5">
-        <f t="shared" si="0"/>
-        <v>1442.953051961505</v>
+        <v>1727354610.5408483</v>
       </c>
       <c r="M23" s="1">
         <v>43897</v>
       </c>
       <c r="N23" s="5">
         <f t="shared" si="2"/>
-        <v>1319.0632795186532</v>
+        <v>1147.3404562581306</v>
       </c>
       <c r="P23" s="5">
         <f t="shared" si="3"/>
-        <v>1993.2800991135582</v>
+        <v>1787.9681286508344</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -6801,20 +6886,27 @@
       <c r="C24">
         <v>9</v>
       </c>
+      <c r="F24">
+        <v>847</v>
+      </c>
       <c r="H24" s="5">
+        <f t="shared" si="0"/>
+        <v>909.11668668752702</v>
+      </c>
+      <c r="K24" s="5">
         <f t="shared" si="1"/>
-        <v>1068.0501053077762</v>
+        <v>11899351784.212982</v>
       </c>
       <c r="M24" s="1">
         <v>43898</v>
       </c>
       <c r="N24" s="5">
         <f t="shared" si="2"/>
-        <v>1623.9696585163392</v>
+        <v>1436.9367159358608</v>
       </c>
       <c r="P24" s="5">
         <f t="shared" si="3"/>
-        <v>2439.3551117163765</v>
+        <v>2212.275696043906</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -6824,20 +6916,27 @@
       <c r="C25">
         <v>10</v>
       </c>
+      <c r="F25">
+        <v>1194</v>
+      </c>
       <c r="H25" s="5">
+        <f t="shared" si="0"/>
+        <v>1147.3404562581306</v>
+      </c>
+      <c r="K25" s="5">
         <f t="shared" si="1"/>
-        <v>1319.0632795186532</v>
+        <v>11934661736.190077</v>
       </c>
       <c r="M25" s="1">
         <v>43899</v>
       </c>
       <c r="N25" s="5">
         <f t="shared" si="2"/>
-        <v>1993.2800991135582</v>
+        <v>1787.9681286508344</v>
       </c>
       <c r="P25" s="5">
         <f t="shared" si="3"/>
-        <v>2976.6961945237013</v>
+        <v>2723.7600371202593</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -6848,19 +6947,19 @@
         <v>11</v>
       </c>
       <c r="H26" s="5">
-        <f t="shared" si="1"/>
-        <v>1623.9696585163392</v>
+        <f t="shared" si="0"/>
+        <v>1436.9367159358608</v>
       </c>
       <c r="M26" s="1">
         <v>43900</v>
       </c>
       <c r="N26" s="5">
         <f t="shared" si="2"/>
-        <v>2439.3551117163765</v>
+        <v>2212.275696043906</v>
       </c>
       <c r="P26" s="5">
         <f t="shared" si="3"/>
-        <v>3622.277838098089</v>
+        <v>3338.7020960557197</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -6871,19 +6970,19 @@
         <v>12</v>
       </c>
       <c r="H27" s="5">
-        <f t="shared" si="1"/>
-        <v>1993.2800991135582</v>
+        <f t="shared" si="0"/>
+        <v>1787.9681286508344</v>
       </c>
       <c r="M27" s="1">
         <v>43901</v>
       </c>
       <c r="N27" s="5">
         <f t="shared" si="2"/>
-        <v>2976.6961945237013</v>
+        <v>2723.7600371202593</v>
       </c>
       <c r="P27" s="5">
         <f t="shared" si="3"/>
-        <v>4395.9251714253242</v>
+        <v>4076.1281182146959</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -6894,19 +6993,19 @@
         <v>13</v>
       </c>
       <c r="H28" s="5">
-        <f t="shared" si="1"/>
-        <v>2439.3551117163765</v>
+        <f t="shared" si="0"/>
+        <v>2212.275696043906</v>
       </c>
       <c r="M28" s="1">
         <v>43902</v>
       </c>
       <c r="N28" s="5">
         <f t="shared" si="2"/>
-        <v>3622.277838098089</v>
+        <v>3338.7020960557197</v>
       </c>
       <c r="P28" s="5">
         <f t="shared" si="3"/>
-        <v>5320.7427443918887</v>
+        <v>4958.2242453843637</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -6917,19 +7016,19 @@
         <v>14</v>
       </c>
       <c r="H29" s="5">
-        <f t="shared" si="1"/>
-        <v>2976.6961945237013</v>
+        <f t="shared" si="0"/>
+        <v>2723.7600371202593</v>
       </c>
       <c r="M29" s="1">
         <v>43903</v>
       </c>
       <c r="N29" s="5">
         <f t="shared" si="2"/>
-        <v>4395.9251714253242</v>
+        <v>4076.1281182146959</v>
       </c>
       <c r="P29" s="5">
         <f t="shared" si="3"/>
-        <v>6423.600512042467</v>
+        <v>6010.8066389213163</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -6940,19 +7039,19 @@
         <v>15</v>
       </c>
       <c r="H30" s="5">
-        <f t="shared" si="1"/>
-        <v>3622.277838098089</v>
+        <f t="shared" si="0"/>
+        <v>3338.7020960557197</v>
       </c>
       <c r="M30" s="1">
         <v>43904</v>
       </c>
       <c r="N30" s="5">
         <f t="shared" si="2"/>
-        <v>5320.7427443918887</v>
+        <v>4958.2242453843637</v>
       </c>
       <c r="P30" s="5">
         <f t="shared" si="3"/>
-        <v>7735.6837064417305</v>
+        <v>7263.8536463009505</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -6963,19 +7062,19 @@
         <v>16</v>
       </c>
       <c r="H31" s="5">
-        <f t="shared" si="1"/>
-        <v>4395.9251714253242</v>
+        <f t="shared" si="0"/>
+        <v>4076.1281182146959</v>
       </c>
       <c r="M31" s="1">
         <v>43905</v>
       </c>
       <c r="N31" s="5">
         <f t="shared" si="2"/>
-        <v>6423.600512042467</v>
+        <v>6010.8066389213163</v>
       </c>
       <c r="P31" s="5">
         <f t="shared" si="3"/>
-        <v>9293.1139560602078</v>
+        <v>8752.1071860071224</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -6986,19 +7085,19 @@
         <v>17</v>
       </c>
       <c r="H32" s="5">
-        <f t="shared" si="1"/>
-        <v>5320.7427443918887</v>
+        <f t="shared" si="0"/>
+        <v>4958.2242453843637</v>
       </c>
       <c r="M32" s="1">
         <v>43906</v>
       </c>
       <c r="N32" s="5">
         <f t="shared" si="2"/>
-        <v>7735.6837064417305</v>
+        <v>7263.8536463009505</v>
       </c>
       <c r="P32" s="5">
         <f t="shared" si="3"/>
-        <v>11137.64974414328</v>
+        <v>10515.751241557307</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -7009,19 +7108,19 @@
         <v>18</v>
       </c>
       <c r="H33" s="5">
-        <f t="shared" si="1"/>
-        <v>6423.600512042467</v>
+        <f t="shared" si="0"/>
+        <v>6010.8066389213163</v>
       </c>
       <c r="M33" s="1">
         <v>43907</v>
       </c>
       <c r="N33" s="5">
         <f t="shared" si="2"/>
-        <v>9293.1139560602078</v>
+        <v>8752.1071860071224</v>
       </c>
       <c r="P33" s="5">
         <f t="shared" si="3"/>
-        <v>13317.475090528151</v>
+        <v>12601.176131686761</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -7032,17 +7131,17 @@
         <v>19</v>
       </c>
       <c r="H34" s="5">
-        <f t="shared" si="1"/>
-        <v>7735.6837064417305</v>
+        <f t="shared" si="0"/>
+        <v>7263.8536463009505</v>
       </c>
       <c r="N34" s="5">
         <f t="shared" si="2"/>
-        <v>11137.64974414328</v>
+        <v>10515.751241557307</v>
       </c>
       <c r="O34" s="1"/>
       <c r="P34" s="5">
         <f t="shared" si="3"/>
-        <v>15888.086200090984</v>
+        <v>15061.838064505604</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -7053,17 +7152,17 @@
         <v>20</v>
       </c>
       <c r="H35" s="5">
-        <f t="shared" si="1"/>
-        <v>9293.1139560602078</v>
+        <f t="shared" si="0"/>
+        <v>8752.1071860071224</v>
       </c>
       <c r="N35" s="5">
         <f t="shared" si="2"/>
-        <v>13317.475090528151</v>
+        <v>12601.176131686761</v>
       </c>
       <c r="O35" s="1"/>
       <c r="P35" s="5">
         <f t="shared" si="3"/>
-        <v>18913.286749912746</v>
+        <v>17959.224393204116</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -7074,12 +7173,12 @@
         <v>21</v>
       </c>
       <c r="H36" s="5">
-        <f t="shared" si="1"/>
-        <v>11137.64974414328</v>
+        <f t="shared" si="0"/>
+        <v>10515.751241557307</v>
       </c>
       <c r="N36" s="5">
         <f t="shared" si="2"/>
-        <v>15888.086200090984</v>
+        <v>15061.838064505604</v>
       </c>
       <c r="O36" s="1"/>
       <c r="P36" s="5"/>
@@ -7092,12 +7191,12 @@
         <v>22</v>
       </c>
       <c r="H37" s="5">
-        <f t="shared" si="1"/>
-        <v>13317.475090528151</v>
+        <f t="shared" si="0"/>
+        <v>12601.176131686761</v>
       </c>
       <c r="N37" s="5">
         <f t="shared" si="2"/>
-        <v>18913.286749912746</v>
+        <v>17959.224393204116</v>
       </c>
       <c r="O37" s="1"/>
       <c r="P37" s="5"/>
@@ -7110,8 +7209,8 @@
         <v>23</v>
       </c>
       <c r="H38" s="5">
-        <f t="shared" si="1"/>
-        <v>15888.086200090984</v>
+        <f t="shared" si="0"/>
+        <v>15061.838064505604</v>
       </c>
       <c r="N38" s="5"/>
       <c r="O38" s="1"/>
@@ -7124,8 +7223,8 @@
         <v>24</v>
       </c>
       <c r="H39" s="5">
-        <f t="shared" si="1"/>
-        <v>18913.286749912746</v>
+        <f t="shared" si="0"/>
+        <v>17959.224393204116</v>
       </c>
       <c r="N39" s="5"/>
       <c r="O39" s="1"/>

</xml_diff>

<commit_message>
update model unlimited r param no linear offset
</commit_message>
<xml_diff>
--- a/Covid19_Germany_Estimates/Corona_Deutschland_Modellierung_08-03-2020.xlsx
+++ b/Covid19_Germany_Estimates/Corona_Deutschland_Modellierung_08-03-2020.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benni\Desktop\Covid19_Germany_Estimates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0AD1C7E-5432-4042-9EB6-29C4BC9E95B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C60324-9FBE-4CD7-96E7-E6F0A3222A57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{8F2FD530-AE1D-479B-B999-25EE25C3C974}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{8F2FD530-AE1D-479B-B999-25EE25C3C974}"/>
   </bookViews>
   <sheets>
     <sheet name="Polynomial-Exponential Growth" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$6:$B$10</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$6:$B$9</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -57,7 +57,7 @@
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">-100</definedName>
     <definedName name="solver_rhs10" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">100</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">30</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">40</definedName>
     <definedName name="solver_rhs6" localSheetId="0" hidden="1">20</definedName>
@@ -586,64 +586,64 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="1">
-                  <c:v>30.876361337559839</c:v>
+                  <c:v>29.81777657449534</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52.697458033206956</c:v>
+                  <c:v>47.256227163532522</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>82.991089491917293</c:v>
+                  <c:v>72.953282922804277</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>124.60989510961691</c:v>
+                  <c:v>110.01759029135798</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>181.23006879741044</c:v>
+                  <c:v>162.46192806212051</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>257.55225352912061</c:v>
+                  <c:v>235.39755088761768</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>359.54303504862804</c:v>
+                  <c:v>335.25714063196648</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>494.72364810730016</c:v>
+                  <c:v>470.04883659023551</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>672.51334256763482</c:v>
+                  <c:v>649.64389337482669</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>904.63576698797078</c:v>
+                  <c:v>886.10059162299387</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1205.5977183907103</c:v>
+                  <c:v>1194.0271017006896</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1593.2506834355358</c:v>
+                  <c:v>1590.9860743466438</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2089.4467629187866</c:v>
+                  <c:v>2097.9438047900244</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2720.8018332758793</c:v>
+                  <c:v>2739.7668883509732</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3519.5801605773704</c:v>
+                  <c:v>3545.7693559555992</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4524.7161495086202</c:v>
+                  <c:v>4550.313347420175</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5782.9904872628686</c:v>
+                  <c:v>5793.4664488331027</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7350.3796355365848</c:v>
+                  <c:v>7321.7188879328478</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9293.5994384017631</c:v>
+                  <c:v>9188.7638480887817</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11691.865555372824</c:v>
+                  <c:v>11456.344227376318</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1391,79 +1391,79 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>30.876361337559839</c:v>
+                  <c:v>29.81777657449534</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52.697458033206956</c:v>
+                  <c:v>47.256227163532522</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>82.991089491917293</c:v>
+                  <c:v>72.953282922804277</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>124.60989510961691</c:v>
+                  <c:v>110.01759029135798</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>181.23006879741044</c:v>
+                  <c:v>162.46192806212051</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>257.55225352912061</c:v>
+                  <c:v>235.39755088761768</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>359.54303504862804</c:v>
+                  <c:v>335.25714063196648</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>494.72364810730016</c:v>
+                  <c:v>470.04883659023551</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>672.51334256763482</c:v>
+                  <c:v>649.64389337482669</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>904.63576698797078</c:v>
+                  <c:v>886.10059162299387</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1205.5977183907103</c:v>
+                  <c:v>1194.0271017006896</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1593.2506834355358</c:v>
+                  <c:v>1590.9860743466438</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2089.4467629187866</c:v>
+                  <c:v>2097.9438047900244</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2720.8018332758793</c:v>
+                  <c:v>2739.7668883509732</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3519.5801605773704</c:v>
+                  <c:v>3545.7693559555992</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4524.7161495086202</c:v>
+                  <c:v>4550.313347420175</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5782.9904872628686</c:v>
+                  <c:v>5793.4664488331027</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7350.3796355365848</c:v>
+                  <c:v>7321.7188879328478</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9293.5994384017631</c:v>
+                  <c:v>9188.7638480887817</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11691.865555372824</c:v>
+                  <c:v>11456.344227376318</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>14638.895503243941</c:v>
+                  <c:v>14195.169234336139</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>18245.179303129124</c:v>
+                  <c:v>17485.904276350782</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>22640.548086600076</c:v>
+                  <c:v>21420.237660192757</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>27977.072523021798</c:v>
+                  <c:v>26102.027687224239</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>34432.32559538725</c:v>
+                  <c:v>31648.533787987428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1593,73 +1593,73 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>82.991089491917293</c:v>
+                  <c:v>72.953282922804277</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>124.60989510961691</c:v>
+                  <c:v>110.01759029135798</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>181.23006879741044</c:v>
+                  <c:v>162.46192806212051</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>257.55225352912061</c:v>
+                  <c:v>235.39755088761768</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>359.54303504862804</c:v>
+                  <c:v>335.25714063196648</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>494.72364810730016</c:v>
+                  <c:v>470.04883659023551</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>672.51334256763482</c:v>
+                  <c:v>649.64389337482669</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>904.63576698797078</c:v>
+                  <c:v>886.10059162299387</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1205.5977183907103</c:v>
+                  <c:v>1194.0271017006896</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1593.2506834355358</c:v>
+                  <c:v>1590.9860743466438</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2089.4467629187866</c:v>
+                  <c:v>2097.9438047900244</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2720.8018332758793</c:v>
+                  <c:v>2739.7668883509732</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3519.5801605773704</c:v>
+                  <c:v>3545.7693559555992</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4524.7161495086202</c:v>
+                  <c:v>4550.313347420175</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5782.9904872628686</c:v>
+                  <c:v>5793.4664488331027</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7350.3796355365848</c:v>
+                  <c:v>7321.7188879328478</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9293.5994384017631</c:v>
+                  <c:v>9188.7638480887817</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11691.865555372824</c:v>
+                  <c:v>11456.344227376318</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>14638.895503243941</c:v>
+                  <c:v>14195.169234336139</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>18245.179303129124</c:v>
+                  <c:v>17485.904276350782</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>22640.548086600076</c:v>
+                  <c:v>21420.237660192757</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>27977.072523021798</c:v>
+                  <c:v>26102.027687224239</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>34432.32559538725</c:v>
+                  <c:v>31648.533787987428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1770,61 +1770,61 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>181.23006879741044</c:v>
+                  <c:v>162.46192806212051</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>257.55225352912061</c:v>
+                  <c:v>235.39755088761768</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>359.54303504862804</c:v>
+                  <c:v>335.25714063196648</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>494.72364810730016</c:v>
+                  <c:v>470.04883659023551</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>672.51334256763482</c:v>
+                  <c:v>649.64389337482669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>904.63576698797078</c:v>
+                  <c:v>886.10059162299387</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1205.5977183907103</c:v>
+                  <c:v>1194.0271017006896</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1593.2506834355358</c:v>
+                  <c:v>1590.9860743466438</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2089.4467629187866</c:v>
+                  <c:v>2097.9438047900244</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2720.8018332758793</c:v>
+                  <c:v>2739.7668883509732</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3519.5801605773704</c:v>
+                  <c:v>3545.7693559555992</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4524.7161495086202</c:v>
+                  <c:v>4550.313347420175</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5782.9904872628686</c:v>
+                  <c:v>5793.4664488331027</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7350.3796355365848</c:v>
+                  <c:v>7321.7188879328478</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9293.5994384017631</c:v>
+                  <c:v>9188.7638480887817</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11691.865555372824</c:v>
+                  <c:v>11456.344227376318</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14638.895503243941</c:v>
+                  <c:v>14195.169234336139</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>18245.179303129124</c:v>
+                  <c:v>17485.904276350782</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>22640.548086600076</c:v>
+                  <c:v>21420.237660192757</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2348,79 +2348,79 @@
               <c:strCache>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>28.02.2020</c:v>
+                  <c:v>2/28/2020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.02.2020</c:v>
+                  <c:v>2/29/2020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>01.03.2020</c:v>
+                  <c:v>3/1/2020</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>02.03.2020</c:v>
+                  <c:v>3/2/2020</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>03.03.2020</c:v>
+                  <c:v>3/3/2020</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>04.03.2020</c:v>
+                  <c:v>3/4/2020</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>05.03.2020</c:v>
+                  <c:v>3/5/2020</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>06.03.2020</c:v>
+                  <c:v>3/6/2020</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>07.03.2020</c:v>
+                  <c:v>3/7/2020</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>08.03.2020</c:v>
+                  <c:v>3/8/2020</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>09.03.2020</c:v>
+                  <c:v>3/9/2020</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10.03.2020</c:v>
+                  <c:v>3/10/2020</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.03.2020</c:v>
+                  <c:v>3/11/2020</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12.03.2020</c:v>
+                  <c:v>3/12/2020</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>13.03.2020</c:v>
+                  <c:v>3/13/2020</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14.03.2020</c:v>
+                  <c:v>3/14/2020</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.03.2020</c:v>
+                  <c:v>3/15/2020</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16.03.2020</c:v>
+                  <c:v>3/16/2020</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>17.03.2020</c:v>
+                  <c:v>3/17/2020</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>18.03.2020</c:v>
+                  <c:v>3/18/2020</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>19.03.2020</c:v>
+                  <c:v>3/19/2020</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>20.03.2020</c:v>
+                  <c:v>3/20/2020</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>21.03.2020</c:v>
+                  <c:v>3/21/2020</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>22.03.2020</c:v>
+                  <c:v>3/22/2020</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>23.03.2020</c:v>
+                  <c:v>3/23/2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2565,79 +2565,79 @@
               <c:strCache>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>28.02.2020</c:v>
+                  <c:v>2/28/2020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.02.2020</c:v>
+                  <c:v>2/29/2020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>01.03.2020</c:v>
+                  <c:v>3/1/2020</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>02.03.2020</c:v>
+                  <c:v>3/2/2020</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>03.03.2020</c:v>
+                  <c:v>3/3/2020</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>04.03.2020</c:v>
+                  <c:v>3/4/2020</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>05.03.2020</c:v>
+                  <c:v>3/5/2020</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>06.03.2020</c:v>
+                  <c:v>3/6/2020</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>07.03.2020</c:v>
+                  <c:v>3/7/2020</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>08.03.2020</c:v>
+                  <c:v>3/8/2020</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>09.03.2020</c:v>
+                  <c:v>3/9/2020</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10.03.2020</c:v>
+                  <c:v>3/10/2020</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.03.2020</c:v>
+                  <c:v>3/11/2020</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12.03.2020</c:v>
+                  <c:v>3/12/2020</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>13.03.2020</c:v>
+                  <c:v>3/13/2020</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14.03.2020</c:v>
+                  <c:v>3/14/2020</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.03.2020</c:v>
+                  <c:v>3/15/2020</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16.03.2020</c:v>
+                  <c:v>3/16/2020</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>17.03.2020</c:v>
+                  <c:v>3/17/2020</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>18.03.2020</c:v>
+                  <c:v>3/18/2020</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>19.03.2020</c:v>
+                  <c:v>3/19/2020</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>20.03.2020</c:v>
+                  <c:v>3/20/2020</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>21.03.2020</c:v>
+                  <c:v>3/21/2020</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>22.03.2020</c:v>
+                  <c:v>3/22/2020</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>23.03.2020</c:v>
+                  <c:v>3/23/2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2649,79 +2649,79 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>30.876361337559839</c:v>
+                  <c:v>29.81777657449534</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>52.697458033206956</c:v>
+                  <c:v>47.256227163532522</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>82.991089491917293</c:v>
+                  <c:v>72.953282922804277</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>124.60989510961691</c:v>
+                  <c:v>110.01759029135798</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>181.23006879741044</c:v>
+                  <c:v>162.46192806212051</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>257.55225352912061</c:v>
+                  <c:v>235.39755088761768</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>359.54303504862804</c:v>
+                  <c:v>335.25714063196648</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>494.72364810730016</c:v>
+                  <c:v>470.04883659023551</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>672.51334256763482</c:v>
+                  <c:v>649.64389337482669</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>904.63576698797078</c:v>
+                  <c:v>886.10059162299387</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1205.5977183907103</c:v>
+                  <c:v>1194.0271017006896</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1593.2506834355358</c:v>
+                  <c:v>1590.9860743466438</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2089.4467629187866</c:v>
+                  <c:v>2097.9438047900244</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2720.8018332758793</c:v>
+                  <c:v>2739.7668883509732</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3519.5801605773704</c:v>
+                  <c:v>3545.7693559555992</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4524.7161495086202</c:v>
+                  <c:v>4550.313347420175</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5782.9904872628686</c:v>
+                  <c:v>5793.4664488331027</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7350.3796355365848</c:v>
+                  <c:v>7321.7188879328478</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9293.5994384017631</c:v>
+                  <c:v>9188.7638480887817</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>11691.865555372824</c:v>
+                  <c:v>11456.344227376318</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>14638.895503243941</c:v>
+                  <c:v>14195.169234336139</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>18245.179303129124</c:v>
+                  <c:v>17485.904276350782</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>22640.548086600076</c:v>
+                  <c:v>21420.237660192757</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>27977.072523021798</c:v>
+                  <c:v>26102.027687224239</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>34432.32559538725</c:v>
+                  <c:v>31648.533787987428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2805,79 +2805,79 @@
               <c:strCache>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>28.02.2020</c:v>
+                  <c:v>2/28/2020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>29.02.2020</c:v>
+                  <c:v>2/29/2020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>01.03.2020</c:v>
+                  <c:v>3/1/2020</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>02.03.2020</c:v>
+                  <c:v>3/2/2020</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>03.03.2020</c:v>
+                  <c:v>3/3/2020</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>04.03.2020</c:v>
+                  <c:v>3/4/2020</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>05.03.2020</c:v>
+                  <c:v>3/5/2020</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>06.03.2020</c:v>
+                  <c:v>3/6/2020</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>07.03.2020</c:v>
+                  <c:v>3/7/2020</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>08.03.2020</c:v>
+                  <c:v>3/8/2020</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>09.03.2020</c:v>
+                  <c:v>3/9/2020</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>10.03.2020</c:v>
+                  <c:v>3/10/2020</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.03.2020</c:v>
+                  <c:v>3/11/2020</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>12.03.2020</c:v>
+                  <c:v>3/12/2020</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>13.03.2020</c:v>
+                  <c:v>3/13/2020</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14.03.2020</c:v>
+                  <c:v>3/14/2020</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>15.03.2020</c:v>
+                  <c:v>3/15/2020</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16.03.2020</c:v>
+                  <c:v>3/16/2020</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>17.03.2020</c:v>
+                  <c:v>3/17/2020</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>18.03.2020</c:v>
+                  <c:v>3/18/2020</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>19.03.2020</c:v>
+                  <c:v>3/19/2020</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>20.03.2020</c:v>
+                  <c:v>3/20/2020</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>21.03.2020</c:v>
+                  <c:v>3/21/2020</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>22.03.2020</c:v>
+                  <c:v>3/22/2020</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>23.03.2020</c:v>
+                  <c:v>3/23/2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2889,73 +2889,73 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>82.991089491917293</c:v>
+                  <c:v>72.953282922804277</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>124.60989510961691</c:v>
+                  <c:v>110.01759029135798</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>181.23006879741044</c:v>
+                  <c:v>162.46192806212051</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>257.55225352912061</c:v>
+                  <c:v>235.39755088761768</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>359.54303504862804</c:v>
+                  <c:v>335.25714063196648</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>494.72364810730016</c:v>
+                  <c:v>470.04883659023551</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>672.51334256763482</c:v>
+                  <c:v>649.64389337482669</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>904.63576698797078</c:v>
+                  <c:v>886.10059162299387</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1205.5977183907103</c:v>
+                  <c:v>1194.0271017006896</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1593.2506834355358</c:v>
+                  <c:v>1590.9860743466438</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2089.4467629187866</c:v>
+                  <c:v>2097.9438047900244</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2720.8018332758793</c:v>
+                  <c:v>2739.7668883509732</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3519.5801605773704</c:v>
+                  <c:v>3545.7693559555992</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4524.7161495086202</c:v>
+                  <c:v>4550.313347420175</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5782.9904872628686</c:v>
+                  <c:v>5793.4664488331027</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7350.3796355365848</c:v>
+                  <c:v>7321.7188879328478</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9293.5994384017631</c:v>
+                  <c:v>9188.7638480887817</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>11691.865555372824</c:v>
+                  <c:v>11456.344227376318</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>14638.895503243941</c:v>
+                  <c:v>14195.169234336139</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>18245.179303129124</c:v>
+                  <c:v>17485.904276350782</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>22640.548086600076</c:v>
+                  <c:v>21420.237660192757</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>27977.072523021798</c:v>
+                  <c:v>26102.027687224239</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>34432.32559538725</c:v>
+                  <c:v>31648.533787987428</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3453,61 +3453,61 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>82.991089491917293</c:v>
+                  <c:v>72.953282922804277</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>124.60989510961691</c:v>
+                  <c:v>110.01759029135798</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>181.23006879741044</c:v>
+                  <c:v>162.46192806212051</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>257.55225352912061</c:v>
+                  <c:v>235.39755088761768</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>359.54303504862804</c:v>
+                  <c:v>335.25714063196648</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>494.72364810730016</c:v>
+                  <c:v>470.04883659023551</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>672.51334256763482</c:v>
+                  <c:v>649.64389337482669</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>904.63576698797078</c:v>
+                  <c:v>886.10059162299387</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1205.5977183907103</c:v>
+                  <c:v>1194.0271017006896</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1593.2506834355358</c:v>
+                  <c:v>1590.9860743466438</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2089.4467629187866</c:v>
+                  <c:v>2097.9438047900244</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2720.8018332758793</c:v>
+                  <c:v>2739.7668883509732</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3519.5801605773704</c:v>
+                  <c:v>3545.7693559555992</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4524.7161495086202</c:v>
+                  <c:v>4550.313347420175</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5782.9904872628686</c:v>
+                  <c:v>5793.4664488331027</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7350.3796355365848</c:v>
+                  <c:v>7321.7188879328478</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9293.5994384017631</c:v>
+                  <c:v>9188.7638480887817</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>11691.865555372824</c:v>
+                  <c:v>11456.344227376318</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>14638.895503243941</c:v>
+                  <c:v>14195.169234336139</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6717,10 +6717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75855736-B2B6-4FFD-943C-E355D55A5C8E}">
-  <dimension ref="A2:U42"/>
+  <dimension ref="A2:U77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AN75" sqref="AN75"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6789,7 +6789,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="8">
-        <v>0.99999999999999967</v>
+        <v>3.3226752845112602</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>4</v>
@@ -6802,11 +6802,11 @@
         <v>7</v>
       </c>
       <c r="B7" s="7">
-        <v>20.586182670858417</v>
+        <v>40</v>
       </c>
       <c r="D7" s="8">
         <f>SUM(K15:K32)</f>
-        <v>68145.898132718154</v>
+        <v>57686.167562556904</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -6816,7 +6816,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="7">
-        <v>1.4263670838975049</v>
+        <v>1.3336642200094939</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -6824,14 +6824,12 @@
         <v>10</v>
       </c>
       <c r="B9" s="7">
-        <v>0.53279454887650068</v>
+        <v>0.19052659525960408</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
-      <c r="B10" s="7">
-        <v>-18.28690681556942</v>
-      </c>
+      <c r="B10" s="7"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -6867,23 +6865,23 @@
         <v>53</v>
       </c>
       <c r="H15" s="5">
-        <f xml:space="preserve"> $B$6* ((($B$6/$B$7)*C15+$B$8)^$B$7)^$B$9 + $B$10</f>
-        <v>30.876361337559839</v>
+        <f xml:space="preserve"> $B$6* ((($B$6/$B$7)*C15+$B$8)^$B$7)^$B$9</f>
+        <v>29.81777657449534</v>
       </c>
       <c r="K15" s="5">
         <f>(H15   -F15) ^2</f>
-        <v>489.45538766621706</v>
+        <v>537.41548295001701</v>
       </c>
       <c r="M15" s="1">
         <v>43889</v>
       </c>
       <c r="N15" s="5">
         <f>H17</f>
-        <v>82.991089491917293</v>
+        <v>72.953282922804277</v>
       </c>
       <c r="P15" s="5">
         <f>H19</f>
-        <v>181.23006879741044</v>
+        <v>162.46192806212051</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -6897,23 +6895,23 @@
         <v>66</v>
       </c>
       <c r="H16" s="5">
-        <f t="shared" ref="H16:H39" si="0" xml:space="preserve"> $B$6* ((($B$6/$B$7)*C16+$B$8)^$B$7)^$B$9 + $B$10</f>
-        <v>52.697458033206956</v>
+        <f t="shared" ref="H16:H77" si="0" xml:space="preserve"> $B$6* ((($B$6/$B$7)*C16+$B$8)^$B$7)^$B$9</f>
+        <v>47.256227163532522</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" ref="K16:K32" si="1">(H16   -F16) ^2</f>
-        <v>176.95762277829013</v>
+        <v>351.32902014509608</v>
       </c>
       <c r="M16" s="1">
         <v>43890</v>
       </c>
       <c r="N16" s="5">
         <f t="shared" ref="N16:N37" si="2">H18</f>
-        <v>124.60989510961691</v>
+        <v>110.01759029135798</v>
       </c>
       <c r="P16" s="5">
         <f t="shared" ref="P16:P35" si="3">H20</f>
-        <v>257.55225352912061</v>
+        <v>235.39755088761768</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -6928,22 +6926,22 @@
       </c>
       <c r="H17" s="5">
         <f t="shared" si="0"/>
-        <v>82.991089491917293</v>
+        <v>72.953282922804277</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" si="1"/>
-        <v>1156.6059939467784</v>
+        <v>1940.1132852785254</v>
       </c>
       <c r="M17" s="1">
         <v>43891</v>
       </c>
       <c r="N17" s="5">
         <f t="shared" si="2"/>
-        <v>181.23006879741044</v>
+        <v>162.46192806212051</v>
       </c>
       <c r="P17" s="5">
         <f t="shared" si="3"/>
-        <v>359.54303504862804</v>
+        <v>335.25714063196648</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -6958,22 +6956,22 @@
       </c>
       <c r="H18" s="5">
         <f t="shared" si="0"/>
-        <v>124.60989510961691</v>
+        <v>110.01759029135798</v>
       </c>
       <c r="K18" s="5">
         <f t="shared" si="1"/>
-        <v>644.65742634465505</v>
+        <v>1598.593086109712</v>
       </c>
       <c r="M18" s="1">
         <v>43892</v>
       </c>
       <c r="N18" s="5">
         <f t="shared" si="2"/>
-        <v>257.55225352912061</v>
+        <v>235.39755088761768</v>
       </c>
       <c r="P18" s="5">
         <f t="shared" si="3"/>
-        <v>494.72364810730016</v>
+        <v>470.04883659023551</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -6988,22 +6986,22 @@
       </c>
       <c r="H19" s="5">
         <f t="shared" si="0"/>
-        <v>181.23006879741044</v>
+        <v>162.46192806212051</v>
       </c>
       <c r="K19" s="5">
         <f t="shared" si="1"/>
-        <v>45.831968487795734</v>
+        <v>652.19311830430809</v>
       </c>
       <c r="M19" s="1">
         <v>43893</v>
       </c>
       <c r="N19" s="5">
         <f t="shared" si="2"/>
-        <v>359.54303504862804</v>
+        <v>335.25714063196648</v>
       </c>
       <c r="P19" s="5">
         <f t="shared" si="3"/>
-        <v>672.51334256763482</v>
+        <v>649.64389337482669</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -7018,22 +7016,22 @@
       </c>
       <c r="H20" s="5">
         <f t="shared" si="0"/>
-        <v>257.55225352912061</v>
+        <v>235.39755088761768</v>
       </c>
       <c r="K20" s="5">
         <f t="shared" si="1"/>
-        <v>308.08160395052676</v>
+        <v>21.182537832068775</v>
       </c>
       <c r="M20" s="1">
         <v>43894</v>
       </c>
       <c r="N20" s="5">
         <f t="shared" si="2"/>
-        <v>494.72364810730016</v>
+        <v>470.04883659023551</v>
       </c>
       <c r="P20" s="5">
         <f t="shared" si="3"/>
-        <v>904.63576698797078</v>
+        <v>886.10059162299387</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -7048,22 +7046,22 @@
       </c>
       <c r="H21" s="5">
         <f t="shared" si="0"/>
-        <v>359.54303504862804</v>
+        <v>335.25714063196648</v>
       </c>
       <c r="K21" s="5">
         <f t="shared" si="1"/>
-        <v>111.1555880365993</v>
+        <v>188.86618360954671</v>
       </c>
       <c r="M21" s="1">
         <v>43895</v>
       </c>
       <c r="N21" s="5">
         <f t="shared" si="2"/>
-        <v>672.51334256763482</v>
+        <v>649.64389337482669</v>
       </c>
       <c r="P21" s="5">
         <f t="shared" si="3"/>
-        <v>1205.5977183907103</v>
+        <v>1194.0271017006896</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -7078,22 +7076,22 @@
       </c>
       <c r="H22" s="5">
         <f t="shared" si="0"/>
-        <v>494.72364810730016</v>
+        <v>470.04883659023551</v>
       </c>
       <c r="K22" s="5">
         <f t="shared" si="1"/>
-        <v>1542.6318179991861</v>
+        <v>4089.7513014624005</v>
       </c>
       <c r="M22" s="1">
         <v>43896</v>
       </c>
       <c r="N22" s="5">
         <f t="shared" si="2"/>
-        <v>904.63576698797078</v>
+        <v>886.10059162299387</v>
       </c>
       <c r="P22" s="5">
         <f t="shared" si="3"/>
-        <v>1593.2506834355358</v>
+        <v>1590.9860743466438</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -7108,22 +7106,22 @@
       </c>
       <c r="H23" s="5">
         <f t="shared" si="0"/>
-        <v>672.51334256763482</v>
+        <v>649.64389337482669</v>
       </c>
       <c r="K23" s="5">
         <f t="shared" si="1"/>
-        <v>131.94329896851016</v>
+        <v>1180.3420624402775</v>
       </c>
       <c r="M23" s="1">
         <v>43897</v>
       </c>
       <c r="N23" s="5">
         <f t="shared" si="2"/>
-        <v>1205.5977183907103</v>
+        <v>1194.0271017006896</v>
       </c>
       <c r="P23" s="5">
         <f t="shared" si="3"/>
-        <v>2089.4467629187866</v>
+        <v>2097.9438047900244</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -7138,22 +7136,22 @@
       </c>
       <c r="H24" s="5">
         <f t="shared" si="0"/>
-        <v>904.63576698797078</v>
+        <v>886.10059162299387</v>
       </c>
       <c r="K24" s="5">
         <f t="shared" si="1"/>
-        <v>3321.8816362916627</v>
+        <v>1528.8562652681387</v>
       </c>
       <c r="M24" s="1">
         <v>43898</v>
       </c>
       <c r="N24" s="5">
         <f t="shared" si="2"/>
-        <v>1593.2506834355358</v>
+        <v>1590.9860743466438</v>
       </c>
       <c r="P24" s="5">
         <f t="shared" si="3"/>
-        <v>2720.8018332758793</v>
+        <v>2739.7668883509732</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -7168,22 +7166,22 @@
       </c>
       <c r="H25" s="5">
         <f t="shared" si="0"/>
-        <v>1205.5977183907103</v>
+        <v>1194.0271017006896</v>
       </c>
       <c r="K25" s="5">
         <f t="shared" si="1"/>
-        <v>8760.5328879467033</v>
+        <v>6728.4454134152793</v>
       </c>
       <c r="M25" s="1">
         <v>43899</v>
       </c>
       <c r="N25" s="5">
         <f t="shared" si="2"/>
-        <v>2089.4467629187866</v>
+        <v>2097.9438047900244</v>
       </c>
       <c r="P25" s="5">
         <f t="shared" si="3"/>
-        <v>3519.5801605773704</v>
+        <v>3545.7693559555992</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -7198,22 +7196,22 @@
       </c>
       <c r="H26" s="5">
         <f t="shared" si="0"/>
-        <v>1593.2506834355358</v>
+        <v>1590.9860743466438</v>
       </c>
       <c r="K26" s="5">
         <f t="shared" si="1"/>
-        <v>798.10111457485948</v>
+        <v>675.27605994929991</v>
       </c>
       <c r="M26" s="1">
         <v>43900</v>
       </c>
       <c r="N26" s="5">
         <f t="shared" si="2"/>
-        <v>2720.8018332758793</v>
+        <v>2739.7668883509732</v>
       </c>
       <c r="P26" s="5">
         <f t="shared" si="3"/>
-        <v>4524.7161495086202</v>
+        <v>4550.313347420175</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -7228,22 +7226,22 @@
       </c>
       <c r="H27" s="5">
         <f t="shared" si="0"/>
-        <v>2089.4467629187866</v>
+        <v>2097.9438047900244</v>
       </c>
       <c r="K27" s="5">
         <f t="shared" si="1"/>
-        <v>15239.103275127103</v>
+        <v>17409.167622468063</v>
       </c>
       <c r="M27" s="1">
         <v>43901</v>
       </c>
       <c r="N27" s="5">
         <f t="shared" si="2"/>
-        <v>3519.5801605773704</v>
+        <v>3545.7693559555992</v>
       </c>
       <c r="P27" s="5">
         <f t="shared" si="3"/>
-        <v>5782.9904872628686</v>
+        <v>5793.4664488331027</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -7258,22 +7256,22 @@
       </c>
       <c r="H28" s="5">
         <f t="shared" si="0"/>
-        <v>2720.8018332758793</v>
+        <v>2739.7668883509732</v>
       </c>
       <c r="K28" s="5">
         <f t="shared" si="1"/>
-        <v>585.55127280834279</v>
+        <v>27.385457531179952</v>
       </c>
       <c r="M28" s="1">
         <v>43902</v>
       </c>
       <c r="N28" s="5">
         <f t="shared" si="2"/>
-        <v>4524.7161495086202</v>
+        <v>4550.313347420175</v>
       </c>
       <c r="P28" s="5">
         <f t="shared" si="3"/>
-        <v>7350.3796355365848</v>
+        <v>7321.7188879328478</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -7288,22 +7286,22 @@
       </c>
       <c r="H29" s="5">
         <f t="shared" si="0"/>
-        <v>3519.5801605773704</v>
+        <v>3545.7693559555992</v>
       </c>
       <c r="K29" s="5">
         <f t="shared" si="1"/>
-        <v>24155.326486155969</v>
+        <v>16700.559360130632</v>
       </c>
       <c r="M29" s="1">
         <v>43903</v>
       </c>
       <c r="N29" s="5">
         <f t="shared" si="2"/>
-        <v>5782.9904872628686</v>
+        <v>5793.4664488331027</v>
       </c>
       <c r="P29" s="5">
         <f t="shared" si="3"/>
-        <v>9293.5994384017631</v>
+        <v>9188.7638480887817</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -7318,22 +7316,22 @@
       </c>
       <c r="H30" s="5">
         <f t="shared" si="0"/>
-        <v>4524.7161495086202</v>
+        <v>4550.313347420175</v>
       </c>
       <c r="K30" s="5">
         <f t="shared" si="1"/>
-        <v>3634.14263006703</v>
+        <v>1203.1638671934818</v>
       </c>
       <c r="M30" s="1">
         <v>43904</v>
       </c>
       <c r="N30" s="5">
         <f t="shared" si="2"/>
-        <v>7350.3796355365848</v>
+        <v>7321.7188879328478</v>
       </c>
       <c r="P30" s="5">
         <f t="shared" si="3"/>
-        <v>11691.865555372824</v>
+        <v>11456.344227376318</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -7348,22 +7346,22 @@
       </c>
       <c r="H31" s="5">
         <f t="shared" si="0"/>
-        <v>5782.9904872628686</v>
+        <v>5793.4664488331027</v>
       </c>
       <c r="K31" s="5">
         <f t="shared" si="1"/>
-        <v>900.5708547200544</v>
+        <v>381.55962118979363</v>
       </c>
       <c r="M31" s="1">
         <v>43905</v>
       </c>
       <c r="N31" s="5">
         <f t="shared" si="2"/>
-        <v>9293.5994384017631</v>
+        <v>9188.7638480887817</v>
       </c>
       <c r="P31" s="5">
         <f t="shared" si="3"/>
-        <v>14638.895503243941</v>
+        <v>14195.169234336139</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -7378,22 +7376,22 @@
       </c>
       <c r="H32" s="5">
         <f t="shared" si="0"/>
-        <v>7350.3796355365848</v>
+        <v>7321.7188879328478</v>
       </c>
       <c r="K32" s="5">
         <f t="shared" si="1"/>
-        <v>6143.3672668478712</v>
+        <v>2471.9678172790777</v>
       </c>
       <c r="M32" s="1">
         <v>43906</v>
       </c>
       <c r="N32" s="5">
         <f t="shared" si="2"/>
-        <v>11691.865555372824</v>
+        <v>11456.344227376318</v>
       </c>
       <c r="P32" s="5">
         <f t="shared" si="3"/>
-        <v>18245.179303129124</v>
+        <v>17485.904276350782</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -7405,18 +7403,18 @@
       </c>
       <c r="H33" s="5">
         <f t="shared" si="0"/>
-        <v>9293.5994384017631</v>
+        <v>9188.7638480887817</v>
       </c>
       <c r="M33" s="1">
         <v>43907</v>
       </c>
       <c r="N33" s="5">
         <f t="shared" si="2"/>
-        <v>14638.895503243941</v>
+        <v>14195.169234336139</v>
       </c>
       <c r="P33" s="5">
         <f t="shared" si="3"/>
-        <v>22640.548086600076</v>
+        <v>21420.237660192757</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -7428,16 +7426,16 @@
       </c>
       <c r="H34" s="5">
         <f t="shared" si="0"/>
-        <v>11691.865555372824</v>
+        <v>11456.344227376318</v>
       </c>
       <c r="N34" s="5">
         <f t="shared" si="2"/>
-        <v>18245.179303129124</v>
+        <v>17485.904276350782</v>
       </c>
       <c r="O34" s="1"/>
       <c r="P34" s="5">
         <f t="shared" si="3"/>
-        <v>27977.072523021798</v>
+        <v>26102.027687224239</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -7449,16 +7447,16 @@
       </c>
       <c r="H35" s="5">
         <f t="shared" si="0"/>
-        <v>14638.895503243941</v>
+        <v>14195.169234336139</v>
       </c>
       <c r="N35" s="5">
         <f t="shared" si="2"/>
-        <v>22640.548086600076</v>
+        <v>21420.237660192757</v>
       </c>
       <c r="O35" s="1"/>
       <c r="P35" s="5">
         <f t="shared" si="3"/>
-        <v>34432.32559538725</v>
+        <v>31648.533787987428</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -7470,11 +7468,11 @@
       </c>
       <c r="H36" s="5">
         <f t="shared" si="0"/>
-        <v>18245.179303129124</v>
+        <v>17485.904276350782</v>
       </c>
       <c r="N36" s="5">
         <f t="shared" si="2"/>
-        <v>27977.072523021798</v>
+        <v>26102.027687224239</v>
       </c>
       <c r="O36" s="1"/>
       <c r="P36" s="5"/>
@@ -7488,11 +7486,11 @@
       </c>
       <c r="H37" s="5">
         <f t="shared" si="0"/>
-        <v>22640.548086600076</v>
+        <v>21420.237660192757</v>
       </c>
       <c r="N37" s="5">
         <f t="shared" si="2"/>
-        <v>34432.32559538725</v>
+        <v>31648.533787987428</v>
       </c>
       <c r="O37" s="1"/>
       <c r="P37" s="5"/>
@@ -7506,7 +7504,7 @@
       </c>
       <c r="H38" s="5">
         <f t="shared" si="0"/>
-        <v>27977.072523021798</v>
+        <v>26102.027687224239</v>
       </c>
       <c r="N38" s="5"/>
       <c r="O38" s="1"/>
@@ -7520,13 +7518,353 @@
       </c>
       <c r="H39" s="5">
         <f t="shared" si="0"/>
-        <v>34432.32559538725</v>
+        <v>31648.533787987428</v>
       </c>
       <c r="N39" s="5"/>
       <c r="O39" s="1"/>
     </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>25</v>
+      </c>
+      <c r="H40" s="5">
+        <f t="shared" si="0"/>
+        <v>38191.735402540158</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>26</v>
+      </c>
+      <c r="H41" s="5">
+        <f t="shared" si="0"/>
+        <v>45879.742373888963</v>
+      </c>
+    </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="5"/>
+      <c r="C42">
+        <v>27</v>
+      </c>
+      <c r="H42" s="5">
+        <f t="shared" si="0"/>
+        <v>54878.300682271503</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <v>28</v>
+      </c>
+      <c r="H43" s="5">
+        <f t="shared" si="0"/>
+        <v>65372.397407863755</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>29</v>
+      </c>
+      <c r="H44" s="5">
+        <f t="shared" si="0"/>
+        <v>77567.968868756361</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>30</v>
+      </c>
+      <c r="H45" s="5">
+        <f t="shared" si="0"/>
+        <v>91693.71593977038</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>31</v>
+      </c>
+      <c r="H46" s="5">
+        <f t="shared" si="0"/>
+        <v>108003.03061589133</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <v>32</v>
+      </c>
+      <c r="H47" s="5">
+        <f t="shared" si="0"/>
+        <v>126776.03794180931</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <v>33</v>
+      </c>
+      <c r="H48" s="5">
+        <f t="shared" si="0"/>
+        <v>148321.75748625695</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <v>34</v>
+      </c>
+      <c r="H49" s="5">
+        <f t="shared" si="0"/>
+        <v>172980.38859658601</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <v>35</v>
+      </c>
+      <c r="H50" s="5">
+        <f t="shared" si="0"/>
+        <v>201125.72372530139</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>36</v>
+      </c>
+      <c r="H51" s="5">
+        <f t="shared" si="0"/>
+        <v>233167.69417610325</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>37</v>
+      </c>
+      <c r="H52" s="5">
+        <f t="shared" si="0"/>
+        <v>269555.05267238722</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>38</v>
+      </c>
+      <c r="H53" s="5">
+        <f t="shared" si="0"/>
+        <v>310778.19720612897</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>39</v>
+      </c>
+      <c r="H54" s="5">
+        <f t="shared" si="0"/>
+        <v>357372.14067964943</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>40</v>
+      </c>
+      <c r="H55" s="5">
+        <f t="shared" si="0"/>
+        <v>409919.63090692088</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>41</v>
+      </c>
+      <c r="H56" s="5">
+        <f t="shared" si="0"/>
+        <v>469054.42559484491</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>42</v>
+      </c>
+      <c r="H57" s="5">
+        <f t="shared" si="0"/>
+        <v>535464.72697834228</v>
+      </c>
+    </row>
+    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>43</v>
+      </c>
+      <c r="H58" s="5">
+        <f t="shared" si="0"/>
+        <v>609896.78083612805</v>
+      </c>
+    </row>
+    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>44</v>
+      </c>
+      <c r="H59" s="5">
+        <f t="shared" si="0"/>
+        <v>693158.64466666582</v>
+      </c>
+    </row>
+    <row r="60" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>45</v>
+      </c>
+      <c r="H60" s="5">
+        <f t="shared" si="0"/>
+        <v>786124.12985620892</v>
+      </c>
+    </row>
+    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>46</v>
+      </c>
+      <c r="H61" s="5">
+        <f t="shared" si="0"/>
+        <v>889736.9227226699</v>
+      </c>
+    </row>
+    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>47</v>
+      </c>
+      <c r="H62" s="5">
+        <f t="shared" si="0"/>
+        <v>1005014.8893708574</v>
+      </c>
+    </row>
+    <row r="63" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <v>48</v>
+      </c>
+      <c r="H63" s="5">
+        <f t="shared" si="0"/>
+        <v>1133054.569345765</v>
+      </c>
+    </row>
+    <row r="64" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <v>49</v>
+      </c>
+      <c r="H64" s="5">
+        <f t="shared" si="0"/>
+        <v>1275035.8631217368</v>
+      </c>
+    </row>
+    <row r="65" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>50</v>
+      </c>
+      <c r="H65" s="5">
+        <f t="shared" si="0"/>
+        <v>1432226.9185158787</v>
+      </c>
+    </row>
+    <row r="66" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <v>51</v>
+      </c>
+      <c r="H66" s="5">
+        <f t="shared" si="0"/>
+        <v>1605989.2211645634</v>
+      </c>
+    </row>
+    <row r="67" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <v>52</v>
+      </c>
+      <c r="H67" s="5">
+        <f t="shared" si="0"/>
+        <v>1797782.8942518805</v>
+      </c>
+    </row>
+    <row r="68" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <v>53</v>
+      </c>
+      <c r="H68" s="5">
+        <f t="shared" si="0"/>
+        <v>2009172.2127286596</v>
+      </c>
+    </row>
+    <row r="69" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <v>54</v>
+      </c>
+      <c r="H69" s="5">
+        <f t="shared" si="0"/>
+        <v>2241831.3373102578</v>
+      </c>
+    </row>
+    <row r="70" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <v>55</v>
+      </c>
+      <c r="H70" s="5">
+        <f t="shared" si="0"/>
+        <v>2497550.2735904045</v>
+      </c>
+    </row>
+    <row r="71" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <v>56</v>
+      </c>
+      <c r="H71" s="5">
+        <f t="shared" si="0"/>
+        <v>2778241.0616573994</v>
+      </c>
+    </row>
+    <row r="72" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C72">
+        <v>57</v>
+      </c>
+      <c r="H72" s="5">
+        <f t="shared" si="0"/>
+        <v>3085944.2016476658</v>
+      </c>
+    </row>
+    <row r="73" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C73">
+        <v>58</v>
+      </c>
+      <c r="H73" s="5">
+        <f t="shared" si="0"/>
+        <v>3422835.320719895</v>
+      </c>
+    </row>
+    <row r="74" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C74">
+        <v>59</v>
+      </c>
+      <c r="H74" s="5">
+        <f t="shared" si="0"/>
+        <v>3791232.0869814293</v>
+      </c>
+    </row>
+    <row r="75" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <v>60</v>
+      </c>
+      <c r="H75" s="5">
+        <f t="shared" si="0"/>
+        <v>4193601.3759459853</v>
+      </c>
+    </row>
+    <row r="76" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C76">
+        <v>61</v>
+      </c>
+      <c r="H76" s="5">
+        <f t="shared" si="0"/>
+        <v>4632566.6951501435</v>
+      </c>
+    </row>
+    <row r="77" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C77">
+        <v>62</v>
+      </c>
+      <c r="H77" s="5">
+        <f t="shared" si="0"/>
+        <v>5110915.8726025634</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update with new logistic model
</commit_message>
<xml_diff>
--- a/Covid19_Germany_Estimates/Corona_Deutschland_Modellierung_08-03-2020.xlsx
+++ b/Covid19_Germany_Estimates/Corona_Deutschland_Modellierung_08-03-2020.xlsx
@@ -8,72 +8,124 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benni\Desktop\Covid19_Germany_Estimates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62605E5-6110-4CB1-960A-B589573E4C65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E72141-3E7C-4E7A-8B41-A690663EBB2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4905" yWindow="195" windowWidth="18060" windowHeight="14940" xr2:uid="{8F2FD530-AE1D-479B-B999-25EE25C3C974}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{8F2FD530-AE1D-479B-B999-25EE25C3C974}"/>
   </bookViews>
   <sheets>
     <sheet name="Polynomial-Exponential Growth" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$6:$B$9</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">Sheet1!$B$5:$B$7</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$10</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">Sheet1!$B$5</definedName>
     <definedName name="solver_lhs10" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$9</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$10</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">Sheet1!$B$5</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$6</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">Sheet1!$B$6</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$6</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">Sheet1!$B$6</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$7</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">Sheet1!$B$7</definedName>
     <definedName name="solver_lhs6" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$7</definedName>
+    <definedName name="solver_lhs6" localSheetId="1" hidden="1">Sheet1!$B$7</definedName>
     <definedName name="solver_lhs7" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$8</definedName>
+    <definedName name="solver_lhs7" localSheetId="1" hidden="1">Sheet1!$B$8</definedName>
     <definedName name="solver_lhs8" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$8</definedName>
+    <definedName name="solver_lhs8" localSheetId="1" hidden="1">Sheet1!$B$8</definedName>
     <definedName name="solver_lhs9" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$B$9</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">10</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">6</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'Polynomial-Exponential Growth'!$D$7</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">Sheet1!$D$6</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel10" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel5" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel6" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel6" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel7" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel7" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel8" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel8" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel9" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">-100</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">100000</definedName>
     <definedName name="solver_rhs10" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">1000</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">40</definedName>
+    <definedName name="solver_rhs5" localSheetId="1" hidden="1">1000</definedName>
     <definedName name="solver_rhs6" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs6" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rhs7" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rhs7" localSheetId="1" hidden="1">1000</definedName>
     <definedName name="solver_rhs8" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rhs8" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rhs9" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -93,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>Bestätigte Fälle</t>
   </si>
@@ -142,12 +194,24 @@
   <si>
     <t>^2 Error</t>
   </si>
+  <si>
+    <t>Fallzahl = a/(1 + exp(-b·(x - c)))</t>
+  </si>
+  <si>
+    <t>Siehe: https://obsigna.com/articles/1584931539.html</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +234,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="6">
@@ -216,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -227,6 +296,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -320,7 +395,7 @@
         <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="2"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
@@ -336,7 +411,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent3"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -347,10 +422,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Polynomial-Exponential Growth'!$C$14:$C$34</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$C$14:$C$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
@@ -410,16 +485,28 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Polynomial-Exponential Growth'!$F$14:$F$34</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$F$14:$F$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="1">
                   <c:v>53</c:v>
                 </c:pt>
@@ -479,6 +566,18 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>12327</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15320</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>19848</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22364</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24873</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -486,12 +585,12 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-40A8-46EE-AAFB-FEBC15CDF71D}"/>
+              <c16:uniqueId val="{00000001-5848-4C2D-8FAF-EBF40DEEDBD9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
-          <c:idx val="3"/>
+          <c:idx val="4"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
@@ -507,7 +606,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent5"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -518,10 +617,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Polynomial-Exponential Growth'!$C$14:$C$34</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$C$14:$C$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
@@ -581,16 +680,28 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Polynomial-Exponential Growth'!$H$14:$H$34</c:f>
+              <c:f>'Polynomial-Exponential Growth'!$H$14:$H$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="21"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="1">
                   <c:v>57.037922156925774</c:v>
                 </c:pt>
@@ -650,6 +761,18 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>12170.325649982035</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15473.612845197047</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>19607.382929936077</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24764.314766447147</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>31178.163650145754</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -657,7 +780,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-40A8-46EE-AAFB-FEBC15CDF71D}"/>
+              <c16:uniqueId val="{00000003-5848-4C2D-8FAF-EBF40DEEDBD9}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1276,6 +1399,18 @@
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>12327</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15320</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>19848</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22364</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24873</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2503,6 +2638,18 @@
                 <c:pt idx="20">
                   <c:v>12327</c:v>
                 </c:pt>
+                <c:pt idx="21">
+                  <c:v>15320</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>19848</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22364</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24873</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -3846,6 +3993,1158 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Early</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Logistical Model</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Bestätigte Fälle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$13:$C$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="64"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$F$13:$F$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="64"/>
+                <c:pt idx="1">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>188</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>349</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>534</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>684</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>847</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1112</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1565</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1966</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2745</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3675</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4585</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5813</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7272</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9360</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12327</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15320</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>19848</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22364</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24873</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D966-4BD8-BCD4-71B3E0FFA54B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Vorhergesagte Fälle</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$C$13:$C$76</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="64"/>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$13:$H$76</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="64"/>
+                <c:pt idx="1">
+                  <c:v>41.999922515864377</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57.731227098782462</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>79.343691366858394</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>109.02614442981582</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>149.77331618671971</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>205.67483533419212</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>282.30103111212105</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>387.21188493963376</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>530.6170501434159</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>726.21048052783112</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>992.18610682527219</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1352.3996233811579</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1837.5580324661978</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2486.1700448994734</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3344.7565895934708</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4466.5092992988166</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5907.2840967386028</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7717.7709844829142</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9931.326523605725</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12548.754917422448</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>15524.204023179205</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18758.912822493527</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>22109.131605133323</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25409.280263859553</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>28503.376074201584</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>31272.760525139111</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>33650.440124121022</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>35619.939875773933</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>37203.462142722397</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>38446.438132170704</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>39403.838407041236</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>40130.59447455428</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>40676.18393923968</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>41082.3666868152</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>41382.889689779702</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>41604.217127119118</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>41766.667196067698</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>41885.605840201664</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>41972.528685164667</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>42035.969073187051</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42082.225814514873</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42115.929391528327</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>42140.473787195224</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>42158.341341320345</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>42171.344796908517</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>42180.80642291157</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>42187.689929119093</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>42192.697276896579</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>42196.339549312252</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>42198.988737529377</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>42200.915532683248</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>42202.316878856473</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>42203.336047320852</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>42204.077254689808</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>42204.61630405474</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>42205.008329047756</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>42205.293428484641</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>42205.500765605146</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>42205.651549995324</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>42205.761206576091</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>42205.840953196101</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>42205.898948033922</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>42205.941124093799</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-D966-4BD8-BCD4-71B3E0FFA54B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="687713776"/>
+        <c:axId val="687716400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="687713776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Days since n &gt;= 53</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="687716400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="687716400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Case Number</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="687713776"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4006,6 +5305,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -5555,6 +6894,522 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6438,6 +8293,47 @@
 </c:userShapes>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>308160</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>90767</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>294408</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>121227</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4787CC3E-8403-45EB-9504-4FE80984C8AB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6737,11 +8633,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75855736-B2B6-4FFD-943C-E355D55A5C8E}">
   <dimension ref="A2:U77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -6753,7 +8649,7 @@
     <col min="16" max="16" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" ht="21" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:21" ht="21">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -6775,7 +8671,7 @@
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21">
       <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
@@ -6802,7 +8698,7 @@
       <c r="T4" s="9"/>
       <c r="U4" s="9"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
@@ -6815,7 +8711,7 @@
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
@@ -6829,7 +8725,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21">
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
@@ -6837,7 +8733,7 @@
         <v>1.2704805293787489</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
@@ -6845,13 +8741,13 @@
         <v>0.42235648449558316</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21">
       <c r="A10" s="7"/>
       <c r="B10" s="7">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -6874,7 +8770,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21">
       <c r="A15" s="1">
         <v>43889</v>
       </c>
@@ -6904,7 +8800,7 @@
         <v>204.97388525803987</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21">
       <c r="A16" s="1">
         <v>43890</v>
       </c>
@@ -6934,7 +8830,7 @@
         <v>278.13140503169456</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16">
       <c r="A17" s="1">
         <v>43891</v>
       </c>
@@ -6964,7 +8860,7 @@
         <v>375.36112160986215</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16">
       <c r="A18" s="1">
         <v>43892</v>
       </c>
@@ -6994,7 +8890,7 @@
         <v>503.93942924996497</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16">
       <c r="A19" s="1">
         <v>43893</v>
       </c>
@@ -7024,7 +8920,7 @@
         <v>673.15487953239381</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16">
       <c r="A20" s="1">
         <v>43894</v>
       </c>
@@ -7054,7 +8950,7 @@
         <v>894.81476942681286</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16">
       <c r="A21" s="1">
         <v>43895</v>
       </c>
@@ -7084,7 +8980,7 @@
         <v>1183.8671881976884</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16">
       <c r="A22" s="1">
         <v>43896</v>
       </c>
@@ -7114,7 +9010,7 @@
         <v>1559.1621847672798</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16">
       <c r="A23" s="1">
         <v>43897</v>
       </c>
@@ -7144,7 +9040,7 @@
         <v>2044.3800420277912</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16">
       <c r="A24" s="1">
         <v>43898</v>
       </c>
@@ -7174,7 +9070,7 @@
         <v>2669.1596675257688</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16">
       <c r="A25" s="1">
         <v>43899</v>
       </c>
@@ -7204,7 +9100,7 @@
         <v>3470.4659291981052</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16">
       <c r="A26" s="1">
         <v>43900</v>
       </c>
@@ -7234,7 +9130,7 @@
         <v>4494.2414905606947</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16">
       <c r="A27" s="1">
         <v>43901</v>
       </c>
@@ -7264,7 +9160,7 @@
         <v>5797.3964551606559</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16">
       <c r="A28" s="1">
         <v>43902</v>
       </c>
@@ -7294,7 +9190,7 @@
         <v>7450.1980528096983</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16">
       <c r="A29" s="1">
         <v>43903</v>
       </c>
@@ -7324,7 +9220,7 @@
         <v>9539.1328435281466</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16">
       <c r="A30" s="1">
         <v>43904</v>
       </c>
@@ -7354,7 +9250,7 @@
         <v>12170.325649982035</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16">
       <c r="A31" s="1">
         <v>43905</v>
       </c>
@@ -7384,7 +9280,7 @@
         <v>15473.612845197047</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16">
       <c r="A32" s="1">
         <v>43906</v>
       </c>
@@ -7414,7 +9310,7 @@
         <v>19607.382929936077</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16">
       <c r="A33" s="1">
         <v>43907</v>
       </c>
@@ -7444,7 +9340,7 @@
         <v>24764.314766447147</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16">
       <c r="A34" s="1">
         <v>43908</v>
       </c>
@@ -7472,12 +9368,15 @@
         <v>31178.163650145754</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16">
       <c r="A35" s="1">
         <v>43909</v>
       </c>
       <c r="C35">
         <v>20</v>
+      </c>
+      <c r="F35">
+        <v>15320</v>
       </c>
       <c r="H35" s="5">
         <f t="shared" si="0"/>
@@ -7493,12 +9392,15 @@
         <v>39131.767882935746</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16">
       <c r="A36" s="1">
         <v>43910</v>
       </c>
       <c r="C36">
         <v>21</v>
+      </c>
+      <c r="F36">
+        <v>19848</v>
       </c>
       <c r="H36" s="5">
         <f t="shared" si="0"/>
@@ -7511,12 +9413,15 @@
       <c r="O36" s="1"/>
       <c r="P36" s="5"/>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16">
       <c r="A37" s="1">
         <v>43911</v>
       </c>
       <c r="C37">
         <v>22</v>
+      </c>
+      <c r="F37">
+        <v>22364</v>
       </c>
       <c r="H37" s="5">
         <f t="shared" si="0"/>
@@ -7529,13 +9434,16 @@
       <c r="O37" s="1"/>
       <c r="P37" s="5"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16">
       <c r="A38" s="1">
         <v>43912</v>
       </c>
       <c r="C38">
         <v>23</v>
       </c>
+      <c r="F38">
+        <v>24873</v>
+      </c>
       <c r="H38" s="5">
         <f t="shared" si="0"/>
         <v>31178.163650145754</v>
@@ -7543,7 +9451,7 @@
       <c r="N38" s="5"/>
       <c r="O38" s="1"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16">
       <c r="A39" s="1">
         <v>43913</v>
       </c>
@@ -7557,7 +9465,7 @@
       <c r="N39" s="5"/>
       <c r="O39" s="1"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16">
       <c r="C40">
         <v>25</v>
       </c>
@@ -7566,7 +9474,7 @@
         <v>48966.473975321882</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16">
       <c r="C41">
         <v>26</v>
       </c>
@@ -7575,7 +9483,7 @@
         <v>61093.20739507574</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16">
       <c r="A42" s="5"/>
       <c r="C42">
         <v>27</v>
@@ -7585,7 +9493,7 @@
         <v>76005.448278385113</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16">
       <c r="C43">
         <v>28</v>
       </c>
@@ -7594,7 +9502,7 @@
         <v>94294.408142978107</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16">
       <c r="C44">
         <v>29</v>
       </c>
@@ -7603,7 +9511,7 @@
         <v>116666.74485008695</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16">
       <c r="C45">
         <v>30</v>
       </c>
@@ -7612,7 +9520,7 @@
         <v>143965.19935557296</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16">
       <c r="C46">
         <v>31</v>
       </c>
@@ -7621,7 +9529,7 @@
         <v>177192.58971977295</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16">
       <c r="C47">
         <v>32</v>
       </c>
@@ -7630,7 +9538,7 @@
         <v>217539.65601160142</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16">
       <c r="C48">
         <v>33</v>
       </c>
@@ -7639,7 +9547,7 @@
         <v>266417.31480116944</v>
       </c>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:8">
       <c r="C49">
         <v>34</v>
       </c>
@@ -7648,7 +9556,7 @@
         <v>325493.95460248081</v>
       </c>
     </row>
-    <row r="50" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:8">
       <c r="C50">
         <v>35</v>
       </c>
@@ -7657,7 +9565,7 @@
         <v>396738.48468307685</v>
       </c>
     </row>
-    <row r="51" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:8">
       <c r="C51">
         <v>36</v>
       </c>
@@ -7666,7 +9574,7 @@
         <v>482469.93994970381</v>
       </c>
     </row>
-    <row r="52" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:8">
       <c r="C52">
         <v>37</v>
       </c>
@@ -7675,7 +9583,7 @@
         <v>585414.545070605</v>
       </c>
     </row>
-    <row r="53" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:8">
       <c r="C53">
         <v>38</v>
       </c>
@@ -7684,7 +9592,7 @@
         <v>708771.25260806025</v>
       </c>
     </row>
-    <row r="54" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:8">
       <c r="C54">
         <v>39</v>
       </c>
@@ -7693,7 +9601,7 @@
         <v>856286.89379689924</v>
       </c>
     </row>
-    <row r="55" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:8">
       <c r="C55">
         <v>40</v>
       </c>
@@ -7702,7 +9610,7 @@
         <v>1032342.2178945248</v>
       </c>
     </row>
-    <row r="56" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:8">
       <c r="C56">
         <v>41</v>
       </c>
@@ -7711,7 +9619,7 @@
         <v>1242050.2480223014</v>
       </c>
     </row>
-    <row r="57" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:8">
       <c r="C57">
         <v>42</v>
       </c>
@@ -7720,7 +9628,7 @@
         <v>1491368.5494987571</v>
       </c>
     </row>
-    <row r="58" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:8">
       <c r="C58">
         <v>43</v>
       </c>
@@ -7729,7 +9637,7 @@
         <v>1787227.1923250416</v>
       </c>
     </row>
-    <row r="59" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:8">
       <c r="C59">
         <v>44</v>
       </c>
@@ -7738,7 +9646,7 @@
         <v>2137674.3943362511</v>
       </c>
     </row>
-    <row r="60" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:8">
       <c r="C60">
         <v>45</v>
       </c>
@@ -7747,7 +9655,7 @@
         <v>2552042.057319208</v>
       </c>
     </row>
-    <row r="61" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:8">
       <c r="C61">
         <v>46</v>
       </c>
@@ -7756,7 +9664,7 @@
         <v>3041133.6569963968</v>
       </c>
     </row>
-    <row r="62" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:8">
       <c r="C62">
         <v>47</v>
       </c>
@@ -7765,7 +9673,7 @@
         <v>3617437.2212088089</v>
       </c>
     </row>
-    <row r="63" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:8">
       <c r="C63">
         <v>48</v>
       </c>
@@ -7774,7 +9682,7 @@
         <v>4295366.431076603</v>
       </c>
     </row>
-    <row r="64" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:8">
       <c r="C64">
         <v>49</v>
       </c>
@@ -7783,7 +9691,7 @@
         <v>5091533.2097179024</v>
       </c>
     </row>
-    <row r="65" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:8">
       <c r="C65">
         <v>50</v>
       </c>
@@ -7792,7 +9700,7 @@
         <v>6025055.5247815559</v>
       </c>
     </row>
-    <row r="66" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:8">
       <c r="C66">
         <v>51</v>
       </c>
@@ -7801,7 +9709,7 @@
         <v>7117904.5273040263</v>
       </c>
     </row>
-    <row r="67" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:8">
       <c r="C67">
         <v>52</v>
       </c>
@@ -7810,7 +9718,7 @@
         <v>8395295.5831390843</v>
       </c>
     </row>
-    <row r="68" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:8">
       <c r="C68">
         <v>53</v>
       </c>
@@ -7819,7 +9727,7 @@
         <v>9886128.2275427822</v>
       </c>
     </row>
-    <row r="69" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:8">
       <c r="C69">
         <v>54</v>
       </c>
@@ -7828,7 +9736,7 @@
         <v>11623480.591766953</v>
       </c>
     </row>
-    <row r="70" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:8">
       <c r="C70">
         <v>55</v>
       </c>
@@ -7837,7 +9745,7 @@
         <v>13645164.416295074</v>
       </c>
     </row>
-    <row r="71" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:8">
       <c r="C71">
         <v>56</v>
       </c>
@@ -7846,7 +9754,7 @@
         <v>15994347.382473061</v>
       </c>
     </row>
-    <row r="72" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:8">
       <c r="C72">
         <v>57</v>
       </c>
@@ -7855,7 +9763,7 @@
         <v>18720250.166835226</v>
       </c>
     </row>
-    <row r="73" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:8">
       <c r="C73">
         <v>58</v>
       </c>
@@ -7864,7 +9772,7 @@
         <v>21878926.354783121</v>
       </c>
     </row>
-    <row r="74" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="3:8">
       <c r="C74">
         <v>59</v>
       </c>
@@ -7873,7 +9781,7 @@
         <v>25534134.14710949</v>
       </c>
     </row>
-    <row r="75" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="3:8">
       <c r="C75">
         <v>60</v>
       </c>
@@ -7882,7 +9790,7 @@
         <v>29758309.659166168</v>
       </c>
     </row>
-    <row r="76" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="3:8">
       <c r="C76">
         <v>61</v>
       </c>
@@ -7891,13 +9799,1200 @@
         <v>34633652.553580321</v>
       </c>
     </row>
-    <row r="77" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="3:8">
       <c r="C77">
         <v>62</v>
       </c>
       <c r="H77" s="5">
         <f t="shared" si="0"/>
         <v>40253335.768994063</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C57C0D72-947E-4C2B-A236-E53FEC630DCE}">
+  <dimension ref="A1:T76"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Z45" sqref="Z45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="11" max="11" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="21">
+      <c r="A1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+    </row>
+    <row r="3" spans="1:20">
+      <c r="B3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="M3" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+    </row>
+    <row r="5" spans="1:20">
+      <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="10">
+        <v>42206.053573429082</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:20">
+      <c r="A6" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0.31850361840631491</v>
+      </c>
+      <c r="D6" s="8">
+        <f>SUM(K14:K37)</f>
+        <v>2499738.0804764559</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:20">
+      <c r="A7" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="11">
+        <v>21.700398849377979</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
+      <c r="A8" s="7"/>
+      <c r="B8" s="7"/>
+    </row>
+    <row r="9" spans="1:20">
+      <c r="A9" s="7"/>
+      <c r="B9" s="7"/>
+    </row>
+    <row r="12" spans="1:20">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12" t="s">
+        <v>15</v>
+      </c>
+      <c r="N12" t="s">
+        <v>12</v>
+      </c>
+      <c r="P12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
+      <c r="A14" s="1">
+        <v>43889</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>53</v>
+      </c>
+      <c r="H14" s="5">
+        <f xml:space="preserve"> $B$5 / ( 1 + EXP(-$B$6 * (C14- $B$7)))</f>
+        <v>41.999922515864377</v>
+      </c>
+      <c r="K14" s="5">
+        <f>(H14   -F14) ^2</f>
+        <v>121.0017046569875</v>
+      </c>
+      <c r="M14" s="1">
+        <v>43889</v>
+      </c>
+      <c r="N14" s="5">
+        <f>H16</f>
+        <v>79.343691366858394</v>
+      </c>
+      <c r="P14" s="5">
+        <f>H18</f>
+        <v>149.77331618671971</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
+      <c r="A15" s="1">
+        <v>43890</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>66</v>
+      </c>
+      <c r="H15" s="5">
+        <f t="shared" ref="H15:H76" si="0" xml:space="preserve"> $B$5 / ( 1 + EXP(-$B$6 * (C15- $B$7)))</f>
+        <v>57.731227098782462</v>
+      </c>
+      <c r="K15" s="5">
+        <f t="shared" ref="K15:K37" si="1">(H15   -F15) ^2</f>
+        <v>68.372605291909508</v>
+      </c>
+      <c r="M15" s="1">
+        <v>43890</v>
+      </c>
+      <c r="N15" s="5">
+        <f t="shared" ref="N15:N36" si="2">H17</f>
+        <v>109.02614442981582</v>
+      </c>
+      <c r="P15" s="5">
+        <f t="shared" ref="P15:P34" si="3">H19</f>
+        <v>205.67483533419212</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
+      <c r="A16" s="1">
+        <v>43891</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>117</v>
+      </c>
+      <c r="H16" s="5">
+        <f t="shared" si="0"/>
+        <v>79.343691366858394</v>
+      </c>
+      <c r="K16" s="5">
+        <f t="shared" si="1"/>
+        <v>1417.9975798744151</v>
+      </c>
+      <c r="M16" s="1">
+        <v>43891</v>
+      </c>
+      <c r="N16" s="5">
+        <f t="shared" si="2"/>
+        <v>149.77331618671971</v>
+      </c>
+      <c r="P16" s="5">
+        <f t="shared" si="3"/>
+        <v>282.30103111212105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
+      <c r="A17" s="1">
+        <v>43892</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="F17">
+        <v>150</v>
+      </c>
+      <c r="H17" s="5">
+        <f t="shared" si="0"/>
+        <v>109.02614442981582</v>
+      </c>
+      <c r="K17" s="5">
+        <f t="shared" si="1"/>
+        <v>1678.8568402863136</v>
+      </c>
+      <c r="M17" s="1">
+        <v>43892</v>
+      </c>
+      <c r="N17" s="5">
+        <f t="shared" si="2"/>
+        <v>205.67483533419212</v>
+      </c>
+      <c r="P17" s="5">
+        <f t="shared" si="3"/>
+        <v>387.21188493963376</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
+      <c r="A18" s="1">
+        <v>43893</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>188</v>
+      </c>
+      <c r="H18" s="5">
+        <f t="shared" si="0"/>
+        <v>149.77331618671971</v>
+      </c>
+      <c r="K18" s="5">
+        <f t="shared" si="1"/>
+        <v>1461.2793553605052</v>
+      </c>
+      <c r="M18" s="1">
+        <v>43893</v>
+      </c>
+      <c r="N18" s="5">
+        <f t="shared" si="2"/>
+        <v>282.30103111212105</v>
+      </c>
+      <c r="P18" s="5">
+        <f t="shared" si="3"/>
+        <v>530.6170501434159</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
+      <c r="A19" s="1">
+        <v>43894</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>240</v>
+      </c>
+      <c r="H19" s="5">
+        <f t="shared" si="0"/>
+        <v>205.67483533419212</v>
+      </c>
+      <c r="K19" s="5">
+        <f t="shared" si="1"/>
+        <v>1178.2169293348254</v>
+      </c>
+      <c r="M19" s="1">
+        <v>43894</v>
+      </c>
+      <c r="N19" s="5">
+        <f t="shared" si="2"/>
+        <v>387.21188493963376</v>
+      </c>
+      <c r="P19" s="5">
+        <f t="shared" si="3"/>
+        <v>726.21048052783112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
+      <c r="A20" s="1">
+        <v>43895</v>
+      </c>
+      <c r="C20">
+        <v>6</v>
+      </c>
+      <c r="F20">
+        <v>349</v>
+      </c>
+      <c r="H20" s="5">
+        <f t="shared" si="0"/>
+        <v>282.30103111212105</v>
+      </c>
+      <c r="K20" s="5">
+        <f t="shared" si="1"/>
+        <v>4448.7524507062435</v>
+      </c>
+      <c r="M20" s="1">
+        <v>43895</v>
+      </c>
+      <c r="N20" s="5">
+        <f t="shared" si="2"/>
+        <v>530.6170501434159</v>
+      </c>
+      <c r="P20" s="5">
+        <f t="shared" si="3"/>
+        <v>992.18610682527219</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
+      <c r="A21" s="1">
+        <v>43896</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
+      </c>
+      <c r="F21">
+        <v>534</v>
+      </c>
+      <c r="H21" s="5">
+        <f t="shared" si="0"/>
+        <v>387.21188493963376</v>
+      </c>
+      <c r="K21" s="5">
+        <f t="shared" si="1"/>
+        <v>21546.750722975317</v>
+      </c>
+      <c r="M21" s="1">
+        <v>43896</v>
+      </c>
+      <c r="N21" s="5">
+        <f t="shared" si="2"/>
+        <v>726.21048052783112</v>
+      </c>
+      <c r="P21" s="5">
+        <f t="shared" si="3"/>
+        <v>1352.3996233811579</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
+      <c r="A22" s="1">
+        <v>43897</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="F22">
+        <v>684</v>
+      </c>
+      <c r="H22" s="5">
+        <f t="shared" si="0"/>
+        <v>530.6170501434159</v>
+      </c>
+      <c r="K22" s="5">
+        <f t="shared" si="1"/>
+        <v>23526.329306707394</v>
+      </c>
+      <c r="M22" s="1">
+        <v>43897</v>
+      </c>
+      <c r="N22" s="5">
+        <f t="shared" si="2"/>
+        <v>992.18610682527219</v>
+      </c>
+      <c r="P22" s="5">
+        <f t="shared" si="3"/>
+        <v>1837.5580324661978</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
+      <c r="A23" s="1">
+        <v>43898</v>
+      </c>
+      <c r="C23">
+        <v>9</v>
+      </c>
+      <c r="F23">
+        <v>847</v>
+      </c>
+      <c r="H23" s="5">
+        <f t="shared" si="0"/>
+        <v>726.21048052783112</v>
+      </c>
+      <c r="K23" s="5">
+        <f t="shared" si="1"/>
+        <v>14590.108014317464</v>
+      </c>
+      <c r="M23" s="1">
+        <v>43898</v>
+      </c>
+      <c r="N23" s="5">
+        <f t="shared" si="2"/>
+        <v>1352.3996233811579</v>
+      </c>
+      <c r="P23" s="5">
+        <f t="shared" si="3"/>
+        <v>2486.1700448994734</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
+      <c r="A24" s="1">
+        <v>43899</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="F24">
+        <v>1112</v>
+      </c>
+      <c r="H24" s="5">
+        <f t="shared" si="0"/>
+        <v>992.18610682527219</v>
+      </c>
+      <c r="K24" s="5">
+        <f t="shared" si="1"/>
+        <v>14355.368997685087</v>
+      </c>
+      <c r="M24" s="1">
+        <v>43899</v>
+      </c>
+      <c r="N24" s="5">
+        <f t="shared" si="2"/>
+        <v>1837.5580324661978</v>
+      </c>
+      <c r="P24" s="5">
+        <f t="shared" si="3"/>
+        <v>3344.7565895934708</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
+      <c r="A25" s="1">
+        <v>43900</v>
+      </c>
+      <c r="C25">
+        <v>11</v>
+      </c>
+      <c r="F25">
+        <v>1565</v>
+      </c>
+      <c r="H25" s="5">
+        <f t="shared" si="0"/>
+        <v>1352.3996233811579</v>
+      </c>
+      <c r="K25" s="5">
+        <f t="shared" si="1"/>
+        <v>45198.920138473513</v>
+      </c>
+      <c r="M25" s="1">
+        <v>43900</v>
+      </c>
+      <c r="N25" s="5">
+        <f t="shared" si="2"/>
+        <v>2486.1700448994734</v>
+      </c>
+      <c r="P25" s="5">
+        <f t="shared" si="3"/>
+        <v>4466.5092992988166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
+      <c r="A26" s="1">
+        <v>43901</v>
+      </c>
+      <c r="C26">
+        <v>12</v>
+      </c>
+      <c r="F26">
+        <v>1966</v>
+      </c>
+      <c r="H26" s="5">
+        <f t="shared" si="0"/>
+        <v>1837.5580324661978</v>
+      </c>
+      <c r="K26" s="5">
+        <f t="shared" si="1"/>
+        <v>16497.339023954297</v>
+      </c>
+      <c r="M26" s="1">
+        <v>43901</v>
+      </c>
+      <c r="N26" s="5">
+        <f t="shared" si="2"/>
+        <v>3344.7565895934708</v>
+      </c>
+      <c r="P26" s="5">
+        <f t="shared" si="3"/>
+        <v>5907.2840967386028</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="A27" s="1">
+        <v>43902</v>
+      </c>
+      <c r="C27">
+        <v>13</v>
+      </c>
+      <c r="F27">
+        <v>2745</v>
+      </c>
+      <c r="H27" s="5">
+        <f t="shared" si="0"/>
+        <v>2486.1700448994734</v>
+      </c>
+      <c r="K27" s="5">
+        <f t="shared" si="1"/>
+        <v>66992.945657340621</v>
+      </c>
+      <c r="M27" s="1">
+        <v>43902</v>
+      </c>
+      <c r="N27" s="5">
+        <f t="shared" si="2"/>
+        <v>4466.5092992988166</v>
+      </c>
+      <c r="P27" s="5">
+        <f t="shared" si="3"/>
+        <v>7717.7709844829142</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="A28" s="1">
+        <v>43903</v>
+      </c>
+      <c r="C28">
+        <v>14</v>
+      </c>
+      <c r="F28">
+        <v>3675</v>
+      </c>
+      <c r="H28" s="5">
+        <f t="shared" si="0"/>
+        <v>3344.7565895934708</v>
+      </c>
+      <c r="K28" s="5">
+        <f t="shared" si="1"/>
+        <v>109060.71011693525</v>
+      </c>
+      <c r="M28" s="1">
+        <v>43903</v>
+      </c>
+      <c r="N28" s="5">
+        <f t="shared" si="2"/>
+        <v>5907.2840967386028</v>
+      </c>
+      <c r="P28" s="5">
+        <f t="shared" si="3"/>
+        <v>9931.326523605725</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="A29" s="1">
+        <v>43904</v>
+      </c>
+      <c r="C29">
+        <v>15</v>
+      </c>
+      <c r="F29">
+        <v>4585</v>
+      </c>
+      <c r="H29" s="5">
+        <f t="shared" si="0"/>
+        <v>4466.5092992988166</v>
+      </c>
+      <c r="K29" s="5">
+        <f t="shared" si="1"/>
+        <v>14040.046152657427</v>
+      </c>
+      <c r="M29" s="1">
+        <v>43904</v>
+      </c>
+      <c r="N29" s="5">
+        <f t="shared" si="2"/>
+        <v>7717.7709844829142</v>
+      </c>
+      <c r="P29" s="5">
+        <f t="shared" si="3"/>
+        <v>12548.754917422448</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="A30" s="1">
+        <v>43905</v>
+      </c>
+      <c r="C30">
+        <v>16</v>
+      </c>
+      <c r="F30">
+        <v>5813</v>
+      </c>
+      <c r="H30" s="5">
+        <f t="shared" si="0"/>
+        <v>5907.2840967386028</v>
+      </c>
+      <c r="K30" s="5">
+        <f t="shared" si="1"/>
+        <v>8889.4908978142084</v>
+      </c>
+      <c r="M30" s="1">
+        <v>43905</v>
+      </c>
+      <c r="N30" s="5">
+        <f t="shared" si="2"/>
+        <v>9931.326523605725</v>
+      </c>
+      <c r="P30" s="5">
+        <f t="shared" si="3"/>
+        <v>15524.204023179205</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="A31" s="1">
+        <v>43906</v>
+      </c>
+      <c r="C31">
+        <v>17</v>
+      </c>
+      <c r="F31">
+        <v>7272</v>
+      </c>
+      <c r="H31" s="5">
+        <f t="shared" si="0"/>
+        <v>7717.7709844829142</v>
+      </c>
+      <c r="K31" s="5">
+        <f t="shared" si="1"/>
+        <v>198711.77060686651</v>
+      </c>
+      <c r="M31" s="1">
+        <v>43906</v>
+      </c>
+      <c r="N31" s="5">
+        <f t="shared" si="2"/>
+        <v>12548.754917422448</v>
+      </c>
+      <c r="P31" s="5">
+        <f t="shared" si="3"/>
+        <v>18758.912822493527</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="A32" s="1">
+        <v>43907</v>
+      </c>
+      <c r="C32">
+        <v>18</v>
+      </c>
+      <c r="F32">
+        <v>9360</v>
+      </c>
+      <c r="H32" s="5">
+        <f t="shared" si="0"/>
+        <v>9931.326523605725</v>
+      </c>
+      <c r="K32" s="5">
+        <f t="shared" si="1"/>
+        <v>326413.99657540309</v>
+      </c>
+      <c r="M32" s="1">
+        <v>43907</v>
+      </c>
+      <c r="N32" s="5">
+        <f t="shared" si="2"/>
+        <v>15524.204023179205</v>
+      </c>
+      <c r="P32" s="5">
+        <f t="shared" si="3"/>
+        <v>22109.131605133323</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16">
+      <c r="A33" s="1">
+        <v>43908</v>
+      </c>
+      <c r="C33">
+        <v>19</v>
+      </c>
+      <c r="F33">
+        <v>12327</v>
+      </c>
+      <c r="H33" s="5">
+        <f t="shared" si="0"/>
+        <v>12548.754917422448</v>
+      </c>
+      <c r="K33" s="5">
+        <f t="shared" si="1"/>
+        <v>49175.243401036627</v>
+      </c>
+      <c r="N33" s="5">
+        <f t="shared" si="2"/>
+        <v>18758.912822493527</v>
+      </c>
+      <c r="O33" s="1"/>
+      <c r="P33" s="5">
+        <f t="shared" si="3"/>
+        <v>25409.280263859553</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16">
+      <c r="A34" s="1">
+        <v>43909</v>
+      </c>
+      <c r="C34">
+        <v>20</v>
+      </c>
+      <c r="F34">
+        <v>15320</v>
+      </c>
+      <c r="H34" s="5">
+        <f t="shared" si="0"/>
+        <v>15524.204023179205</v>
+      </c>
+      <c r="K34" s="5">
+        <f t="shared" si="1"/>
+        <v>41699.283082573398</v>
+      </c>
+      <c r="N34" s="5">
+        <f t="shared" si="2"/>
+        <v>22109.131605133323</v>
+      </c>
+      <c r="O34" s="1"/>
+      <c r="P34" s="5">
+        <f t="shared" si="3"/>
+        <v>28503.376074201584</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16">
+      <c r="A35" s="1">
+        <v>43910</v>
+      </c>
+      <c r="C35">
+        <v>21</v>
+      </c>
+      <c r="F35">
+        <v>19848</v>
+      </c>
+      <c r="H35" s="5">
+        <f t="shared" si="0"/>
+        <v>18758.912822493527</v>
+      </c>
+      <c r="K35" s="5">
+        <f t="shared" si="1"/>
+        <v>1186110.8802090166</v>
+      </c>
+      <c r="N35" s="5">
+        <f t="shared" si="2"/>
+        <v>25409.280263859553</v>
+      </c>
+      <c r="O35" s="1"/>
+      <c r="P35" s="5"/>
+    </row>
+    <row r="36" spans="1:16">
+      <c r="A36" s="1">
+        <v>43911</v>
+      </c>
+      <c r="C36">
+        <v>22</v>
+      </c>
+      <c r="F36">
+        <v>22364</v>
+      </c>
+      <c r="H36" s="5">
+        <f t="shared" si="0"/>
+        <v>22109.131605133323</v>
+      </c>
+      <c r="K36" s="5">
+        <f t="shared" si="1"/>
+        <v>64957.898701916223</v>
+      </c>
+      <c r="N36" s="5">
+        <f t="shared" si="2"/>
+        <v>28503.376074201584</v>
+      </c>
+      <c r="O36" s="1"/>
+      <c r="P36" s="5"/>
+    </row>
+    <row r="37" spans="1:16">
+      <c r="A37" s="1">
+        <v>43912</v>
+      </c>
+      <c r="C37">
+        <v>23</v>
+      </c>
+      <c r="F37">
+        <v>24873</v>
+      </c>
+      <c r="H37" s="5">
+        <f t="shared" si="0"/>
+        <v>25409.280263859553</v>
+      </c>
+      <c r="K37" s="5">
+        <f t="shared" si="1"/>
+        <v>287596.52140527189</v>
+      </c>
+      <c r="N37" s="5"/>
+      <c r="O37" s="1"/>
+    </row>
+    <row r="38" spans="1:16">
+      <c r="A38" s="1">
+        <v>43913</v>
+      </c>
+      <c r="C38">
+        <v>24</v>
+      </c>
+      <c r="H38" s="5">
+        <f t="shared" si="0"/>
+        <v>28503.376074201584</v>
+      </c>
+      <c r="N38" s="5"/>
+      <c r="O38" s="1"/>
+    </row>
+    <row r="39" spans="1:16">
+      <c r="C39">
+        <v>25</v>
+      </c>
+      <c r="H39" s="5">
+        <f t="shared" si="0"/>
+        <v>31272.760525139111</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16">
+      <c r="C40">
+        <v>26</v>
+      </c>
+      <c r="H40" s="5">
+        <f t="shared" si="0"/>
+        <v>33650.440124121022</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16">
+      <c r="A41" s="5"/>
+      <c r="C41">
+        <v>27</v>
+      </c>
+      <c r="H41" s="5">
+        <f t="shared" si="0"/>
+        <v>35619.939875773933</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16">
+      <c r="C42">
+        <v>28</v>
+      </c>
+      <c r="H42" s="5">
+        <f t="shared" si="0"/>
+        <v>37203.462142722397</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16">
+      <c r="C43">
+        <v>29</v>
+      </c>
+      <c r="H43" s="5">
+        <f t="shared" si="0"/>
+        <v>38446.438132170704</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16">
+      <c r="C44">
+        <v>30</v>
+      </c>
+      <c r="H44" s="5">
+        <f t="shared" si="0"/>
+        <v>39403.838407041236</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16">
+      <c r="C45">
+        <v>31</v>
+      </c>
+      <c r="H45" s="5">
+        <f t="shared" si="0"/>
+        <v>40130.59447455428</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16">
+      <c r="C46">
+        <v>32</v>
+      </c>
+      <c r="H46" s="5">
+        <f t="shared" si="0"/>
+        <v>40676.18393923968</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16">
+      <c r="C47">
+        <v>33</v>
+      </c>
+      <c r="H47" s="5">
+        <f t="shared" si="0"/>
+        <v>41082.3666868152</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16">
+      <c r="C48">
+        <v>34</v>
+      </c>
+      <c r="H48" s="5">
+        <f t="shared" si="0"/>
+        <v>41382.889689779702</v>
+      </c>
+    </row>
+    <row r="49" spans="3:8">
+      <c r="C49">
+        <v>35</v>
+      </c>
+      <c r="H49" s="5">
+        <f t="shared" si="0"/>
+        <v>41604.217127119118</v>
+      </c>
+    </row>
+    <row r="50" spans="3:8">
+      <c r="C50">
+        <v>36</v>
+      </c>
+      <c r="H50" s="5">
+        <f t="shared" si="0"/>
+        <v>41766.667196067698</v>
+      </c>
+    </row>
+    <row r="51" spans="3:8">
+      <c r="C51">
+        <v>37</v>
+      </c>
+      <c r="H51" s="5">
+        <f t="shared" si="0"/>
+        <v>41885.605840201664</v>
+      </c>
+    </row>
+    <row r="52" spans="3:8">
+      <c r="C52">
+        <v>38</v>
+      </c>
+      <c r="H52" s="5">
+        <f t="shared" si="0"/>
+        <v>41972.528685164667</v>
+      </c>
+    </row>
+    <row r="53" spans="3:8">
+      <c r="C53">
+        <v>39</v>
+      </c>
+      <c r="H53" s="5">
+        <f t="shared" si="0"/>
+        <v>42035.969073187051</v>
+      </c>
+    </row>
+    <row r="54" spans="3:8">
+      <c r="C54">
+        <v>40</v>
+      </c>
+      <c r="H54" s="5">
+        <f t="shared" si="0"/>
+        <v>42082.225814514873</v>
+      </c>
+    </row>
+    <row r="55" spans="3:8">
+      <c r="C55">
+        <v>41</v>
+      </c>
+      <c r="H55" s="5">
+        <f t="shared" si="0"/>
+        <v>42115.929391528327</v>
+      </c>
+    </row>
+    <row r="56" spans="3:8">
+      <c r="C56">
+        <v>42</v>
+      </c>
+      <c r="H56" s="5">
+        <f t="shared" si="0"/>
+        <v>42140.473787195224</v>
+      </c>
+    </row>
+    <row r="57" spans="3:8">
+      <c r="C57">
+        <v>43</v>
+      </c>
+      <c r="H57" s="5">
+        <f t="shared" si="0"/>
+        <v>42158.341341320345</v>
+      </c>
+    </row>
+    <row r="58" spans="3:8">
+      <c r="C58">
+        <v>44</v>
+      </c>
+      <c r="H58" s="5">
+        <f t="shared" si="0"/>
+        <v>42171.344796908517</v>
+      </c>
+    </row>
+    <row r="59" spans="3:8">
+      <c r="C59">
+        <v>45</v>
+      </c>
+      <c r="H59" s="5">
+        <f t="shared" si="0"/>
+        <v>42180.80642291157</v>
+      </c>
+    </row>
+    <row r="60" spans="3:8">
+      <c r="C60">
+        <v>46</v>
+      </c>
+      <c r="H60" s="5">
+        <f t="shared" si="0"/>
+        <v>42187.689929119093</v>
+      </c>
+    </row>
+    <row r="61" spans="3:8">
+      <c r="C61">
+        <v>47</v>
+      </c>
+      <c r="H61" s="5">
+        <f t="shared" si="0"/>
+        <v>42192.697276896579</v>
+      </c>
+    </row>
+    <row r="62" spans="3:8">
+      <c r="C62">
+        <v>48</v>
+      </c>
+      <c r="H62" s="5">
+        <f t="shared" si="0"/>
+        <v>42196.339549312252</v>
+      </c>
+    </row>
+    <row r="63" spans="3:8">
+      <c r="C63">
+        <v>49</v>
+      </c>
+      <c r="H63" s="5">
+        <f t="shared" si="0"/>
+        <v>42198.988737529377</v>
+      </c>
+    </row>
+    <row r="64" spans="3:8">
+      <c r="C64">
+        <v>50</v>
+      </c>
+      <c r="H64" s="5">
+        <f t="shared" si="0"/>
+        <v>42200.915532683248</v>
+      </c>
+    </row>
+    <row r="65" spans="3:8">
+      <c r="C65">
+        <v>51</v>
+      </c>
+      <c r="H65" s="5">
+        <f t="shared" si="0"/>
+        <v>42202.316878856473</v>
+      </c>
+    </row>
+    <row r="66" spans="3:8">
+      <c r="C66">
+        <v>52</v>
+      </c>
+      <c r="H66" s="5">
+        <f t="shared" si="0"/>
+        <v>42203.336047320852</v>
+      </c>
+    </row>
+    <row r="67" spans="3:8">
+      <c r="C67">
+        <v>53</v>
+      </c>
+      <c r="H67" s="5">
+        <f t="shared" si="0"/>
+        <v>42204.077254689808</v>
+      </c>
+    </row>
+    <row r="68" spans="3:8">
+      <c r="C68">
+        <v>54</v>
+      </c>
+      <c r="H68" s="5">
+        <f t="shared" si="0"/>
+        <v>42204.61630405474</v>
+      </c>
+    </row>
+    <row r="69" spans="3:8">
+      <c r="C69">
+        <v>55</v>
+      </c>
+      <c r="H69" s="5">
+        <f t="shared" si="0"/>
+        <v>42205.008329047756</v>
+      </c>
+    </row>
+    <row r="70" spans="3:8">
+      <c r="C70">
+        <v>56</v>
+      </c>
+      <c r="H70" s="5">
+        <f t="shared" si="0"/>
+        <v>42205.293428484641</v>
+      </c>
+    </row>
+    <row r="71" spans="3:8">
+      <c r="C71">
+        <v>57</v>
+      </c>
+      <c r="H71" s="5">
+        <f t="shared" si="0"/>
+        <v>42205.500765605146</v>
+      </c>
+    </row>
+    <row r="72" spans="3:8">
+      <c r="C72">
+        <v>58</v>
+      </c>
+      <c r="H72" s="5">
+        <f t="shared" si="0"/>
+        <v>42205.651549995324</v>
+      </c>
+    </row>
+    <row r="73" spans="3:8">
+      <c r="C73">
+        <v>59</v>
+      </c>
+      <c r="H73" s="5">
+        <f t="shared" si="0"/>
+        <v>42205.761206576091</v>
+      </c>
+    </row>
+    <row r="74" spans="3:8">
+      <c r="C74">
+        <v>60</v>
+      </c>
+      <c r="H74" s="5">
+        <f t="shared" si="0"/>
+        <v>42205.840953196101</v>
+      </c>
+    </row>
+    <row r="75" spans="3:8">
+      <c r="C75">
+        <v>61</v>
+      </c>
+      <c r="H75" s="5">
+        <f t="shared" si="0"/>
+        <v>42205.898948033922</v>
+      </c>
+    </row>
+    <row r="76" spans="3:8">
+      <c r="C76">
+        <v>62</v>
+      </c>
+      <c r="H76" s="5">
+        <f t="shared" si="0"/>
+        <v>42205.941124093799</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make logistic model graph pretty, update dataset
</commit_message>
<xml_diff>
--- a/Covid19_Germany_Estimates/Corona_Deutschland_Modellierung_08-03-2020.xlsx
+++ b/Covid19_Germany_Estimates/Corona_Deutschland_Modellierung_08-03-2020.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benni\Desktop\Covid19_Germany_Estimates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17E72141-3E7C-4E7A-8B41-A690663EBB2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E310310-11D2-4E79-BB8C-E04CA7DBFA0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{8F2FD530-AE1D-479B-B999-25EE25C3C974}"/>
   </bookViews>
@@ -4027,16 +4027,8 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Early</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Logistical Model</a:t>
+              <a:rPr lang="de-DE"/>
+              <a:t>Logistische Anpassung: Deutschland</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4073,8 +4065,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="2"/>
@@ -4092,17 +4084,27 @@
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="22225">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
-          <c:xVal>
+          <c:cat>
             <c:numRef>
               <c:f>Sheet1!$C$13:$C$76</c:f>
               <c:numCache>
@@ -4299,8 +4301,8 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>Sheet1!$F$13:$F$76</c:f>
               <c:numCache>
@@ -4378,9 +4380,12 @@
                 <c:pt idx="24">
                   <c:v>24873</c:v>
                 </c:pt>
+                <c:pt idx="25">
+                  <c:v>29056</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
+          </c:val>
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4405,7 +4410,7 @@
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:schemeClr val="tx2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -4414,7 +4419,7 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
-          <c:xVal>
+          <c:cat>
             <c:numRef>
               <c:f>Sheet1!$C$13:$C$76</c:f>
               <c:numCache>
@@ -4611,205 +4616,205 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
               <c:f>Sheet1!$H$13:$H$76</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="64"/>
                 <c:pt idx="1">
-                  <c:v>41.999922515864377</c:v>
+                  <c:v>46.10606568428711</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57.731227098782462</c:v>
+                  <c:v>62.976328817339486</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>79.343691366858394</c:v>
+                  <c:v>86.007457418180763</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>109.02614442981582</c:v>
+                  <c:v>117.43898504064637</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>149.77331618671971</c:v>
+                  <c:v>160.3155990290868</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>205.67483533419212</c:v>
+                  <c:v>218.76890972813055</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>282.30103111212105</c:v>
+                  <c:v>298.39119914690639</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>387.21188493963376</c:v>
+                  <c:v>406.72543018279725</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>530.6170501434159</c:v>
+                  <c:v>553.89704856396111</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>726.21048052783112</c:v>
+                  <c:v>753.40896575592774</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>992.18610682527219</c:v>
+                  <c:v>1023.1056383870567</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1352.3996233811579</c:v>
+                  <c:v>1386.2753538684074</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1837.5580324661978</c:v>
+                  <c:v>1872.7864131290899</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2486.1700448994734</c:v>
+                  <c:v>2520.0229594649909</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3344.7565895934708</c:v>
+                  <c:v>3373.1816798974473</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4466.5092992988166</c:v>
+                  <c:v>4484.2149978913576</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5907.2840967386028</c:v>
+                  <c:v>5908.4265767581337</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7717.7709844829142</c:v>
+                  <c:v>7697.6338455377409</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9931.326523605725</c:v>
+                  <c:v>9889.2694058674006</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12548.754917422448</c:v>
+                  <c:v>12492.220815579374</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>15524.204023179205</c:v>
+                  <c:v>15472.676065443371</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>18758.912822493527</c:v>
+                  <c:v>18745.798190773781</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>22109.131605133323</c:v>
+                  <c:v>22179.511881116596</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>25409.280263859553</c:v>
+                  <c:v>25613.003311283301</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>28503.376074201584</c:v>
+                  <c:v>28885.499801841001</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>31272.760525139111</c:v>
+                  <c:v>31865.034112979854</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>33650.440124121022</c:v>
+                  <c:v>34466.907392891546</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>35619.939875773933</c:v>
+                  <c:v>36657.437226060101</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>37203.462142722397</c:v>
+                  <c:v>38445.607634627006</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>38446.438132170704</c:v>
+                  <c:v>39868.907671344241</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>39403.838407041236</c:v>
+                  <c:v>40979.176842625908</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>40130.59447455428</c:v>
+                  <c:v>41831.717218937862</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>40676.18393923968</c:v>
+                  <c:v>42478.466380149323</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>41082.3666868152</c:v>
+                  <c:v>42964.6006979534</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>41382.889689779702</c:v>
+                  <c:v>43327.483373740906</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>41604.217127119118</c:v>
+                  <c:v>43596.963671401871</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>41766.667196067698</c:v>
+                  <c:v>43796.31375948889</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>41885.605840201664</c:v>
+                  <c:v>43943.365042589248</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>41972.528685164667</c:v>
+                  <c:v>44051.610172654233</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>42035.969073187051</c:v>
+                  <c:v>44131.16669384727</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>42082.225814514873</c:v>
+                  <c:v>44189.571569987333</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>42115.929391528327</c:v>
+                  <c:v>44232.41257450165</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>42140.473787195224</c:v>
+                  <c:v>44263.817953936705</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>42158.341341320345</c:v>
+                  <c:v>44286.82989910469</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>42171.344796908517</c:v>
+                  <c:v>44303.686097730868</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>42180.80642291157</c:v>
+                  <c:v>44316.030248445408</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>42187.689929119093</c:v>
+                  <c:v>44325.068534647289</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>42192.697276896579</c:v>
+                  <c:v>44331.685438156106</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>42196.339549312252</c:v>
+                  <c:v>44336.529195712174</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>42198.988737529377</c:v>
+                  <c:v>44340.074715342962</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>42200.915532683248</c:v>
+                  <c:v>44342.669822882781</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>42202.316878856473</c:v>
+                  <c:v>44344.569215294272</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>42203.336047320852</c:v>
+                  <c:v>44345.959367120973</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>42204.077254689808</c:v>
+                  <c:v>44346.976789139866</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>42204.61630405474</c:v>
+                  <c:v>44347.721407443671</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>42205.008329047756</c:v>
+                  <c:v>44348.266363716168</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>42205.293428484641</c:v>
+                  <c:v>44348.665192245826</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>42205.500765605146</c:v>
+                  <c:v>44348.957074909384</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>42205.651549995324</c:v>
+                  <c:v>44349.170688347614</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>42205.761206576091</c:v>
+                  <c:v>44349.327020213845</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>42205.840953196101</c:v>
+                  <c:v>44349.44143060832</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>42205.898948033922</c:v>
+                  <c:v>44349.525160926722</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>42205.941124093799</c:v>
+                  <c:v>44349.586438207094</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
+          </c:val>
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -4825,10 +4830,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="687713776"/>
         <c:axId val="687716400"/>
-      </c:scatterChart>
-      <c:valAx>
+      </c:lineChart>
+      <c:catAx>
         <c:axId val="687713776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -4849,6 +4856,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -4905,7 +4926,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -4943,8 +4964,11 @@
         </c:txPr>
         <c:crossAx val="687716400"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
+      </c:catAx>
       <c:valAx>
         <c:axId val="687716400"/>
         <c:scaling>
@@ -4966,6 +4990,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -5022,7 +5060,7 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -5060,7 +5098,7 @@
         </c:txPr>
         <c:crossAx val="687713776"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -5071,7 +5109,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5126,6 +5164,11 @@
       <a:round/>
     </a:ln>
     <a:effectLst/>
+    <a:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </a:scene3d>
+    <a:sp3d/>
   </c:spPr>
   <c:txPr>
     <a:bodyPr/>
@@ -5306,12 +5349,9 @@
 </file>
 
 <file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
   <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
@@ -8337,7 +8377,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007-2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -8345,34 +8385,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -8633,8 +8673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75855736-B2B6-4FFD-943C-E355D55A5C8E}">
   <dimension ref="A2:U77"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="M43" sqref="M43"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9818,8 +9858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C57C0D72-947E-4C2B-A236-E53FEC630DCE}">
   <dimension ref="A1:T76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Z45" sqref="Z45"/>
+    <sheetView tabSelected="1" topLeftCell="U4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AU12" sqref="AU12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9880,7 +9920,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="10">
-        <v>42206.053573429082</v>
+        <v>44349.75367075036</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>4</v>
@@ -9893,11 +9933,11 @@
         <v>18</v>
       </c>
       <c r="B6" s="10">
-        <v>0.31850361840631491</v>
+        <v>0.31219526446047818</v>
       </c>
       <c r="D6" s="8">
-        <f>SUM(K14:K37)</f>
-        <v>2499738.0804764559</v>
+        <f>SUM(K14:K38)</f>
+        <v>2594705.1186947385</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -9907,7 +9947,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="11">
-        <v>21.700398849377979</v>
+        <v>21.998660950909464</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -9953,22 +9993,22 @@
       </c>
       <c r="H14" s="5">
         <f xml:space="preserve"> $B$5 / ( 1 + EXP(-$B$6 * (C14- $B$7)))</f>
-        <v>41.999922515864377</v>
+        <v>46.10606568428711</v>
       </c>
       <c r="K14" s="5">
         <f>(H14   -F14) ^2</f>
-        <v>121.0017046569875</v>
+        <v>47.526330349363754</v>
       </c>
       <c r="M14" s="1">
         <v>43889</v>
       </c>
       <c r="N14" s="5">
         <f>H16</f>
-        <v>79.343691366858394</v>
+        <v>86.007457418180763</v>
       </c>
       <c r="P14" s="5">
         <f>H18</f>
-        <v>149.77331618671971</v>
+        <v>160.3155990290868</v>
       </c>
     </row>
     <row r="15" spans="1:20">
@@ -9983,22 +10023,22 @@
       </c>
       <c r="H15" s="5">
         <f t="shared" ref="H15:H76" si="0" xml:space="preserve"> $B$5 / ( 1 + EXP(-$B$6 * (C15- $B$7)))</f>
-        <v>57.731227098782462</v>
+        <v>62.976328817339486</v>
       </c>
       <c r="K15" s="5">
-        <f t="shared" ref="K15:K37" si="1">(H15   -F15) ^2</f>
-        <v>68.372605291909508</v>
+        <f t="shared" ref="K15:K38" si="1">(H15   -F15) ^2</f>
+        <v>9.1425874208516351</v>
       </c>
       <c r="M15" s="1">
         <v>43890</v>
       </c>
       <c r="N15" s="5">
         <f t="shared" ref="N15:N36" si="2">H17</f>
-        <v>109.02614442981582</v>
+        <v>117.43898504064637</v>
       </c>
       <c r="P15" s="5">
         <f t="shared" ref="P15:P34" si="3">H19</f>
-        <v>205.67483533419212</v>
+        <v>218.76890972813055</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -10013,22 +10053,22 @@
       </c>
       <c r="H16" s="5">
         <f t="shared" si="0"/>
-        <v>79.343691366858394</v>
+        <v>86.007457418180763</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="1"/>
-        <v>1417.9975798744151</v>
+        <v>960.53769568587859</v>
       </c>
       <c r="M16" s="1">
         <v>43891</v>
       </c>
       <c r="N16" s="5">
         <f t="shared" si="2"/>
-        <v>149.77331618671971</v>
+        <v>160.3155990290868</v>
       </c>
       <c r="P16" s="5">
         <f t="shared" si="3"/>
-        <v>282.30103111212105</v>
+        <v>298.39119914690639</v>
       </c>
     </row>
     <row r="17" spans="1:16">
@@ -10043,22 +10083,22 @@
       </c>
       <c r="H17" s="5">
         <f t="shared" si="0"/>
-        <v>109.02614442981582</v>
+        <v>117.43898504064637</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" si="1"/>
-        <v>1678.8568402863136</v>
+        <v>1060.2196951832507</v>
       </c>
       <c r="M17" s="1">
         <v>43892</v>
       </c>
       <c r="N17" s="5">
         <f t="shared" si="2"/>
-        <v>205.67483533419212</v>
+        <v>218.76890972813055</v>
       </c>
       <c r="P17" s="5">
         <f t="shared" si="3"/>
-        <v>387.21188493963376</v>
+        <v>406.72543018279725</v>
       </c>
     </row>
     <row r="18" spans="1:16">
@@ -10073,22 +10113,22 @@
       </c>
       <c r="H18" s="5">
         <f t="shared" si="0"/>
-        <v>149.77331618671971</v>
+        <v>160.3155990290868</v>
       </c>
       <c r="K18" s="5">
         <f t="shared" si="1"/>
-        <v>1461.2793553605052</v>
+        <v>766.42605711829981</v>
       </c>
       <c r="M18" s="1">
         <v>43893</v>
       </c>
       <c r="N18" s="5">
         <f t="shared" si="2"/>
-        <v>282.30103111212105</v>
+        <v>298.39119914690639</v>
       </c>
       <c r="P18" s="5">
         <f t="shared" si="3"/>
-        <v>530.6170501434159</v>
+        <v>553.89704856396111</v>
       </c>
     </row>
     <row r="19" spans="1:16">
@@ -10103,22 +10143,22 @@
       </c>
       <c r="H19" s="5">
         <f t="shared" si="0"/>
-        <v>205.67483533419212</v>
+        <v>218.76890972813055</v>
       </c>
       <c r="K19" s="5">
         <f t="shared" si="1"/>
-        <v>1178.2169293348254</v>
+        <v>450.7591941322695</v>
       </c>
       <c r="M19" s="1">
         <v>43894</v>
       </c>
       <c r="N19" s="5">
         <f t="shared" si="2"/>
-        <v>387.21188493963376</v>
+        <v>406.72543018279725</v>
       </c>
       <c r="P19" s="5">
         <f t="shared" si="3"/>
-        <v>726.21048052783112</v>
+        <v>753.40896575592774</v>
       </c>
     </row>
     <row r="20" spans="1:16">
@@ -10133,22 +10173,22 @@
       </c>
       <c r="H20" s="5">
         <f t="shared" si="0"/>
-        <v>282.30103111212105</v>
+        <v>298.39119914690639</v>
       </c>
       <c r="K20" s="5">
         <f t="shared" si="1"/>
-        <v>4448.7524507062435</v>
+        <v>2561.2507237880886</v>
       </c>
       <c r="M20" s="1">
         <v>43895</v>
       </c>
       <c r="N20" s="5">
         <f t="shared" si="2"/>
-        <v>530.6170501434159</v>
+        <v>553.89704856396111</v>
       </c>
       <c r="P20" s="5">
         <f t="shared" si="3"/>
-        <v>992.18610682527219</v>
+        <v>1023.1056383870567</v>
       </c>
     </row>
     <row r="21" spans="1:16">
@@ -10163,22 +10203,22 @@
       </c>
       <c r="H21" s="5">
         <f t="shared" si="0"/>
-        <v>387.21188493963376</v>
+        <v>406.72543018279725</v>
       </c>
       <c r="K21" s="5">
         <f t="shared" si="1"/>
-        <v>21546.750722975317</v>
+        <v>16198.816122154016</v>
       </c>
       <c r="M21" s="1">
         <v>43896</v>
       </c>
       <c r="N21" s="5">
         <f t="shared" si="2"/>
-        <v>726.21048052783112</v>
+        <v>753.40896575592774</v>
       </c>
       <c r="P21" s="5">
         <f t="shared" si="3"/>
-        <v>1352.3996233811579</v>
+        <v>1386.2753538684074</v>
       </c>
     </row>
     <row r="22" spans="1:16">
@@ -10193,22 +10233,22 @@
       </c>
       <c r="H22" s="5">
         <f t="shared" si="0"/>
-        <v>530.6170501434159</v>
+        <v>553.89704856396111</v>
       </c>
       <c r="K22" s="5">
         <f t="shared" si="1"/>
-        <v>23526.329306707394</v>
+        <v>16926.777972368294</v>
       </c>
       <c r="M22" s="1">
         <v>43897</v>
       </c>
       <c r="N22" s="5">
         <f t="shared" si="2"/>
-        <v>992.18610682527219</v>
+        <v>1023.1056383870567</v>
       </c>
       <c r="P22" s="5">
         <f t="shared" si="3"/>
-        <v>1837.5580324661978</v>
+        <v>1872.7864131290899</v>
       </c>
     </row>
     <row r="23" spans="1:16">
@@ -10223,22 +10263,22 @@
       </c>
       <c r="H23" s="5">
         <f t="shared" si="0"/>
-        <v>726.21048052783112</v>
+        <v>753.40896575592774</v>
       </c>
       <c r="K23" s="5">
         <f t="shared" si="1"/>
-        <v>14590.108014317464</v>
+        <v>8759.2816908751065</v>
       </c>
       <c r="M23" s="1">
         <v>43898</v>
       </c>
       <c r="N23" s="5">
         <f t="shared" si="2"/>
-        <v>1352.3996233811579</v>
+        <v>1386.2753538684074</v>
       </c>
       <c r="P23" s="5">
         <f t="shared" si="3"/>
-        <v>2486.1700448994734</v>
+        <v>2520.0229594649909</v>
       </c>
     </row>
     <row r="24" spans="1:16">
@@ -10253,22 +10293,22 @@
       </c>
       <c r="H24" s="5">
         <f t="shared" si="0"/>
-        <v>992.18610682527219</v>
+        <v>1023.1056383870567</v>
       </c>
       <c r="K24" s="5">
         <f t="shared" si="1"/>
-        <v>14355.368997685087</v>
+        <v>7902.2075265727226</v>
       </c>
       <c r="M24" s="1">
         <v>43899</v>
       </c>
       <c r="N24" s="5">
         <f t="shared" si="2"/>
-        <v>1837.5580324661978</v>
+        <v>1872.7864131290899</v>
       </c>
       <c r="P24" s="5">
         <f t="shared" si="3"/>
-        <v>3344.7565895934708</v>
+        <v>3373.1816798974473</v>
       </c>
     </row>
     <row r="25" spans="1:16">
@@ -10283,22 +10323,22 @@
       </c>
       <c r="H25" s="5">
         <f t="shared" si="0"/>
-        <v>1352.3996233811579</v>
+        <v>1386.2753538684074</v>
       </c>
       <c r="K25" s="5">
         <f t="shared" si="1"/>
-        <v>45198.920138473513</v>
+        <v>31942.49913486301</v>
       </c>
       <c r="M25" s="1">
         <v>43900</v>
       </c>
       <c r="N25" s="5">
         <f t="shared" si="2"/>
-        <v>2486.1700448994734</v>
+        <v>2520.0229594649909</v>
       </c>
       <c r="P25" s="5">
         <f t="shared" si="3"/>
-        <v>4466.5092992988166</v>
+        <v>4484.2149978913576</v>
       </c>
     </row>
     <row r="26" spans="1:16">
@@ -10313,22 +10353,22 @@
       </c>
       <c r="H26" s="5">
         <f t="shared" si="0"/>
-        <v>1837.5580324661978</v>
+        <v>1872.7864131290899</v>
       </c>
       <c r="K26" s="5">
         <f t="shared" si="1"/>
-        <v>16497.339023954297</v>
+        <v>8688.7727773407132</v>
       </c>
       <c r="M26" s="1">
         <v>43901</v>
       </c>
       <c r="N26" s="5">
         <f t="shared" si="2"/>
-        <v>3344.7565895934708</v>
+        <v>3373.1816798974473</v>
       </c>
       <c r="P26" s="5">
         <f t="shared" si="3"/>
-        <v>5907.2840967386028</v>
+        <v>5908.4265767581337</v>
       </c>
     </row>
     <row r="27" spans="1:16">
@@ -10343,22 +10383,22 @@
       </c>
       <c r="H27" s="5">
         <f t="shared" si="0"/>
-        <v>2486.1700448994734</v>
+        <v>2520.0229594649909</v>
       </c>
       <c r="K27" s="5">
         <f t="shared" si="1"/>
-        <v>66992.945657340621</v>
+        <v>50614.668767891133</v>
       </c>
       <c r="M27" s="1">
         <v>43902</v>
       </c>
       <c r="N27" s="5">
         <f t="shared" si="2"/>
-        <v>4466.5092992988166</v>
+        <v>4484.2149978913576</v>
       </c>
       <c r="P27" s="5">
         <f t="shared" si="3"/>
-        <v>7717.7709844829142</v>
+        <v>7697.6338455377409</v>
       </c>
     </row>
     <row r="28" spans="1:16">
@@ -10373,22 +10413,22 @@
       </c>
       <c r="H28" s="5">
         <f t="shared" si="0"/>
-        <v>3344.7565895934708</v>
+        <v>3373.1816798974473</v>
       </c>
       <c r="K28" s="5">
         <f t="shared" si="1"/>
-        <v>109060.71011693525</v>
+        <v>91094.298349526944</v>
       </c>
       <c r="M28" s="1">
         <v>43903</v>
       </c>
       <c r="N28" s="5">
         <f t="shared" si="2"/>
-        <v>5907.2840967386028</v>
+        <v>5908.4265767581337</v>
       </c>
       <c r="P28" s="5">
         <f t="shared" si="3"/>
-        <v>9931.326523605725</v>
+        <v>9889.2694058674006</v>
       </c>
     </row>
     <row r="29" spans="1:16">
@@ -10403,22 +10443,22 @@
       </c>
       <c r="H29" s="5">
         <f t="shared" si="0"/>
-        <v>4466.5092992988166</v>
+        <v>4484.2149978913576</v>
       </c>
       <c r="K29" s="5">
         <f t="shared" si="1"/>
-        <v>14040.046152657427</v>
+        <v>10157.616650039054</v>
       </c>
       <c r="M29" s="1">
         <v>43904</v>
       </c>
       <c r="N29" s="5">
         <f t="shared" si="2"/>
-        <v>7717.7709844829142</v>
+        <v>7697.6338455377409</v>
       </c>
       <c r="P29" s="5">
         <f t="shared" si="3"/>
-        <v>12548.754917422448</v>
+        <v>12492.220815579374</v>
       </c>
     </row>
     <row r="30" spans="1:16">
@@ -10433,22 +10473,22 @@
       </c>
       <c r="H30" s="5">
         <f t="shared" si="0"/>
-        <v>5907.2840967386028</v>
+        <v>5908.4265767581337</v>
       </c>
       <c r="K30" s="5">
         <f t="shared" si="1"/>
-        <v>8889.4908978142084</v>
+        <v>9106.2315517759835</v>
       </c>
       <c r="M30" s="1">
         <v>43905</v>
       </c>
       <c r="N30" s="5">
         <f t="shared" si="2"/>
-        <v>9931.326523605725</v>
+        <v>9889.2694058674006</v>
       </c>
       <c r="P30" s="5">
         <f t="shared" si="3"/>
-        <v>15524.204023179205</v>
+        <v>15472.676065443371</v>
       </c>
     </row>
     <row r="31" spans="1:16">
@@ -10463,22 +10503,22 @@
       </c>
       <c r="H31" s="5">
         <f t="shared" si="0"/>
-        <v>7717.7709844829142</v>
+        <v>7697.6338455377409</v>
       </c>
       <c r="K31" s="5">
         <f t="shared" si="1"/>
-        <v>198711.77060686651</v>
+        <v>181164.17046724545</v>
       </c>
       <c r="M31" s="1">
         <v>43906</v>
       </c>
       <c r="N31" s="5">
         <f t="shared" si="2"/>
-        <v>12548.754917422448</v>
+        <v>12492.220815579374</v>
       </c>
       <c r="P31" s="5">
         <f t="shared" si="3"/>
-        <v>18758.912822493527</v>
+        <v>18745.798190773781</v>
       </c>
     </row>
     <row r="32" spans="1:16">
@@ -10493,22 +10533,22 @@
       </c>
       <c r="H32" s="5">
         <f t="shared" si="0"/>
-        <v>9931.326523605725</v>
+        <v>9889.2694058674006</v>
       </c>
       <c r="K32" s="5">
         <f t="shared" si="1"/>
-        <v>326413.99657540309</v>
+        <v>280126.10398723121</v>
       </c>
       <c r="M32" s="1">
         <v>43907</v>
       </c>
       <c r="N32" s="5">
         <f t="shared" si="2"/>
-        <v>15524.204023179205</v>
+        <v>15472.676065443371</v>
       </c>
       <c r="P32" s="5">
         <f t="shared" si="3"/>
-        <v>22109.131605133323</v>
+        <v>22179.511881116596</v>
       </c>
     </row>
     <row r="33" spans="1:16">
@@ -10523,20 +10563,20 @@
       </c>
       <c r="H33" s="5">
         <f t="shared" si="0"/>
-        <v>12548.754917422448</v>
+        <v>12492.220815579374</v>
       </c>
       <c r="K33" s="5">
         <f t="shared" si="1"/>
-        <v>49175.243401036627</v>
+        <v>27297.917900713572</v>
       </c>
       <c r="N33" s="5">
         <f t="shared" si="2"/>
-        <v>18758.912822493527</v>
+        <v>18745.798190773781</v>
       </c>
       <c r="O33" s="1"/>
       <c r="P33" s="5">
         <f t="shared" si="3"/>
-        <v>25409.280263859553</v>
+        <v>25613.003311283301</v>
       </c>
     </row>
     <row r="34" spans="1:16">
@@ -10551,20 +10591,20 @@
       </c>
       <c r="H34" s="5">
         <f t="shared" si="0"/>
-        <v>15524.204023179205</v>
+        <v>15472.676065443371</v>
       </c>
       <c r="K34" s="5">
         <f t="shared" si="1"/>
-        <v>41699.283082573398</v>
+        <v>23309.98095926852</v>
       </c>
       <c r="N34" s="5">
         <f t="shared" si="2"/>
-        <v>22109.131605133323</v>
+        <v>22179.511881116596</v>
       </c>
       <c r="O34" s="1"/>
       <c r="P34" s="5">
         <f t="shared" si="3"/>
-        <v>28503.376074201584</v>
+        <v>28885.499801841001</v>
       </c>
     </row>
     <row r="35" spans="1:16">
@@ -10579,15 +10619,15 @@
       </c>
       <c r="H35" s="5">
         <f t="shared" si="0"/>
-        <v>18758.912822493527</v>
+        <v>18745.798190773781</v>
       </c>
       <c r="K35" s="5">
         <f t="shared" si="1"/>
-        <v>1186110.8802090166</v>
+        <v>1214848.8282615498</v>
       </c>
       <c r="N35" s="5">
         <f t="shared" si="2"/>
-        <v>25409.280263859553</v>
+        <v>25613.003311283301</v>
       </c>
       <c r="O35" s="1"/>
       <c r="P35" s="5"/>
@@ -10604,15 +10644,15 @@
       </c>
       <c r="H36" s="5">
         <f t="shared" si="0"/>
-        <v>22109.131605133323</v>
+        <v>22179.511881116596</v>
       </c>
       <c r="K36" s="5">
         <f t="shared" si="1"/>
-        <v>64957.898701916223</v>
+        <v>34035.866009137098</v>
       </c>
       <c r="N36" s="5">
         <f t="shared" si="2"/>
-        <v>28503.376074201584</v>
+        <v>28885.499801841001</v>
       </c>
       <c r="O36" s="1"/>
       <c r="P36" s="5"/>
@@ -10629,11 +10669,11 @@
       </c>
       <c r="H37" s="5">
         <f t="shared" si="0"/>
-        <v>25409.280263859553</v>
+        <v>25613.003311283301</v>
       </c>
       <c r="K37" s="5">
         <f t="shared" si="1"/>
-        <v>287596.52140527189</v>
+        <v>547604.90071024967</v>
       </c>
       <c r="N37" s="5"/>
       <c r="O37" s="1"/>
@@ -10645,9 +10685,16 @@
       <c r="C38">
         <v>24</v>
       </c>
+      <c r="F38">
+        <v>29056</v>
+      </c>
       <c r="H38" s="5">
         <f t="shared" si="0"/>
-        <v>28503.376074201584</v>
+        <v>28885.499801841001</v>
+      </c>
+      <c r="K38" s="5">
+        <f t="shared" si="1"/>
+        <v>29070.317572258067</v>
       </c>
       <c r="N38" s="5"/>
       <c r="O38" s="1"/>
@@ -10658,7 +10705,7 @@
       </c>
       <c r="H39" s="5">
         <f t="shared" si="0"/>
-        <v>31272.760525139111</v>
+        <v>31865.034112979854</v>
       </c>
     </row>
     <row r="40" spans="1:16">
@@ -10667,7 +10714,7 @@
       </c>
       <c r="H40" s="5">
         <f t="shared" si="0"/>
-        <v>33650.440124121022</v>
+        <v>34466.907392891546</v>
       </c>
     </row>
     <row r="41" spans="1:16">
@@ -10677,7 +10724,7 @@
       </c>
       <c r="H41" s="5">
         <f t="shared" si="0"/>
-        <v>35619.939875773933</v>
+        <v>36657.437226060101</v>
       </c>
     </row>
     <row r="42" spans="1:16">
@@ -10686,7 +10733,7 @@
       </c>
       <c r="H42" s="5">
         <f t="shared" si="0"/>
-        <v>37203.462142722397</v>
+        <v>38445.607634627006</v>
       </c>
     </row>
     <row r="43" spans="1:16">
@@ -10695,7 +10742,7 @@
       </c>
       <c r="H43" s="5">
         <f t="shared" si="0"/>
-        <v>38446.438132170704</v>
+        <v>39868.907671344241</v>
       </c>
     </row>
     <row r="44" spans="1:16">
@@ -10704,7 +10751,7 @@
       </c>
       <c r="H44" s="5">
         <f t="shared" si="0"/>
-        <v>39403.838407041236</v>
+        <v>40979.176842625908</v>
       </c>
     </row>
     <row r="45" spans="1:16">
@@ -10713,7 +10760,7 @@
       </c>
       <c r="H45" s="5">
         <f t="shared" si="0"/>
-        <v>40130.59447455428</v>
+        <v>41831.717218937862</v>
       </c>
     </row>
     <row r="46" spans="1:16">
@@ -10722,7 +10769,7 @@
       </c>
       <c r="H46" s="5">
         <f t="shared" si="0"/>
-        <v>40676.18393923968</v>
+        <v>42478.466380149323</v>
       </c>
     </row>
     <row r="47" spans="1:16">
@@ -10731,7 +10778,7 @@
       </c>
       <c r="H47" s="5">
         <f t="shared" si="0"/>
-        <v>41082.3666868152</v>
+        <v>42964.6006979534</v>
       </c>
     </row>
     <row r="48" spans="1:16">
@@ -10740,7 +10787,7 @@
       </c>
       <c r="H48" s="5">
         <f t="shared" si="0"/>
-        <v>41382.889689779702</v>
+        <v>43327.483373740906</v>
       </c>
     </row>
     <row r="49" spans="3:8">
@@ -10749,7 +10796,7 @@
       </c>
       <c r="H49" s="5">
         <f t="shared" si="0"/>
-        <v>41604.217127119118</v>
+        <v>43596.963671401871</v>
       </c>
     </row>
     <row r="50" spans="3:8">
@@ -10758,7 +10805,7 @@
       </c>
       <c r="H50" s="5">
         <f t="shared" si="0"/>
-        <v>41766.667196067698</v>
+        <v>43796.31375948889</v>
       </c>
     </row>
     <row r="51" spans="3:8">
@@ -10767,7 +10814,7 @@
       </c>
       <c r="H51" s="5">
         <f t="shared" si="0"/>
-        <v>41885.605840201664</v>
+        <v>43943.365042589248</v>
       </c>
     </row>
     <row r="52" spans="3:8">
@@ -10776,7 +10823,7 @@
       </c>
       <c r="H52" s="5">
         <f t="shared" si="0"/>
-        <v>41972.528685164667</v>
+        <v>44051.610172654233</v>
       </c>
     </row>
     <row r="53" spans="3:8">
@@ -10785,7 +10832,7 @@
       </c>
       <c r="H53" s="5">
         <f t="shared" si="0"/>
-        <v>42035.969073187051</v>
+        <v>44131.16669384727</v>
       </c>
     </row>
     <row r="54" spans="3:8">
@@ -10794,7 +10841,7 @@
       </c>
       <c r="H54" s="5">
         <f t="shared" si="0"/>
-        <v>42082.225814514873</v>
+        <v>44189.571569987333</v>
       </c>
     </row>
     <row r="55" spans="3:8">
@@ -10803,7 +10850,7 @@
       </c>
       <c r="H55" s="5">
         <f t="shared" si="0"/>
-        <v>42115.929391528327</v>
+        <v>44232.41257450165</v>
       </c>
     </row>
     <row r="56" spans="3:8">
@@ -10812,7 +10859,7 @@
       </c>
       <c r="H56" s="5">
         <f t="shared" si="0"/>
-        <v>42140.473787195224</v>
+        <v>44263.817953936705</v>
       </c>
     </row>
     <row r="57" spans="3:8">
@@ -10821,7 +10868,7 @@
       </c>
       <c r="H57" s="5">
         <f t="shared" si="0"/>
-        <v>42158.341341320345</v>
+        <v>44286.82989910469</v>
       </c>
     </row>
     <row r="58" spans="3:8">
@@ -10830,7 +10877,7 @@
       </c>
       <c r="H58" s="5">
         <f t="shared" si="0"/>
-        <v>42171.344796908517</v>
+        <v>44303.686097730868</v>
       </c>
     </row>
     <row r="59" spans="3:8">
@@ -10839,7 +10886,7 @@
       </c>
       <c r="H59" s="5">
         <f t="shared" si="0"/>
-        <v>42180.80642291157</v>
+        <v>44316.030248445408</v>
       </c>
     </row>
     <row r="60" spans="3:8">
@@ -10848,7 +10895,7 @@
       </c>
       <c r="H60" s="5">
         <f t="shared" si="0"/>
-        <v>42187.689929119093</v>
+        <v>44325.068534647289</v>
       </c>
     </row>
     <row r="61" spans="3:8">
@@ -10857,7 +10904,7 @@
       </c>
       <c r="H61" s="5">
         <f t="shared" si="0"/>
-        <v>42192.697276896579</v>
+        <v>44331.685438156106</v>
       </c>
     </row>
     <row r="62" spans="3:8">
@@ -10866,7 +10913,7 @@
       </c>
       <c r="H62" s="5">
         <f t="shared" si="0"/>
-        <v>42196.339549312252</v>
+        <v>44336.529195712174</v>
       </c>
     </row>
     <row r="63" spans="3:8">
@@ -10875,7 +10922,7 @@
       </c>
       <c r="H63" s="5">
         <f t="shared" si="0"/>
-        <v>42198.988737529377</v>
+        <v>44340.074715342962</v>
       </c>
     </row>
     <row r="64" spans="3:8">
@@ -10884,7 +10931,7 @@
       </c>
       <c r="H64" s="5">
         <f t="shared" si="0"/>
-        <v>42200.915532683248</v>
+        <v>44342.669822882781</v>
       </c>
     </row>
     <row r="65" spans="3:8">
@@ -10893,7 +10940,7 @@
       </c>
       <c r="H65" s="5">
         <f t="shared" si="0"/>
-        <v>42202.316878856473</v>
+        <v>44344.569215294272</v>
       </c>
     </row>
     <row r="66" spans="3:8">
@@ -10902,7 +10949,7 @@
       </c>
       <c r="H66" s="5">
         <f t="shared" si="0"/>
-        <v>42203.336047320852</v>
+        <v>44345.959367120973</v>
       </c>
     </row>
     <row r="67" spans="3:8">
@@ -10911,7 +10958,7 @@
       </c>
       <c r="H67" s="5">
         <f t="shared" si="0"/>
-        <v>42204.077254689808</v>
+        <v>44346.976789139866</v>
       </c>
     </row>
     <row r="68" spans="3:8">
@@ -10920,7 +10967,7 @@
       </c>
       <c r="H68" s="5">
         <f t="shared" si="0"/>
-        <v>42204.61630405474</v>
+        <v>44347.721407443671</v>
       </c>
     </row>
     <row r="69" spans="3:8">
@@ -10929,7 +10976,7 @@
       </c>
       <c r="H69" s="5">
         <f t="shared" si="0"/>
-        <v>42205.008329047756</v>
+        <v>44348.266363716168</v>
       </c>
     </row>
     <row r="70" spans="3:8">
@@ -10938,7 +10985,7 @@
       </c>
       <c r="H70" s="5">
         <f t="shared" si="0"/>
-        <v>42205.293428484641</v>
+        <v>44348.665192245826</v>
       </c>
     </row>
     <row r="71" spans="3:8">
@@ -10947,7 +10994,7 @@
       </c>
       <c r="H71" s="5">
         <f t="shared" si="0"/>
-        <v>42205.500765605146</v>
+        <v>44348.957074909384</v>
       </c>
     </row>
     <row r="72" spans="3:8">
@@ -10956,7 +11003,7 @@
       </c>
       <c r="H72" s="5">
         <f t="shared" si="0"/>
-        <v>42205.651549995324</v>
+        <v>44349.170688347614</v>
       </c>
     </row>
     <row r="73" spans="3:8">
@@ -10965,7 +11012,7 @@
       </c>
       <c r="H73" s="5">
         <f t="shared" si="0"/>
-        <v>42205.761206576091</v>
+        <v>44349.327020213845</v>
       </c>
     </row>
     <row r="74" spans="3:8">
@@ -10974,7 +11021,7 @@
       </c>
       <c r="H74" s="5">
         <f t="shared" si="0"/>
-        <v>42205.840953196101</v>
+        <v>44349.44143060832</v>
       </c>
     </row>
     <row r="75" spans="3:8">
@@ -10983,7 +11030,7 @@
       </c>
       <c r="H75" s="5">
         <f t="shared" si="0"/>
-        <v>42205.898948033922</v>
+        <v>44349.525160926722</v>
       </c>
     </row>
     <row r="76" spans="3:8">
@@ -10992,7 +11039,7 @@
       </c>
       <c r="H76" s="5">
         <f t="shared" si="0"/>
-        <v>42205.941124093799</v>
+        <v>44349.586438207094</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update model new data
</commit_message>
<xml_diff>
--- a/Covid19_Germany_Estimates/Corona_Deutschland_Modellierung_08-03-2020.xlsx
+++ b/Covid19_Germany_Estimates/Corona_Deutschland_Modellierung_08-03-2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benni\Desktop\Covid19_Germany_Estimates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB6AF76-194C-421E-B727-025057A04342}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C50656-3F71-4498-A475-E728F49EDC3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{8F2FD530-AE1D-479B-B999-25EE25C3C974}"/>
   </bookViews>
@@ -23,14 +23,14 @@
     <definedName name="solver_adj" localSheetId="1" hidden="1">'Logistic Model Germany'!$B$5:$B$7</definedName>
     <definedName name="solver_adj" localSheetId="3" hidden="1">'Logistic Model USA'!$B$5:$B$7</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'Polynomial-Exponential Germany'!$B$6:$B$9</definedName>
-    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.00001</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_drv" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">1</definedName>
@@ -206,10 +206,10 @@
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_ssz" localSheetId="2" hidden="1">1000</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
-    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">1000</definedName>
     <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="3" hidden="1">2147483647</definedName>
@@ -526,22 +526,32 @@
           </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Polynomial-Exponential Germany'!$C$14:$C$38</c:f>
+              <c:f>'Polynomial-Exponential Germany'!$C$14:$C$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
@@ -613,16 +623,31 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Polynomial-Exponential Germany'!$F$14:$F$38</c:f>
+              <c:f>'Polynomial-Exponential Germany'!$F$14:$F$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="1">
                   <c:v>53</c:v>
                 </c:pt>
@@ -694,6 +719,21 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>24873</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>29056</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>32911</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>37323</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43211</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>49039</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -733,10 +773,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Polynomial-Exponential Germany'!$C$14:$C$38</c:f>
+              <c:f>'Polynomial-Exponential Germany'!$C$14:$C$43</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="1">
                   <c:v>0</c:v>
                 </c:pt>
@@ -808,87 +848,117 @@
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>28</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Polynomial-Exponential Germany'!$H$14:$H$38</c:f>
+              <c:f>'Polynomial-Exponential Germany'!$H$14:$H$43</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="25"/>
+                <c:ptCount val="30"/>
                 <c:pt idx="1">
-                  <c:v>57.037922156925774</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>79.257489368455737</c:v>
+                  <c:v>0.3090453081973949</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>109.44293233023083</c:v>
+                  <c:v>3.7472086845621413</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150.21324882880424</c:v>
+                  <c:v>16.129592361958583</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>204.97388525803987</c:v>
+                  <c:v>45.435321466486194</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>278.13140503169456</c:v>
+                  <c:v>101.45243755891812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>375.36112160986215</c:v>
+                  <c:v>195.57309874632756</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>503.93942924996497</c:v>
+                  <c:v>340.65330701635042</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>673.15487953239381</c:v>
+                  <c:v>550.90831884217869</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>894.81476942681286</c:v>
+                  <c:v>841.83044641719528</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1183.8671881976884</c:v>
+                  <c:v>1230.1220727413745</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1559.1621847672798</c:v>
+                  <c:v>1733.6395943038647</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2044.3800420277912</c:v>
+                  <c:v>2371.3455427088279</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2669.1596675257688</c:v>
+                  <c:v>3163.2670262247125</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3470.4659291981052</c:v>
+                  <c:v>4130.4591806362259</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4494.2414905606947</c:v>
+                  <c:v>5294.9726740624255</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5797.3964551606559</c:v>
+                  <c:v>6679.8245500118637</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7450.1980528096983</c:v>
+                  <c:v>8308.9718599936223</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9539.1328435281466</c:v>
+                  <c:v>10207.287656761551</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12170.325649982035</c:v>
+                  <c:v>12400.539007196463</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>15473.612845197047</c:v>
+                  <c:v>14915.366749731853</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>19607.382929936077</c:v>
+                  <c:v>17779.266771515988</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>24764.314766447147</c:v>
+                  <c:v>21020.572619490737</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>31178.163650145754</c:v>
+                  <c:v>24668.439290221933</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>28752.828067723298</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>33304.492298171521</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>38354.964006401337</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>43936.541272201241</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>50082.276295304589</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1528,6 +1598,9 @@
                 <c:pt idx="24">
                   <c:v>24873</c:v>
                 </c:pt>
+                <c:pt idx="25">
+                  <c:v>29056</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -1654,79 +1727,79 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>57.037922156925774</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>79.257489368455737</c:v>
+                  <c:v>0.3090453081973949</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>109.44293233023083</c:v>
+                  <c:v>3.7472086845621413</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150.21324882880424</c:v>
+                  <c:v>16.129592361958583</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>204.97388525803987</c:v>
+                  <c:v>45.435321466486194</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>278.13140503169456</c:v>
+                  <c:v>101.45243755891812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>375.36112160986215</c:v>
+                  <c:v>195.57309874632756</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>503.93942924996497</c:v>
+                  <c:v>340.65330701635042</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>673.15487953239381</c:v>
+                  <c:v>550.90831884217869</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>894.81476942681286</c:v>
+                  <c:v>841.83044641719528</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1183.8671881976884</c:v>
+                  <c:v>1230.1220727413745</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1559.1621847672798</c:v>
+                  <c:v>1733.6395943038647</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2044.3800420277912</c:v>
+                  <c:v>2371.3455427088279</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2669.1596675257688</c:v>
+                  <c:v>3163.2670262247125</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3470.4659291981052</c:v>
+                  <c:v>4130.4591806362259</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4494.2414905606947</c:v>
+                  <c:v>5294.9726740624255</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5797.3964551606559</c:v>
+                  <c:v>6679.8245500118637</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7450.1980528096983</c:v>
+                  <c:v>8308.9718599936223</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9539.1328435281466</c:v>
+                  <c:v>10207.287656761551</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12170.325649982035</c:v>
+                  <c:v>12400.539007196463</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>15473.612845197047</c:v>
+                  <c:v>14915.366749731853</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>19607.382929936077</c:v>
+                  <c:v>17779.266771515988</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>24764.314766447147</c:v>
+                  <c:v>21020.572619490737</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>31178.163650145754</c:v>
+                  <c:v>24668.439290221933</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>39131.767882935746</c:v>
+                  <c:v>28752.828067723298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1856,73 +1929,73 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>109.44293233023083</c:v>
+                  <c:v>3.7472086845621413</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>150.21324882880424</c:v>
+                  <c:v>16.129592361958583</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>204.97388525803987</c:v>
+                  <c:v>45.435321466486194</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>278.13140503169456</c:v>
+                  <c:v>101.45243755891812</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>375.36112160986215</c:v>
+                  <c:v>195.57309874632756</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>503.93942924996497</c:v>
+                  <c:v>340.65330701635042</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>673.15487953239381</c:v>
+                  <c:v>550.90831884217869</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>894.81476942681286</c:v>
+                  <c:v>841.83044641719528</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1183.8671881976884</c:v>
+                  <c:v>1230.1220727413745</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1559.1621847672798</c:v>
+                  <c:v>1733.6395943038647</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2044.3800420277912</c:v>
+                  <c:v>2371.3455427088279</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2669.1596675257688</c:v>
+                  <c:v>3163.2670262247125</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3470.4659291981052</c:v>
+                  <c:v>4130.4591806362259</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4494.2414905606947</c:v>
+                  <c:v>5294.9726740624255</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5797.3964551606559</c:v>
+                  <c:v>6679.8245500118637</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7450.1980528096983</c:v>
+                  <c:v>8308.9718599936223</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9539.1328435281466</c:v>
+                  <c:v>10207.287656761551</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>12170.325649982035</c:v>
+                  <c:v>12400.539007196463</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>15473.612845197047</c:v>
+                  <c:v>14915.366749731853</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>19607.382929936077</c:v>
+                  <c:v>17779.266771515988</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>24764.314766447147</c:v>
+                  <c:v>21020.572619490737</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>31178.163650145754</c:v>
+                  <c:v>24668.439290221933</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>39131.767882935746</c:v>
+                  <c:v>28752.828067723298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2033,61 +2106,61 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>204.97388525803987</c:v>
+                  <c:v>45.435321466486194</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>278.13140503169456</c:v>
+                  <c:v>101.45243755891812</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>375.36112160986215</c:v>
+                  <c:v>195.57309874632756</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>503.93942924996497</c:v>
+                  <c:v>340.65330701635042</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>673.15487953239381</c:v>
+                  <c:v>550.90831884217869</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>894.81476942681286</c:v>
+                  <c:v>841.83044641719528</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1183.8671881976884</c:v>
+                  <c:v>1230.1220727413745</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1559.1621847672798</c:v>
+                  <c:v>1733.6395943038647</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2044.3800420277912</c:v>
+                  <c:v>2371.3455427088279</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2669.1596675257688</c:v>
+                  <c:v>3163.2670262247125</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3470.4659291981052</c:v>
+                  <c:v>4130.4591806362259</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4494.2414905606947</c:v>
+                  <c:v>5294.9726740624255</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5797.3964551606559</c:v>
+                  <c:v>6679.8245500118637</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7450.1980528096983</c:v>
+                  <c:v>8308.9718599936223</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>9539.1328435281466</c:v>
+                  <c:v>10207.287656761551</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>12170.325649982035</c:v>
+                  <c:v>12400.539007196463</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>15473.612845197047</c:v>
+                  <c:v>14915.366749731853</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>19607.382929936077</c:v>
+                  <c:v>17779.266771515988</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>24764.314766447147</c:v>
+                  <c:v>21020.572619490737</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2766,6 +2839,9 @@
                 <c:pt idx="24">
                   <c:v>24873</c:v>
                 </c:pt>
+                <c:pt idx="25">
+                  <c:v>29056</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -2930,79 +3006,79 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>57.037922156925774</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>79.257489368455737</c:v>
+                  <c:v>0.3090453081973949</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>109.44293233023083</c:v>
+                  <c:v>3.7472086845621413</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>150.21324882880424</c:v>
+                  <c:v>16.129592361958583</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>204.97388525803987</c:v>
+                  <c:v>45.435321466486194</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>278.13140503169456</c:v>
+                  <c:v>101.45243755891812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>375.36112160986215</c:v>
+                  <c:v>195.57309874632756</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>503.93942924996497</c:v>
+                  <c:v>340.65330701635042</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>673.15487953239381</c:v>
+                  <c:v>550.90831884217869</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>894.81476942681286</c:v>
+                  <c:v>841.83044641719528</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1183.8671881976884</c:v>
+                  <c:v>1230.1220727413745</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1559.1621847672798</c:v>
+                  <c:v>1733.6395943038647</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2044.3800420277912</c:v>
+                  <c:v>2371.3455427088279</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2669.1596675257688</c:v>
+                  <c:v>3163.2670262247125</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3470.4659291981052</c:v>
+                  <c:v>4130.4591806362259</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4494.2414905606947</c:v>
+                  <c:v>5294.9726740624255</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5797.3964551606559</c:v>
+                  <c:v>6679.8245500118637</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7450.1980528096983</c:v>
+                  <c:v>8308.9718599936223</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9539.1328435281466</c:v>
+                  <c:v>10207.287656761551</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12170.325649982035</c:v>
+                  <c:v>12400.539007196463</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>15473.612845197047</c:v>
+                  <c:v>14915.366749731853</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>19607.382929936077</c:v>
+                  <c:v>17779.266771515988</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>24764.314766447147</c:v>
+                  <c:v>21020.572619490737</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>31178.163650145754</c:v>
+                  <c:v>24668.439290221933</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>39131.767882935746</c:v>
+                  <c:v>28752.828067723298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3170,73 +3246,73 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="1">
-                  <c:v>109.44293233023083</c:v>
+                  <c:v>3.7472086845621413</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>150.21324882880424</c:v>
+                  <c:v>16.129592361958583</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>204.97388525803987</c:v>
+                  <c:v>45.435321466486194</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>278.13140503169456</c:v>
+                  <c:v>101.45243755891812</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>375.36112160986215</c:v>
+                  <c:v>195.57309874632756</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>503.93942924996497</c:v>
+                  <c:v>340.65330701635042</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>673.15487953239381</c:v>
+                  <c:v>550.90831884217869</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>894.81476942681286</c:v>
+                  <c:v>841.83044641719528</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1183.8671881976884</c:v>
+                  <c:v>1230.1220727413745</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1559.1621847672798</c:v>
+                  <c:v>1733.6395943038647</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2044.3800420277912</c:v>
+                  <c:v>2371.3455427088279</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2669.1596675257688</c:v>
+                  <c:v>3163.2670262247125</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3470.4659291981052</c:v>
+                  <c:v>4130.4591806362259</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4494.2414905606947</c:v>
+                  <c:v>5294.9726740624255</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5797.3964551606559</c:v>
+                  <c:v>6679.8245500118637</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7450.1980528096983</c:v>
+                  <c:v>8308.9718599936223</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>9539.1328435281466</c:v>
+                  <c:v>10207.287656761551</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>12170.325649982035</c:v>
+                  <c:v>12400.539007196463</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>15473.612845197047</c:v>
+                  <c:v>14915.366749731853</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>19607.382929936077</c:v>
+                  <c:v>17779.266771515988</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>24764.314766447147</c:v>
+                  <c:v>21020.572619490737</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>31178.163650145754</c:v>
+                  <c:v>24668.439290221933</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>39131.767882935746</c:v>
+                  <c:v>28752.828067723298</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3734,61 +3810,61 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="19"/>
                 <c:pt idx="0">
-                  <c:v>109.44293233023083</c:v>
+                  <c:v>3.7472086845621413</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>150.21324882880424</c:v>
+                  <c:v>16.129592361958583</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>204.97388525803987</c:v>
+                  <c:v>45.435321466486194</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>278.13140503169456</c:v>
+                  <c:v>101.45243755891812</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>375.36112160986215</c:v>
+                  <c:v>195.57309874632756</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>503.93942924996497</c:v>
+                  <c:v>340.65330701635042</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>673.15487953239381</c:v>
+                  <c:v>550.90831884217869</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>894.81476942681286</c:v>
+                  <c:v>841.83044641719528</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1183.8671881976884</c:v>
+                  <c:v>1230.1220727413745</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1559.1621847672798</c:v>
+                  <c:v>1733.6395943038647</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2044.3800420277912</c:v>
+                  <c:v>2371.3455427088279</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2669.1596675257688</c:v>
+                  <c:v>3163.2670262247125</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3470.4659291981052</c:v>
+                  <c:v>4130.4591806362259</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4494.2414905606947</c:v>
+                  <c:v>5294.9726740624255</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5797.3964551606559</c:v>
+                  <c:v>6679.8245500118637</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7450.1980528096983</c:v>
+                  <c:v>8308.9718599936223</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9539.1328435281466</c:v>
+                  <c:v>10207.287656761551</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>12170.325649982035</c:v>
+                  <c:v>12400.539007196463</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>15473.612845197047</c:v>
+                  <c:v>14915.366749731853</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4505,6 +4581,15 @@
                 <c:pt idx="27">
                   <c:v>37323</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>43211</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>49039</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>54268</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -4746,193 +4831,193 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="64"/>
                 <c:pt idx="1">
-                  <c:v>68.303618998809156</c:v>
+                  <c:v>158.24860932963421</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>90.965492878143237</c:v>
+                  <c:v>200.13208872517259</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>121.12896113698618</c:v>
+                  <c:v>253.06745485112174</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>161.26394088790207</c:v>
+                  <c:v>319.95102992103489</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>214.643335590269</c:v>
+                  <c:v>404.42624006866242</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>285.59621048808287</c:v>
+                  <c:v>511.06921850834965</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>379.83472587751538</c:v>
+                  <c:v>645.61626803348372</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>504.87160346495972</c:v>
+                  <c:v>815.24004624698159</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>670.54489150100426</c:v>
+                  <c:v>1028.880801304208</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>889.66299086053834</c:v>
+                  <c:v>1297.637080419235</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1178.7717886166843</c:v>
+                  <c:v>1635.2161357509153</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1559.0217023610269</c:v>
+                  <c:v>2058.4364229617486</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2057.0672487014303</c:v>
+                  <c:v>2587.7612928824856</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2705.8549183906634</c:v>
+                  <c:v>3247.8219120093945</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3545.0366160270642</c:v>
+                  <c:v>4067.856113565148</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4620.5839948215489</c:v>
+                  <c:v>5081.9463686354266</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5982.9970232969827</c:v>
+                  <c:v>6328.8847288327743</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7683.3732794728712</c:v>
+                  <c:v>7851.4309989848898</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9766.6871293489621</c:v>
+                  <c:v>9694.6776870519116</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12262.146107635637</c:v>
+                  <c:v>11903.220958402673</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>15171.635184648756</c:v>
+                  <c:v>14516.906905723705</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>18458.923488631015</c:v>
+                  <c:v>17565.132547694819</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>22043.788622023767</c:v>
+                  <c:v>21060.07189364206</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>25805.240837329446</c:v>
+                  <c:v>24989.74913216709</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>29595.572735160196</c:v>
+                  <c:v>29312.45865400559</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>33262.529379811182</c:v>
+                  <c:v>33954.367087480714</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>36672.933615439004</c:v>
+                  <c:v>38811.903157882982</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>39730.346724714836</c:v>
+                  <c:v>43759.566989078616</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>42382.354097126859</c:v>
+                  <c:v>48662.254887716961</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>44617.678298200379</c:v>
+                  <c:v>53389.687938094576</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>46456.691744204021</c:v>
+                  <c:v>57829.774423223273</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>47939.738269915484</c:v>
+                  <c:v>61898.124441750391</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>49116.57371381329</c:v>
+                  <c:v>65542.264209436646</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>50038.520212990705</c:v>
+                  <c:v>68740.704811288</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>50753.551881858009</c:v>
+                  <c:v>71498.226204060993</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>51303.790993575371</c:v>
+                  <c:v>73839.211764449356</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>51724.676509154349</c:v>
+                  <c:v>75800.689564375207</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>52045.138013739277</c:v>
+                  <c:v>77426.20497618636</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>52288.28205892507</c:v>
+                  <c:v>78761.066754865271</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>52472.272188098643</c:v>
+                  <c:v>79849.056716641455</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>52611.219355907269</c:v>
+                  <c:v>80730.424780020927</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>52715.990909288703</c:v>
+                  <c:v>81440.88006793255</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>52794.902025058655</c:v>
+                  <c:v>82011.280544749272</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>52854.284348607027</c:v>
+                  <c:v>82467.767564984897</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>52898.941741262737</c:v>
+                  <c:v>82832.152624154201</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>52932.509073506204</c:v>
+                  <c:v>83122.422044591469</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>52957.731124179081</c:v>
+                  <c:v>83353.273049438518</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>52976.677398026754</c:v>
+                  <c:v>83536.629969071699</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>52990.906482876708</c:v>
+                  <c:v>83682.113576150892</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>53001.591183074503</c:v>
+                  <c:v>83797.452181829562</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>53009.613444485462</c:v>
+                  <c:v>83888.832566129247</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>53015.636169841826</c:v>
+                  <c:v>83961.194063558956</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>53020.157441637435</c:v>
+                  <c:v>84018.471681137642</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>53023.551400945558</c:v>
+                  <c:v>84063.79504180506</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>53026.099031664846</c:v>
+                  <c:v>84099.649923075151</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>53028.011323563725</c:v>
+                  <c:v>84128.008646616392</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>53029.44668998674</c:v>
+                  <c:v>84150.434843402894</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>53030.524059151925</c:v>
+                  <c:v>84168.167330967262</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>53031.332710225921</c:v>
+                  <c:v>84182.187081227676</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>53031.939661658762</c:v>
+                  <c:v>84193.270571902263</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>53032.395219810824</c:v>
+                  <c:v>84202.032217901244</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>53032.737145344749</c:v>
+                  <c:v>84208.95807280502</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>53032.993781367346</c:v>
+                  <c:v>84214.432568462347</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5324,69 +5409,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="de-DE"/>
-              <a:t>Logistic Model With Linear amount of unknown Cases:</a:t>
-            </a:r>
-            <a:br>
-              <a:rPr lang="de-DE"/>
-            </a:br>
-            <a:r>
-              <a:rPr lang="de-DE"/>
-              <a:t>Germany </a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="de-DE"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -5713,6 +5736,18 @@
                 <c:pt idx="27">
                   <c:v>37323</c:v>
                 </c:pt>
+                <c:pt idx="28">
+                  <c:v>43211</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>49039</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>54268</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>58655</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -5954,193 +5989,193 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="64"/>
                 <c:pt idx="1">
-                  <c:v>90.636145428703131</c:v>
+                  <c:v>387.69645273786119</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>91.46305745816548</c:v>
+                  <c:v>258.83945124451031</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>101.25939558249988</c:v>
+                  <c:v>155.46549942241768</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>122.82441084526189</c:v>
+                  <c:v>82.390736393145971</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>159.81760974569073</c:v>
+                  <c:v>45.306532597530804</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>217.01344071940468</c:v>
+                  <c:v>50.92378364832166</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>300.62435699916819</c:v>
+                  <c:v>107.13470032347141</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>418.70545253443061</c:v>
+                  <c:v>223.1913854301547</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>581.65239796990647</c:v>
+                  <c:v>409.89887219632919</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>802.79895140868052</c:v>
+                  <c:v>679.81791829133772</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1099.1077581784596</c:v>
+                  <c:v>1047.4694745254906</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1491.9237867461243</c:v>
+                  <c:v>1529.5281302091885</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2007.7171615497291</c:v>
+                  <c:v>2144.9857503027552</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2678.673935021362</c:v>
+                  <c:v>2915.2588250648469</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3542.8938465611386</c:v>
+                  <c:v>3864.2038205801846</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4643.8261897918283</c:v>
+                  <c:v>5017.9945035789497</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>6028.4425458745591</c:v>
+                  <c:v>6404.8049003961269</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7743.571667643082</c:v>
+                  <c:v>8054.2332394736932</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>9829.9249028294944</c:v>
+                  <c:v>9996.399107451507</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>12313.779276328774</c:v>
+                  <c:v>12260.652602763241</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>15197.178474842767</c:v>
+                  <c:v>14873.855987455525</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>18448.764081966692</c:v>
+                  <c:v>17858.24072527419</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>21998.459416840924</c:v>
+                  <c:v>21228.909403484842</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>25739.318032988282</c:v>
+                  <c:v>24991.141478772719</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>29538.172447073117</c:v>
+                  <c:v>29137.764309066162</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>33253.503902870929</c:v>
+                  <c:v>33646.946006973303</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>36755.76240241812</c:v>
+                  <c:v>38480.823871020941</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>39944.196954618186</c:v>
+                  <c:v>43585.367640592689</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>42755.909075778647</c:v>
+                  <c:v>48891.765556695129</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>45166.196227668479</c:v>
+                  <c:v>54319.411986313346</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>47182.266972676043</c:v>
+                  <c:v>59780.301153723172</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>48833.741449435525</c:v>
+                  <c:v>65184.357015681235</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>50163.004469400832</c:v>
+                  <c:v>70445.032156266403</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>51217.28456904435</c:v>
+                  <c:v>75484.450004784594</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>52043.122105219263</c:v>
+                  <c:v>80237.463618263952</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>52683.081391422958</c:v>
+                  <c:v>84654.228941423469</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>53174.196266760577</c:v>
+                  <c:v>88701.172362658952</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>53547.578842317911</c:v>
+                  <c:v>92360.494677754701</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>53828.712488193967</c:v>
+                  <c:v>95628.538731991939</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>54038.084983609333</c:v>
+                  <c:v>98513.432469016174</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>54191.941437103924</c:v>
+                  <c:v>101032.41169433438</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>54303.030200850721</c:v>
+                  <c:v>103209.15635991676</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>54381.278008387439</c:v>
+                  <c:v>105071.37453459842</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>54434.369280969018</c:v>
+                  <c:v>106648.76761506648</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>54468.22632919297</c:v>
+                  <c:v>107971.42635255762</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>54487.398139486926</c:v>
+                  <c:v>109068.64716371786</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>54495.369967410159</c:v>
+                  <c:v>109968.12171665633</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>54494.806940187475</c:v>
+                  <c:v>110695.43561665383</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>54487.744067601125</c:v>
+                  <c:v>111273.80850978619</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>54475.733498122783</c:v>
+                  <c:v>111724.0127909053</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>54459.958094101334</c:v>
+                  <c:v>112064.41719683455</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>54441.318715596499</c:v>
+                  <c:v>112311.11203089969</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>54420.501118300323</c:v>
+                  <c:v>112478.08286949387</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>54398.02712276802</c:v>
+                  <c:v>112577.40845354805</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>54374.293693003725</c:v>
+                  <c:v>112619.46573477048</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>54349.602746662436</c:v>
+                  <c:v>112613.13072786326</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>54324.183875110321</c:v>
+                  <c:v>112565.96808629629</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>54298.211648158132</c:v>
+                  <c:v>112484.40540879617</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>54271.818787558106</c:v>
+                  <c:v>112373.89044197858</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>54245.106191691564</c:v>
+                  <c:v>112239.03079358321</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>54218.15056187669</c:v>
+                  <c:v>112083.71669683857</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>54191.010202821337</c:v>
+                  <c:v>111911.22791812012</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>54163.729433618711</c:v>
+                  <c:v>111724.3261913434</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11979,16 +12014,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75855736-B2B6-4FFD-943C-E355D55A5C8E}">
   <dimension ref="A2:U77"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H39" sqref="H39"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
     <col min="8" max="8" width="16.7109375" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5703125" customWidth="1"/>
     <col min="13" max="13" width="13.140625" customWidth="1"/>
     <col min="14" max="14" width="20.5703125" customWidth="1"/>
     <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
@@ -12049,7 +12084,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="8">
-        <v>0.99931200671311204</v>
+        <v>2.2853237971739246</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>4</v>
@@ -12062,11 +12097,11 @@
         <v>7</v>
       </c>
       <c r="B7" s="7">
-        <v>40</v>
+        <v>3.984014573818091</v>
       </c>
       <c r="D7" s="8">
-        <f>SUM(K15:K34)</f>
-        <v>161792.65009602223</v>
+        <f>SUM(K15:K41)</f>
+        <v>11400929.854819035</v>
       </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -12076,7 +12111,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="7">
-        <v>1.2704805293787489</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
@@ -12084,7 +12119,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="7">
-        <v>0.42235648449558316</v>
+        <v>0.90359259233470302</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
@@ -12128,22 +12163,22 @@
       </c>
       <c r="H15" s="5">
         <f xml:space="preserve"> $B$6* ((($B$6/$B$7)*C15+$B$8)^$B$7)^$B$9</f>
-        <v>57.037922156925774</v>
+        <v>0</v>
       </c>
       <c r="K15" s="5">
         <f>(H15   -F15) ^2</f>
-        <v>16.304815345392093</v>
+        <v>2809</v>
       </c>
       <c r="M15" s="1">
         <v>43889</v>
       </c>
       <c r="N15" s="5">
         <f>H17</f>
-        <v>109.44293233023083</v>
+        <v>3.7472086845621413</v>
       </c>
       <c r="P15" s="5">
         <f>H19</f>
-        <v>204.97388525803987</v>
+        <v>45.435321466486194</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
@@ -12158,22 +12193,22 @@
       </c>
       <c r="H16" s="5">
         <f t="shared" ref="H16:H77" si="0" xml:space="preserve"> $B$6* ((($B$6/$B$7)*C16+$B$8)^$B$7)^$B$9</f>
-        <v>79.257489368455737</v>
+        <v>0.3090453081973949</v>
       </c>
       <c r="K16" s="5">
-        <f t="shared" ref="K16:K34" si="1">(H16   -F16) ^2</f>
-        <v>175.76102435471688</v>
+        <f t="shared" ref="K16:K41" si="1">(H16   -F16) ^2</f>
+        <v>4315.3015283204622</v>
       </c>
       <c r="M16" s="1">
         <v>43890</v>
       </c>
       <c r="N16" s="5">
         <f t="shared" ref="N16:N37" si="2">H18</f>
-        <v>150.21324882880424</v>
+        <v>16.129592361958583</v>
       </c>
       <c r="P16" s="5">
         <f t="shared" ref="P16:P35" si="3">H20</f>
-        <v>278.13140503169456</v>
+        <v>101.45243755891812</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -12188,22 +12223,22 @@
       </c>
       <c r="H17" s="5">
         <f t="shared" si="0"/>
-        <v>109.44293233023083</v>
+        <v>3.7472086845621413</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" si="1"/>
-        <v>57.109271765470403</v>
+        <v>12826.194740738118</v>
       </c>
       <c r="M17" s="1">
         <v>43891</v>
       </c>
       <c r="N17" s="5">
         <f t="shared" si="2"/>
-        <v>204.97388525803987</v>
+        <v>45.435321466486194</v>
       </c>
       <c r="P17" s="5">
         <f t="shared" si="3"/>
-        <v>375.36112160986215</v>
+        <v>195.57309874632756</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -12218,22 +12253,22 @@
       </c>
       <c r="H18" s="5">
         <f t="shared" si="0"/>
-        <v>150.21324882880424</v>
+        <v>16.129592361958583</v>
       </c>
       <c r="K18" s="5">
         <f t="shared" si="1"/>
-        <v>4.5475062986379877E-2</v>
+        <v>17921.286041175379</v>
       </c>
       <c r="M18" s="1">
         <v>43892</v>
       </c>
       <c r="N18" s="5">
         <f t="shared" si="2"/>
-        <v>278.13140503169456</v>
+        <v>101.45243755891812</v>
       </c>
       <c r="P18" s="5">
         <f t="shared" si="3"/>
-        <v>503.93942924996497</v>
+        <v>340.65330701635042</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -12248,22 +12283,22 @@
       </c>
       <c r="H19" s="5">
         <f t="shared" si="0"/>
-        <v>204.97388525803987</v>
+        <v>45.435321466486194</v>
       </c>
       <c r="K19" s="5">
         <f t="shared" si="1"/>
-        <v>288.11278075310327</v>
+        <v>20324.687565364133</v>
       </c>
       <c r="M19" s="1">
         <v>43893</v>
       </c>
       <c r="N19" s="5">
         <f t="shared" si="2"/>
-        <v>375.36112160986215</v>
+        <v>195.57309874632756</v>
       </c>
       <c r="P19" s="5">
         <f t="shared" si="3"/>
-        <v>673.15487953239381</v>
+        <v>550.90831884217869</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -12278,22 +12313,22 @@
       </c>
       <c r="H20" s="5">
         <f t="shared" si="0"/>
-        <v>278.13140503169456</v>
+        <v>101.45243755891812</v>
       </c>
       <c r="K20" s="5">
         <f t="shared" si="1"/>
-        <v>1454.0040496911408</v>
+        <v>19195.427058365483</v>
       </c>
       <c r="M20" s="1">
         <v>43894</v>
       </c>
       <c r="N20" s="5">
         <f t="shared" si="2"/>
-        <v>503.93942924996497</v>
+        <v>340.65330701635042</v>
       </c>
       <c r="P20" s="5">
         <f t="shared" si="3"/>
-        <v>894.81476942681286</v>
+        <v>841.83044641719528</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -12308,22 +12343,22 @@
       </c>
       <c r="H21" s="5">
         <f t="shared" si="0"/>
-        <v>375.36112160986215</v>
+        <v>195.57309874632756</v>
       </c>
       <c r="K21" s="5">
         <f t="shared" si="1"/>
-        <v>694.9087325299414</v>
+        <v>23539.814028304154</v>
       </c>
       <c r="M21" s="1">
         <v>43895</v>
       </c>
       <c r="N21" s="5">
         <f t="shared" si="2"/>
-        <v>673.15487953239381</v>
+        <v>550.90831884217869</v>
       </c>
       <c r="P21" s="5">
         <f t="shared" si="3"/>
-        <v>1183.8671881976884</v>
+        <v>1230.1220727413745</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -12338,22 +12373,22 @@
       </c>
       <c r="H22" s="5">
         <f t="shared" si="0"/>
-        <v>503.93942924996497</v>
+        <v>340.65330701635042</v>
       </c>
       <c r="K22" s="5">
         <f t="shared" si="1"/>
-        <v>903.63791381786143</v>
+        <v>37382.943687713647</v>
       </c>
       <c r="M22" s="1">
         <v>43896</v>
       </c>
       <c r="N22" s="5">
         <f t="shared" si="2"/>
-        <v>894.81476942681286</v>
+        <v>841.83044641719528</v>
       </c>
       <c r="P22" s="5">
         <f t="shared" si="3"/>
-        <v>1559.1621847672798</v>
+        <v>1733.6395943038647</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -12368,22 +12403,22 @@
       </c>
       <c r="H23" s="5">
         <f t="shared" si="0"/>
-        <v>673.15487953239381</v>
+        <v>550.90831884217869</v>
       </c>
       <c r="K23" s="5">
         <f t="shared" si="1"/>
-        <v>117.61663795689078</v>
+        <v>17713.395593415167</v>
       </c>
       <c r="M23" s="1">
         <v>43897</v>
       </c>
       <c r="N23" s="5">
         <f t="shared" si="2"/>
-        <v>1183.8671881976884</v>
+        <v>1230.1220727413745</v>
       </c>
       <c r="P23" s="5">
         <f t="shared" si="3"/>
-        <v>2044.3800420277912</v>
+        <v>2371.3455427088279</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -12398,22 +12433,22 @@
       </c>
       <c r="H24" s="5">
         <f t="shared" si="0"/>
-        <v>894.81476942681286</v>
+        <v>841.83044641719528</v>
       </c>
       <c r="K24" s="5">
         <f t="shared" si="1"/>
-        <v>2286.2521753392775</v>
+        <v>26.724284245489159</v>
       </c>
       <c r="M24" s="1">
         <v>43898</v>
       </c>
       <c r="N24" s="5">
         <f t="shared" si="2"/>
-        <v>1559.1621847672798</v>
+        <v>1733.6395943038647</v>
       </c>
       <c r="P24" s="5">
         <f t="shared" si="3"/>
-        <v>2669.1596675257688</v>
+        <v>3163.2670262247125</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -12428,22 +12463,22 @@
       </c>
       <c r="H25" s="5">
         <f t="shared" si="0"/>
-        <v>1183.8671881976884</v>
+        <v>1230.1220727413745</v>
       </c>
       <c r="K25" s="5">
         <f t="shared" si="1"/>
-        <v>5164.8927394419616</v>
+        <v>13952.824068718568</v>
       </c>
       <c r="M25" s="1">
         <v>43899</v>
       </c>
       <c r="N25" s="5">
         <f t="shared" si="2"/>
-        <v>2044.3800420277912</v>
+        <v>2371.3455427088279</v>
       </c>
       <c r="P25" s="5">
         <f t="shared" si="3"/>
-        <v>3470.4659291981052</v>
+        <v>4130.4591806362259</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -12458,22 +12493,22 @@
       </c>
       <c r="H26" s="5">
         <f t="shared" si="0"/>
-        <v>1559.1621847672798</v>
+        <v>1733.6395943038647</v>
       </c>
       <c r="K26" s="5">
         <f t="shared" si="1"/>
-        <v>34.080086691380373</v>
+        <v>28439.312766972063</v>
       </c>
       <c r="M26" s="1">
         <v>43900</v>
       </c>
       <c r="N26" s="5">
         <f t="shared" si="2"/>
-        <v>2669.1596675257688</v>
+        <v>3163.2670262247125</v>
       </c>
       <c r="P26" s="5">
         <f t="shared" si="3"/>
-        <v>4494.2414905606947</v>
+        <v>5294.9726740624255</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -12488,22 +12523,22 @@
       </c>
       <c r="H27" s="5">
         <f t="shared" si="0"/>
-        <v>2044.3800420277912</v>
+        <v>2371.3455427088279</v>
       </c>
       <c r="K27" s="5">
         <f t="shared" si="1"/>
-        <v>6143.4309882783155</v>
+        <v>164305.00899391423</v>
       </c>
       <c r="M27" s="1">
         <v>43901</v>
       </c>
       <c r="N27" s="5">
         <f t="shared" si="2"/>
-        <v>3470.4659291981052</v>
+        <v>4130.4591806362259</v>
       </c>
       <c r="P27" s="5">
         <f t="shared" si="3"/>
-        <v>5797.3964551606559</v>
+        <v>6679.8245500118637</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -12518,22 +12553,22 @@
       </c>
       <c r="H28" s="5">
         <f t="shared" si="0"/>
-        <v>2669.1596675257688</v>
+        <v>3163.2670262247125</v>
       </c>
       <c r="K28" s="5">
         <f t="shared" si="1"/>
-        <v>5751.7560298019298</v>
+        <v>174947.30522686432</v>
       </c>
       <c r="M28" s="1">
         <v>43902</v>
       </c>
       <c r="N28" s="5">
         <f t="shared" si="2"/>
-        <v>4494.2414905606947</v>
+        <v>5294.9726740624255</v>
       </c>
       <c r="P28" s="5">
         <f t="shared" si="3"/>
-        <v>7450.1980528096983</v>
+        <v>8308.9718599936223</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -12548,22 +12583,22 @@
       </c>
       <c r="H29" s="5">
         <f t="shared" si="0"/>
-        <v>3470.4659291981052</v>
+        <v>4130.4591806362259</v>
       </c>
       <c r="K29" s="5">
         <f t="shared" si="1"/>
-        <v>41834.186118794518</v>
+        <v>207443.0652258223</v>
       </c>
       <c r="M29" s="1">
         <v>43903</v>
       </c>
       <c r="N29" s="5">
         <f t="shared" si="2"/>
-        <v>5797.3964551606559</v>
+        <v>6679.8245500118637</v>
       </c>
       <c r="P29" s="5">
         <f t="shared" si="3"/>
-        <v>9539.1328435281466</v>
+        <v>10207.287656761551</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -12578,22 +12613,22 @@
       </c>
       <c r="H30" s="5">
         <f t="shared" si="0"/>
-        <v>4494.2414905606947</v>
+        <v>5294.9726740624255</v>
       </c>
       <c r="K30" s="5">
         <f t="shared" si="1"/>
-        <v>8237.1070356444634</v>
+        <v>504061.19791535113</v>
       </c>
       <c r="M30" s="1">
         <v>43904</v>
       </c>
       <c r="N30" s="5">
         <f t="shared" si="2"/>
-        <v>7450.1980528096983</v>
+        <v>8308.9718599936223</v>
       </c>
       <c r="P30" s="5">
         <f t="shared" si="3"/>
-        <v>12170.325649982035</v>
+        <v>12400.539007196463</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -12608,22 +12643,22 @@
       </c>
       <c r="H31" s="5">
         <f t="shared" si="0"/>
-        <v>5797.3964551606559</v>
+        <v>6679.8245500118637</v>
       </c>
       <c r="K31" s="5">
         <f t="shared" si="1"/>
-        <v>243.47061155342087</v>
+        <v>751384.80050327</v>
       </c>
       <c r="M31" s="1">
         <v>43905</v>
       </c>
       <c r="N31" s="5">
         <f t="shared" si="2"/>
-        <v>9539.1328435281466</v>
+        <v>10207.287656761551</v>
       </c>
       <c r="P31" s="5">
         <f t="shared" si="3"/>
-        <v>15473.612845197047</v>
+        <v>14915.366749731853</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -12638,22 +12673,22 @@
       </c>
       <c r="H32" s="5">
         <f t="shared" si="0"/>
-        <v>7450.1980528096983</v>
+        <v>8308.9718599936223</v>
       </c>
       <c r="K32" s="5">
         <f t="shared" si="1"/>
-        <v>31754.546025168027</v>
+        <v>1075310.6384186326</v>
       </c>
       <c r="M32" s="1">
         <v>43906</v>
       </c>
       <c r="N32" s="5">
         <f t="shared" si="2"/>
-        <v>12170.325649982035</v>
+        <v>12400.539007196463</v>
       </c>
       <c r="P32" s="5">
         <f t="shared" si="3"/>
-        <v>19607.382929936077</v>
+        <v>17779.266771515988</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -12668,22 +12703,22 @@
       </c>
       <c r="H33" s="5">
         <f t="shared" si="0"/>
-        <v>9539.1328435281466</v>
+        <v>10207.287656761551</v>
       </c>
       <c r="K33" s="5">
         <f t="shared" si="1"/>
-        <v>32088.575630479463</v>
+        <v>717896.37330048031</v>
       </c>
       <c r="M33" s="1">
         <v>43907</v>
       </c>
       <c r="N33" s="5">
         <f t="shared" si="2"/>
-        <v>15473.612845197047</v>
+        <v>14915.366749731853</v>
       </c>
       <c r="P33" s="5">
         <f t="shared" si="3"/>
-        <v>24764.314766447147</v>
+        <v>21020.572619490737</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -12698,20 +12733,20 @@
       </c>
       <c r="H34" s="5">
         <f t="shared" si="0"/>
-        <v>12170.325649982035</v>
+        <v>12400.539007196463</v>
       </c>
       <c r="K34" s="5">
         <f t="shared" si="1"/>
-        <v>24546.851953551959</v>
+        <v>5407.9855794414352</v>
       </c>
       <c r="N34" s="5">
         <f t="shared" si="2"/>
-        <v>19607.382929936077</v>
+        <v>17779.266771515988</v>
       </c>
       <c r="O34" s="1"/>
       <c r="P34" s="5">
         <f t="shared" si="3"/>
-        <v>31178.163650145754</v>
+        <v>24668.439290221933</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -12726,16 +12761,20 @@
       </c>
       <c r="H35" s="5">
         <f t="shared" si="0"/>
-        <v>15473.612845197047</v>
+        <v>14915.366749731853</v>
+      </c>
+      <c r="K35" s="5">
+        <f t="shared" si="1"/>
+        <v>163728.06722256495</v>
       </c>
       <c r="N35" s="5">
         <f t="shared" si="2"/>
-        <v>24764.314766447147</v>
+        <v>21020.572619490737</v>
       </c>
       <c r="O35" s="1"/>
       <c r="P35" s="5">
         <f t="shared" si="3"/>
-        <v>39131.767882935746</v>
+        <v>28752.828067723298</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -12750,11 +12789,15 @@
       </c>
       <c r="H36" s="5">
         <f t="shared" si="0"/>
-        <v>19607.382929936077</v>
+        <v>17779.266771515988</v>
+      </c>
+      <c r="K36" s="5">
+        <f t="shared" si="1"/>
+        <v>4279657.1706338841</v>
       </c>
       <c r="N36" s="5">
         <f t="shared" si="2"/>
-        <v>31178.163650145754</v>
+        <v>24668.439290221933</v>
       </c>
       <c r="O36" s="1"/>
       <c r="P36" s="5"/>
@@ -12771,11 +12814,15 @@
       </c>
       <c r="H37" s="5">
         <f t="shared" si="0"/>
-        <v>24764.314766447147</v>
+        <v>21020.572619490737</v>
+      </c>
+      <c r="K37" s="5">
+        <f t="shared" si="1"/>
+        <v>1804797.1267019813</v>
       </c>
       <c r="N37" s="5">
         <f t="shared" si="2"/>
-        <v>39131.767882935746</v>
+        <v>28752.828067723298</v>
       </c>
       <c r="O37" s="1"/>
       <c r="P37" s="5"/>
@@ -12792,7 +12839,11 @@
       </c>
       <c r="H38" s="5">
         <f t="shared" si="0"/>
-        <v>31178.163650145754</v>
+        <v>24668.439290221933</v>
+      </c>
+      <c r="K38" s="5">
+        <f t="shared" si="1"/>
+        <v>41845.083984906421</v>
       </c>
       <c r="N38" s="5"/>
       <c r="O38" s="1"/>
@@ -12804,9 +12855,16 @@
       <c r="C39">
         <v>24</v>
       </c>
+      <c r="F39">
+        <v>29056</v>
+      </c>
       <c r="H39" s="5">
         <f t="shared" si="0"/>
-        <v>39131.767882935746</v>
+        <v>28752.828067723298</v>
+      </c>
+      <c r="K39" s="5">
+        <f t="shared" si="1"/>
+        <v>91913.220520389266</v>
       </c>
       <c r="N39" s="5"/>
       <c r="O39" s="1"/>
@@ -12815,18 +12873,32 @@
       <c r="C40">
         <v>25</v>
       </c>
+      <c r="F40">
+        <v>32911</v>
+      </c>
       <c r="H40" s="5">
         <f t="shared" si="0"/>
-        <v>48966.473975321882</v>
+        <v>33304.492298171521</v>
+      </c>
+      <c r="K40" s="5">
+        <f t="shared" si="1"/>
+        <v>154836.18872030504</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C41">
         <v>26</v>
       </c>
+      <c r="F41">
+        <v>37323</v>
+      </c>
       <c r="H41" s="5">
         <f t="shared" si="0"/>
-        <v>61093.20739507574</v>
+        <v>38354.964006401337</v>
+      </c>
+      <c r="K41" s="5">
+        <f t="shared" si="1"/>
+        <v>1064949.7105078977</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
@@ -12834,27 +12906,48 @@
       <c r="C42">
         <v>27</v>
       </c>
+      <c r="F42">
+        <v>43211</v>
+      </c>
       <c r="H42" s="5">
         <f t="shared" si="0"/>
-        <v>76005.448278385113</v>
+        <v>43936.541272201241</v>
+      </c>
+      <c r="K42" s="5">
+        <f>(H42   -F42) ^2</f>
+        <v>526410.13766739483</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C43">
         <v>28</v>
       </c>
+      <c r="F43">
+        <v>49039</v>
+      </c>
       <c r="H43" s="5">
         <f t="shared" si="0"/>
-        <v>94294.408142978107</v>
+        <v>50082.276295304589</v>
+      </c>
+      <c r="K43" s="5">
+        <f t="shared" ref="K43:K44" si="4">(H43   -F43) ^2</f>
+        <v>1088425.4283444688</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C44">
         <v>29</v>
       </c>
+      <c r="F44">
+        <v>55000</v>
+      </c>
       <c r="H44" s="5">
         <f t="shared" si="0"/>
-        <v>116666.74485008695</v>
+        <v>56825.964087052496</v>
+      </c>
+      <c r="K44" s="5">
+        <f t="shared" si="4"/>
+        <v>3334144.8472054563</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -12863,7 +12956,7 @@
       </c>
       <c r="H45" s="5">
         <f t="shared" si="0"/>
-        <v>143965.19935557296</v>
+        <v>64202.131734330709</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -12872,7 +12965,7 @@
       </c>
       <c r="H46" s="5">
         <f t="shared" si="0"/>
-        <v>177192.58971977295</v>
+        <v>72246.028187845179</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -12881,7 +12974,7 @@
       </c>
       <c r="H47" s="5">
         <f t="shared" si="0"/>
-        <v>217539.65601160142</v>
+        <v>80993.614532300635</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -12890,7 +12983,7 @@
       </c>
       <c r="H48" s="5">
         <f t="shared" si="0"/>
-        <v>266417.31480116944</v>
+        <v>90481.554700749606</v>
       </c>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
@@ -12899,7 +12992,7 @@
       </c>
       <c r="H49" s="5">
         <f t="shared" si="0"/>
-        <v>325493.95460248081</v>
+        <v>100747.20659944008</v>
       </c>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
@@ -12908,7 +13001,7 @@
       </c>
       <c r="H50" s="5">
         <f t="shared" si="0"/>
-        <v>396738.48468307685</v>
+        <v>111828.61361299436</v>
       </c>
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.25">
@@ -12917,7 +13010,7 @@
       </c>
       <c r="H51" s="5">
         <f t="shared" si="0"/>
-        <v>482469.93994970381</v>
+        <v>123764.49646279821</v>
       </c>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.25">
@@ -12926,7 +13019,7 @@
       </c>
       <c r="H52" s="5">
         <f t="shared" si="0"/>
-        <v>585414.545070605</v>
+        <v>136594.24539414418</v>
       </c>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.25">
@@ -12935,7 +13028,7 @@
       </c>
       <c r="H53" s="5">
         <f t="shared" si="0"/>
-        <v>708771.25260806025</v>
+        <v>150357.91267000351</v>
       </c>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.25">
@@ -12944,7 +13037,7 @@
       </c>
       <c r="H54" s="5">
         <f t="shared" si="0"/>
-        <v>856286.89379689924</v>
+        <v>165096.20535135397</v>
       </c>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.25">
@@ -12953,7 +13046,7 @@
       </c>
       <c r="H55" s="5">
         <f t="shared" si="0"/>
-        <v>1032342.2178945248</v>
+        <v>180850.47834580194</v>
       </c>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.25">
@@ -12962,7 +13055,7 @@
       </c>
       <c r="H56" s="5">
         <f t="shared" si="0"/>
-        <v>1242050.2480223014</v>
+        <v>197662.72770784819</v>
       </c>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.25">
@@ -12971,7 +13064,7 @@
       </c>
       <c r="H57" s="5">
         <f t="shared" si="0"/>
-        <v>1491368.5494987571</v>
+        <v>215575.58417556804</v>
       </c>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.25">
@@ -12980,7 +13073,7 @@
       </c>
       <c r="H58" s="5">
         <f t="shared" si="0"/>
-        <v>1787227.1923250416</v>
+        <v>234632.30692975302</v>
       </c>
     </row>
     <row r="59" spans="3:8" x14ac:dyDescent="0.25">
@@ -12989,7 +13082,7 @@
       </c>
       <c r="H59" s="5">
         <f t="shared" si="0"/>
-        <v>2137674.3943362511</v>
+        <v>254876.77756270414</v>
       </c>
     </row>
     <row r="60" spans="3:8" x14ac:dyDescent="0.25">
@@ -12998,7 +13091,7 @@
       </c>
       <c r="H60" s="5">
         <f t="shared" si="0"/>
-        <v>2552042.057319208</v>
+        <v>276353.49424488243</v>
       </c>
     </row>
     <row r="61" spans="3:8" x14ac:dyDescent="0.25">
@@ -13007,7 +13100,7 @@
       </c>
       <c r="H61" s="5">
         <f t="shared" si="0"/>
-        <v>3041133.6569963968</v>
+        <v>299107.56607853493</v>
       </c>
     </row>
     <row r="62" spans="3:8" x14ac:dyDescent="0.25">
@@ -13016,7 +13109,7 @@
       </c>
       <c r="H62" s="5">
         <f t="shared" si="0"/>
-        <v>3617437.2212088089</v>
+        <v>323184.70762826584</v>
       </c>
     </row>
     <row r="63" spans="3:8" x14ac:dyDescent="0.25">
@@ -13025,7 +13118,7 @@
       </c>
       <c r="H63" s="5">
         <f t="shared" si="0"/>
-        <v>4295366.431076603</v>
+        <v>348631.23361923586</v>
       </c>
     </row>
     <row r="64" spans="3:8" x14ac:dyDescent="0.25">
@@ -13034,7 +13127,7 @@
       </c>
       <c r="H64" s="5">
         <f t="shared" si="0"/>
-        <v>5091533.2097179024</v>
+        <v>375494.05379438831</v>
       </c>
     </row>
     <row r="65" spans="3:8" x14ac:dyDescent="0.25">
@@ -13043,7 +13136,7 @@
       </c>
       <c r="H65" s="5">
         <f t="shared" si="0"/>
-        <v>6025055.5247815559</v>
+        <v>403820.66792267567</v>
       </c>
     </row>
     <row r="66" spans="3:8" x14ac:dyDescent="0.25">
@@ -13052,7 +13145,7 @@
       </c>
       <c r="H66" s="5">
         <f t="shared" si="0"/>
-        <v>7117904.5273040263</v>
+        <v>433659.16095086007</v>
       </c>
     </row>
     <row r="67" spans="3:8" x14ac:dyDescent="0.25">
@@ -13061,7 +13154,7 @@
       </c>
       <c r="H67" s="5">
         <f t="shared" si="0"/>
-        <v>8395295.5831390843</v>
+        <v>465058.19829193276</v>
       </c>
     </row>
     <row r="68" spans="3:8" x14ac:dyDescent="0.25">
@@ -13070,7 +13163,7 @@
       </c>
       <c r="H68" s="5">
         <f t="shared" si="0"/>
-        <v>9886128.2275427822</v>
+        <v>498067.0212437014</v>
       </c>
     </row>
     <row r="69" spans="3:8" x14ac:dyDescent="0.25">
@@ -13079,7 +13172,7 @@
       </c>
       <c r="H69" s="5">
         <f t="shared" si="0"/>
-        <v>11623480.591766953</v>
+        <v>532735.44253147522</v>
       </c>
     </row>
     <row r="70" spans="3:8" x14ac:dyDescent="0.25">
@@ -13088,7 +13181,7 @@
       </c>
       <c r="H70" s="5">
         <f t="shared" si="0"/>
-        <v>13645164.416295074</v>
+        <v>569113.84196921927</v>
       </c>
     </row>
     <row r="71" spans="3:8" x14ac:dyDescent="0.25">
@@ -13097,7 +13190,7 @@
       </c>
       <c r="H71" s="5">
         <f t="shared" si="0"/>
-        <v>15994347.382473061</v>
+        <v>607253.16223386093</v>
       </c>
     </row>
     <row r="72" spans="3:8" x14ac:dyDescent="0.25">
@@ -13106,7 +13199,7 @@
       </c>
       <c r="H72" s="5">
         <f t="shared" si="0"/>
-        <v>18720250.166835226</v>
+        <v>647204.90474778763</v>
       </c>
     </row>
     <row r="73" spans="3:8" x14ac:dyDescent="0.25">
@@ -13115,7 +13208,7 @@
       </c>
       <c r="H73" s="5">
         <f t="shared" si="0"/>
-        <v>21878926.354783121</v>
+        <v>689021.12566488283</v>
       </c>
     </row>
     <row r="74" spans="3:8" x14ac:dyDescent="0.25">
@@ -13124,7 +13217,7 @@
       </c>
       <c r="H74" s="5">
         <f t="shared" si="0"/>
-        <v>25534134.14710949</v>
+        <v>732754.43195569201</v>
       </c>
     </row>
     <row r="75" spans="3:8" x14ac:dyDescent="0.25">
@@ -13133,7 +13226,7 @@
       </c>
       <c r="H75" s="5">
         <f t="shared" si="0"/>
-        <v>29758309.659166168</v>
+        <v>778457.97758761898</v>
       </c>
     </row>
     <row r="76" spans="3:8" x14ac:dyDescent="0.25">
@@ -13142,7 +13235,7 @@
       </c>
       <c r="H76" s="5">
         <f t="shared" si="0"/>
-        <v>34633652.553580321</v>
+        <v>826185.45979624882</v>
       </c>
     </row>
     <row r="77" spans="3:8" x14ac:dyDescent="0.25">
@@ -13151,7 +13244,7 @@
       </c>
       <c r="H77" s="5">
         <f t="shared" si="0"/>
-        <v>40253335.768994063</v>
+        <v>875991.11544414156</v>
       </c>
     </row>
   </sheetData>
@@ -13164,13 +13257,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C57C0D72-947E-4C2B-A236-E53FEC630DCE}">
   <dimension ref="A1:V76"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AL41" sqref="AL41"/>
+    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="8" max="8" width="12.28515625" customWidth="1"/>
     <col min="11" max="11" width="13.85546875" customWidth="1"/>
     <col min="22" max="22" width="14.85546875" customWidth="1"/>
@@ -13229,8 +13322,8 @@
       <c r="A5" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="10">
-        <v>53033.765978847536</v>
+      <c r="B5">
+        <v>84235.074145566847</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>4</v>
@@ -13242,12 +13335,12 @@
       <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="10">
-        <v>0.2869454363851805</v>
+      <c r="B6">
+        <v>0.23530860035973067</v>
       </c>
       <c r="D6" s="8">
-        <f>SUM(K14:K40)</f>
-        <v>4172227.5909556332</v>
+        <f>SUM(K14:K43)</f>
+        <v>15311919.440978015</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -13257,7 +13350,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="11">
-        <v>23.187100162200856</v>
+        <v>26.668464164877538</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -13303,22 +13396,22 @@
       </c>
       <c r="H14" s="5">
         <f xml:space="preserve"> $B$5 / ( 1 + EXP(-$B$6 * (C14- $B$7)))</f>
-        <v>68.303618998809156</v>
+        <v>158.24860932963421</v>
       </c>
       <c r="K14" s="5">
         <f>(H14   -F14) ^2</f>
-        <v>234.20075446071257</v>
+        <v>11077.269765821964</v>
       </c>
       <c r="M14" s="1">
         <v>43889</v>
       </c>
       <c r="N14" s="5">
         <f>H16</f>
-        <v>121.12896113698618</v>
+        <v>253.06745485112174</v>
       </c>
       <c r="P14" s="5">
         <f>H18</f>
-        <v>214.643335590269</v>
+        <v>404.42624006866242</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -13333,22 +13426,22 @@
       </c>
       <c r="H15" s="5">
         <f t="shared" ref="H15:H76" si="0" xml:space="preserve"> $B$5 / ( 1 + EXP(-$B$6 * (C15- $B$7)))</f>
-        <v>90.965492878143237</v>
+        <v>200.13208872517259</v>
       </c>
       <c r="K15" s="5">
-        <f t="shared" ref="K15:K40" si="1">(H15   -F15) ^2</f>
-        <v>623.27583464862073</v>
+        <f t="shared" ref="K15:K43" si="1">(H15   -F15) ^2</f>
+        <v>17991.417225777572</v>
       </c>
       <c r="M15" s="1">
         <v>43890</v>
       </c>
       <c r="N15" s="5">
         <f t="shared" ref="N15:N36" si="2">H17</f>
-        <v>161.26394088790207</v>
+        <v>319.95102992103489</v>
       </c>
       <c r="P15" s="5">
         <f t="shared" ref="P15:P34" si="3">H19</f>
-        <v>285.59621048808287</v>
+        <v>511.06921850834965</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -13363,22 +13456,22 @@
       </c>
       <c r="H16" s="5">
         <f t="shared" si="0"/>
-        <v>121.12896113698618</v>
+        <v>253.06745485112174</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="1"/>
-        <v>17.048320070742186</v>
+        <v>18514.352269662053</v>
       </c>
       <c r="M16" s="1">
         <v>43891</v>
       </c>
       <c r="N16" s="5">
         <f t="shared" si="2"/>
-        <v>214.643335590269</v>
+        <v>404.42624006866242</v>
       </c>
       <c r="P16" s="5">
         <f t="shared" si="3"/>
-        <v>379.83472587751538</v>
+        <v>645.61626803348372</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -13393,22 +13486,22 @@
       </c>
       <c r="H17" s="5">
         <f t="shared" si="0"/>
-        <v>161.26394088790207</v>
+        <v>319.95102992103489</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" si="1"/>
-        <v>126.87636432615199</v>
+        <v>28883.352571220497</v>
       </c>
       <c r="M17" s="1">
         <v>43892</v>
       </c>
       <c r="N17" s="5">
         <f t="shared" si="2"/>
-        <v>285.59621048808287</v>
+        <v>511.06921850834965</v>
       </c>
       <c r="P17" s="5">
         <f t="shared" si="3"/>
-        <v>504.87160346495972</v>
+        <v>815.24004624698159</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -13423,22 +13516,22 @@
       </c>
       <c r="H18" s="5">
         <f t="shared" si="0"/>
-        <v>214.643335590269</v>
+        <v>404.42624006866242</v>
       </c>
       <c r="K18" s="5">
         <f t="shared" si="1"/>
-        <v>709.86733137569502</v>
+        <v>46840.3173902583</v>
       </c>
       <c r="M18" s="1">
         <v>43893</v>
       </c>
       <c r="N18" s="5">
         <f t="shared" si="2"/>
-        <v>379.83472587751538</v>
+        <v>645.61626803348372</v>
       </c>
       <c r="P18" s="5">
         <f t="shared" si="3"/>
-        <v>670.54489150100426</v>
+        <v>1028.880801304208</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -13453,22 +13546,22 @@
       </c>
       <c r="H19" s="5">
         <f t="shared" si="0"/>
-        <v>285.59621048808287</v>
+        <v>511.06921850834965</v>
       </c>
       <c r="K19" s="5">
         <f t="shared" si="1"/>
-        <v>2079.0144108735585</v>
+        <v>73478.521222727402</v>
       </c>
       <c r="M19" s="1">
         <v>43894</v>
       </c>
       <c r="N19" s="5">
         <f t="shared" si="2"/>
-        <v>504.87160346495972</v>
+        <v>815.24004624698159</v>
       </c>
       <c r="P19" s="5">
         <f t="shared" si="3"/>
-        <v>889.66299086053834</v>
+        <v>1297.637080419235</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -13483,22 +13576,22 @@
       </c>
       <c r="H20" s="5">
         <f t="shared" si="0"/>
-        <v>379.83472587751538</v>
+        <v>645.61626803348372</v>
       </c>
       <c r="K20" s="5">
         <f t="shared" si="1"/>
-        <v>950.78031994151672</v>
+        <v>87981.210462111456</v>
       </c>
       <c r="M20" s="1">
         <v>43895</v>
       </c>
       <c r="N20" s="5">
         <f t="shared" si="2"/>
-        <v>670.54489150100426</v>
+        <v>1028.880801304208</v>
       </c>
       <c r="P20" s="5">
         <f t="shared" si="3"/>
-        <v>1178.7717886166843</v>
+        <v>1635.2161357509153</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -13513,22 +13606,22 @@
       </c>
       <c r="H21" s="5">
         <f t="shared" si="0"/>
-        <v>504.87160346495972</v>
+        <v>815.24004624698159</v>
       </c>
       <c r="K21" s="5">
         <f t="shared" si="1"/>
-        <v>848.46348470254668</v>
+        <v>79095.963613004351</v>
       </c>
       <c r="M21" s="1">
         <v>43896</v>
       </c>
       <c r="N21" s="5">
         <f t="shared" si="2"/>
-        <v>889.66299086053834</v>
+        <v>1297.637080419235</v>
       </c>
       <c r="P21" s="5">
         <f t="shared" si="3"/>
-        <v>1559.0217023610269</v>
+        <v>2058.4364229617486</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -13543,22 +13636,22 @@
       </c>
       <c r="H22" s="5">
         <f t="shared" si="0"/>
-        <v>670.54489150100426</v>
+        <v>1028.880801304208</v>
       </c>
       <c r="K22" s="5">
         <f t="shared" si="1"/>
-        <v>181.03994471974744</v>
+        <v>118942.76710823263</v>
       </c>
       <c r="M22" s="1">
         <v>43897</v>
       </c>
       <c r="N22" s="5">
         <f t="shared" si="2"/>
-        <v>1178.7717886166843</v>
+        <v>1635.2161357509153</v>
       </c>
       <c r="P22" s="5">
         <f t="shared" si="3"/>
-        <v>2057.0672487014303</v>
+        <v>2587.7612928824856</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -13573,22 +13666,22 @@
       </c>
       <c r="H23" s="5">
         <f t="shared" si="0"/>
-        <v>889.66299086053834</v>
+        <v>1297.637080419235</v>
       </c>
       <c r="K23" s="5">
         <f t="shared" si="1"/>
-        <v>1820.1307891663782</v>
+        <v>203073.77824877203</v>
       </c>
       <c r="M23" s="1">
         <v>43898</v>
       </c>
       <c r="N23" s="5">
         <f t="shared" si="2"/>
-        <v>1559.0217023610269</v>
+        <v>2058.4364229617486</v>
       </c>
       <c r="P23" s="5">
         <f t="shared" si="3"/>
-        <v>2705.8549183906634</v>
+        <v>3247.8219120093945</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -13603,22 +13696,22 @@
       </c>
       <c r="H24" s="5">
         <f t="shared" si="0"/>
-        <v>1178.7717886166843</v>
+        <v>1635.2161357509153</v>
       </c>
       <c r="K24" s="5">
         <f t="shared" si="1"/>
-        <v>4458.4717550711657</v>
+        <v>273755.12471012026</v>
       </c>
       <c r="M24" s="1">
         <v>43899</v>
       </c>
       <c r="N24" s="5">
         <f t="shared" si="2"/>
-        <v>2057.0672487014303</v>
+        <v>2587.7612928824856</v>
       </c>
       <c r="P24" s="5">
         <f t="shared" si="3"/>
-        <v>3545.0366160270642</v>
+        <v>4067.856113565148</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -13633,22 +13726,22 @@
       </c>
       <c r="H25" s="5">
         <f t="shared" si="0"/>
-        <v>1559.0217023610269</v>
+        <v>2058.4364229617486</v>
       </c>
       <c r="K25" s="5">
         <f t="shared" si="1"/>
-        <v>35.740042660151552</v>
+        <v>243479.50350528563</v>
       </c>
       <c r="M25" s="1">
         <v>43900</v>
       </c>
       <c r="N25" s="5">
         <f t="shared" si="2"/>
-        <v>2705.8549183906634</v>
+        <v>3247.8219120093945</v>
       </c>
       <c r="P25" s="5">
         <f t="shared" si="3"/>
-        <v>4620.5839948215489</v>
+        <v>5081.9463686354266</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -13663,22 +13756,22 @@
       </c>
       <c r="H26" s="5">
         <f t="shared" si="0"/>
-        <v>2057.0672487014303</v>
+        <v>2587.7612928824856</v>
       </c>
       <c r="K26" s="5">
         <f t="shared" si="1"/>
-        <v>8293.2437860481659</v>
+        <v>386587.10532690003</v>
       </c>
       <c r="M26" s="1">
         <v>43901</v>
       </c>
       <c r="N26" s="5">
         <f t="shared" si="2"/>
-        <v>3545.0366160270642</v>
+        <v>4067.856113565148</v>
       </c>
       <c r="P26" s="5">
         <f t="shared" si="3"/>
-        <v>5982.9970232969827</v>
+        <v>6328.8847288327743</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -13693,22 +13786,22 @@
       </c>
       <c r="H27" s="5">
         <f t="shared" si="0"/>
-        <v>2705.8549183906634</v>
+        <v>3247.8219120093945</v>
       </c>
       <c r="K27" s="5">
         <f t="shared" si="1"/>
-        <v>1532.3374142016191</v>
+        <v>252829.87519678328</v>
       </c>
       <c r="M27" s="1">
         <v>43902</v>
       </c>
       <c r="N27" s="5">
         <f t="shared" si="2"/>
-        <v>4620.5839948215489</v>
+        <v>5081.9463686354266</v>
       </c>
       <c r="P27" s="5">
         <f t="shared" si="3"/>
-        <v>7683.3732794728712</v>
+        <v>7851.4309989848898</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -13723,22 +13816,22 @@
       </c>
       <c r="H28" s="5">
         <f t="shared" si="0"/>
-        <v>3545.0366160270642</v>
+        <v>4067.856113565148</v>
       </c>
       <c r="K28" s="5">
         <f t="shared" si="1"/>
-        <v>16890.481173696757</v>
+        <v>154335.92596551246</v>
       </c>
       <c r="M28" s="1">
         <v>43903</v>
       </c>
       <c r="N28" s="5">
         <f t="shared" si="2"/>
-        <v>5982.9970232969827</v>
+        <v>6328.8847288327743</v>
       </c>
       <c r="P28" s="5">
         <f t="shared" si="3"/>
-        <v>9766.6871293489621</v>
+        <v>9694.6776870519116</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -13753,22 +13846,22 @@
       </c>
       <c r="H29" s="5">
         <f t="shared" si="0"/>
-        <v>4620.5839948215489</v>
+        <v>5081.9463686354266</v>
       </c>
       <c r="K29" s="5">
         <f t="shared" si="1"/>
-        <v>1266.2206874600199</v>
+        <v>246955.69329993727</v>
       </c>
       <c r="M29" s="1">
         <v>43904</v>
       </c>
       <c r="N29" s="5">
         <f t="shared" si="2"/>
-        <v>7683.3732794728712</v>
+        <v>7851.4309989848898</v>
       </c>
       <c r="P29" s="5">
         <f t="shared" si="3"/>
-        <v>12262.146107635637</v>
+        <v>11903.220958402673</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -13783,22 +13876,22 @@
       </c>
       <c r="H30" s="5">
         <f t="shared" si="0"/>
-        <v>5982.9970232969827</v>
+        <v>6328.8847288327743</v>
       </c>
       <c r="K30" s="5">
         <f t="shared" si="1"/>
-        <v>28898.987929834864</v>
+        <v>266137.05344286503</v>
       </c>
       <c r="M30" s="1">
         <v>43905</v>
       </c>
       <c r="N30" s="5">
         <f t="shared" si="2"/>
-        <v>9766.6871293489621</v>
+        <v>9694.6776870519116</v>
       </c>
       <c r="P30" s="5">
         <f t="shared" si="3"/>
-        <v>15171.635184648756</v>
+        <v>14516.906905723705</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -13813,22 +13906,22 @@
       </c>
       <c r="H31" s="5">
         <f t="shared" si="0"/>
-        <v>7683.3732794728712</v>
+        <v>7851.4309989848898</v>
       </c>
       <c r="K31" s="5">
         <f t="shared" si="1"/>
-        <v>169227.97506426502</v>
+        <v>335740.28258462739</v>
       </c>
       <c r="M31" s="1">
         <v>43906</v>
       </c>
       <c r="N31" s="5">
         <f t="shared" si="2"/>
-        <v>12262.146107635637</v>
+        <v>11903.220958402673</v>
       </c>
       <c r="P31" s="5">
         <f t="shared" si="3"/>
-        <v>18458.923488631015</v>
+        <v>17565.132547694819</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -13843,22 +13936,22 @@
       </c>
       <c r="H32" s="5">
         <f t="shared" si="0"/>
-        <v>9766.6871293489621</v>
+        <v>9694.6776870519116</v>
       </c>
       <c r="K32" s="5">
         <f t="shared" si="1"/>
-        <v>165394.42117809944</v>
+        <v>112009.15421041725</v>
       </c>
       <c r="M32" s="1">
         <v>43907</v>
       </c>
       <c r="N32" s="5">
         <f t="shared" si="2"/>
-        <v>15171.635184648756</v>
+        <v>14516.906905723705</v>
       </c>
       <c r="P32" s="5">
         <f t="shared" si="3"/>
-        <v>22043.788622023767</v>
+        <v>21060.07189364206</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -13873,20 +13966,20 @@
       </c>
       <c r="H33" s="5">
         <f t="shared" si="0"/>
-        <v>12262.146107635637</v>
+        <v>11903.220958402673</v>
       </c>
       <c r="K33" s="5">
         <f t="shared" si="1"/>
-        <v>4469.4429242658016</v>
+        <v>181287.79226353814</v>
       </c>
       <c r="N33" s="5">
         <f t="shared" si="2"/>
-        <v>18458.923488631015</v>
+        <v>17565.132547694819</v>
       </c>
       <c r="O33" s="1"/>
       <c r="P33" s="5">
         <f t="shared" si="3"/>
-        <v>25805.240837329446</v>
+        <v>24989.74913216709</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -13901,20 +13994,20 @@
       </c>
       <c r="H34" s="5">
         <f t="shared" si="0"/>
-        <v>15171.635184648756</v>
+        <v>14516.906905723705</v>
       </c>
       <c r="K34" s="5">
         <f t="shared" si="1"/>
-        <v>22609.577695613712</v>
+        <v>648174.89045137959</v>
       </c>
       <c r="N34" s="5">
         <f t="shared" si="2"/>
-        <v>22043.788622023767</v>
+        <v>21060.07189364206</v>
       </c>
       <c r="O34" s="1"/>
       <c r="P34" s="5">
         <f t="shared" si="3"/>
-        <v>29595.572735160196</v>
+        <v>29312.45865400559</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -13929,15 +14022,15 @@
       </c>
       <c r="H35" s="5">
         <f t="shared" si="0"/>
-        <v>18458.923488631015</v>
+        <v>17565.132547694819</v>
       </c>
       <c r="K35" s="5">
         <f t="shared" si="1"/>
-        <v>1935093.8604825058</v>
+        <v>5220619.2746035699</v>
       </c>
       <c r="N35" s="5">
         <f t="shared" si="2"/>
-        <v>25805.240837329446</v>
+        <v>24989.74913216709</v>
       </c>
       <c r="O35" s="1"/>
       <c r="P35" s="5"/>
@@ -13954,15 +14047,15 @@
       </c>
       <c r="H36" s="5">
         <f t="shared" si="0"/>
-        <v>22043.788622023767</v>
+        <v>21060.07189364206</v>
       </c>
       <c r="K36" s="5">
         <f t="shared" si="1"/>
-        <v>103820.17209734292</v>
+        <v>1705448.2189756355</v>
       </c>
       <c r="N36" s="5">
         <f t="shared" si="2"/>
-        <v>29595.572735160196</v>
+        <v>29312.45865400559</v>
       </c>
       <c r="O36" s="1"/>
       <c r="P36" s="5"/>
@@ -13979,11 +14072,11 @@
       </c>
       <c r="H37" s="5">
         <f t="shared" si="0"/>
-        <v>25805.240837329446</v>
+        <v>24989.74913216709</v>
       </c>
       <c r="K37" s="5">
         <f t="shared" si="1"/>
-        <v>865348.0154353882</v>
+        <v>13167.363333100187</v>
       </c>
       <c r="N37" s="5"/>
       <c r="O37" s="1"/>
@@ -14000,11 +14093,11 @@
       </c>
       <c r="H38" s="5">
         <f t="shared" si="0"/>
-        <v>29595.572735160196</v>
+        <v>29312.45865400559</v>
       </c>
       <c r="K38" s="5">
         <f t="shared" si="1"/>
-        <v>291138.73652825534</v>
+        <v>65771.041214358804</v>
       </c>
       <c r="N38" s="5"/>
       <c r="O38" s="1"/>
@@ -14018,11 +14111,11 @@
       </c>
       <c r="H39" s="5">
         <f t="shared" si="0"/>
-        <v>33262.529379811182</v>
+        <v>33954.367087480714</v>
       </c>
       <c r="K39" s="5">
         <f t="shared" si="1"/>
-        <v>123572.90487043395</v>
+        <v>1088614.8792379878</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -14034,11 +14127,11 @@
       </c>
       <c r="H40" s="5">
         <f t="shared" si="0"/>
-        <v>36672.933615439004</v>
+        <v>38811.903157882982</v>
       </c>
       <c r="K40" s="5">
         <f t="shared" si="1"/>
-        <v>422586.30433620483</v>
+        <v>2216832.6135539152</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -14046,27 +14139,48 @@
       <c r="C41">
         <v>27</v>
       </c>
+      <c r="F41">
+        <v>43211</v>
+      </c>
       <c r="H41" s="5">
         <f t="shared" si="0"/>
-        <v>39730.346724714836</v>
+        <v>43759.566989078616</v>
+      </c>
+      <c r="K41" s="5">
+        <f t="shared" si="1"/>
+        <v>300925.74150677811</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>28</v>
       </c>
+      <c r="F42">
+        <v>49039</v>
+      </c>
       <c r="H42" s="5">
         <f t="shared" si="0"/>
-        <v>42382.354097126859</v>
+        <v>48662.254887716961</v>
+      </c>
+      <c r="K42" s="5">
+        <f t="shared" si="1"/>
+        <v>141936.87962915958</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C43">
         <v>29</v>
       </c>
+      <c r="F43">
+        <v>54268</v>
+      </c>
       <c r="H43" s="5">
         <f t="shared" si="0"/>
-        <v>44617.678298200379</v>
+        <v>53389.687938094576</v>
+      </c>
+      <c r="K43" s="5">
+        <f t="shared" si="1"/>
+        <v>771432.07808855793</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
@@ -14075,7 +14189,7 @@
       </c>
       <c r="H44" s="5">
         <f t="shared" si="0"/>
-        <v>46456.691744204021</v>
+        <v>57829.774423223273</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -14084,7 +14198,7 @@
       </c>
       <c r="H45" s="5">
         <f t="shared" si="0"/>
-        <v>47939.738269915484</v>
+        <v>61898.124441750391</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -14093,7 +14207,7 @@
       </c>
       <c r="H46" s="5">
         <f t="shared" si="0"/>
-        <v>49116.57371381329</v>
+        <v>65542.264209436646</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -14102,7 +14216,7 @@
       </c>
       <c r="H47" s="5">
         <f t="shared" si="0"/>
-        <v>50038.520212990705</v>
+        <v>68740.704811288</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -14111,7 +14225,7 @@
       </c>
       <c r="H48" s="5">
         <f t="shared" si="0"/>
-        <v>50753.551881858009</v>
+        <v>71498.226204060993</v>
       </c>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
@@ -14120,7 +14234,7 @@
       </c>
       <c r="H49" s="5">
         <f t="shared" si="0"/>
-        <v>51303.790993575371</v>
+        <v>73839.211764449356</v>
       </c>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
@@ -14129,7 +14243,7 @@
       </c>
       <c r="H50" s="5">
         <f t="shared" si="0"/>
-        <v>51724.676509154349</v>
+        <v>75800.689564375207</v>
       </c>
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.25">
@@ -14138,7 +14252,7 @@
       </c>
       <c r="H51" s="5">
         <f t="shared" si="0"/>
-        <v>52045.138013739277</v>
+        <v>77426.20497618636</v>
       </c>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.25">
@@ -14147,7 +14261,7 @@
       </c>
       <c r="H52" s="5">
         <f t="shared" si="0"/>
-        <v>52288.28205892507</v>
+        <v>78761.066754865271</v>
       </c>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.25">
@@ -14156,7 +14270,7 @@
       </c>
       <c r="H53" s="5">
         <f t="shared" si="0"/>
-        <v>52472.272188098643</v>
+        <v>79849.056716641455</v>
       </c>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.25">
@@ -14165,7 +14279,7 @@
       </c>
       <c r="H54" s="5">
         <f t="shared" si="0"/>
-        <v>52611.219355907269</v>
+        <v>80730.424780020927</v>
       </c>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.25">
@@ -14174,7 +14288,7 @@
       </c>
       <c r="H55" s="5">
         <f t="shared" si="0"/>
-        <v>52715.990909288703</v>
+        <v>81440.88006793255</v>
       </c>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.25">
@@ -14183,7 +14297,7 @@
       </c>
       <c r="H56" s="5">
         <f t="shared" si="0"/>
-        <v>52794.902025058655</v>
+        <v>82011.280544749272</v>
       </c>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.25">
@@ -14192,7 +14306,7 @@
       </c>
       <c r="H57" s="5">
         <f t="shared" si="0"/>
-        <v>52854.284348607027</v>
+        <v>82467.767564984897</v>
       </c>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.25">
@@ -14201,7 +14315,7 @@
       </c>
       <c r="H58" s="5">
         <f t="shared" si="0"/>
-        <v>52898.941741262737</v>
+        <v>82832.152624154201</v>
       </c>
     </row>
     <row r="59" spans="3:8" x14ac:dyDescent="0.25">
@@ -14210,7 +14324,7 @@
       </c>
       <c r="H59" s="5">
         <f t="shared" si="0"/>
-        <v>52932.509073506204</v>
+        <v>83122.422044591469</v>
       </c>
     </row>
     <row r="60" spans="3:8" x14ac:dyDescent="0.25">
@@ -14219,7 +14333,7 @@
       </c>
       <c r="H60" s="5">
         <f t="shared" si="0"/>
-        <v>52957.731124179081</v>
+        <v>83353.273049438518</v>
       </c>
     </row>
     <row r="61" spans="3:8" x14ac:dyDescent="0.25">
@@ -14228,7 +14342,7 @@
       </c>
       <c r="H61" s="5">
         <f t="shared" si="0"/>
-        <v>52976.677398026754</v>
+        <v>83536.629969071699</v>
       </c>
     </row>
     <row r="62" spans="3:8" x14ac:dyDescent="0.25">
@@ -14237,7 +14351,7 @@
       </c>
       <c r="H62" s="5">
         <f t="shared" si="0"/>
-        <v>52990.906482876708</v>
+        <v>83682.113576150892</v>
       </c>
     </row>
     <row r="63" spans="3:8" x14ac:dyDescent="0.25">
@@ -14246,7 +14360,7 @@
       </c>
       <c r="H63" s="5">
         <f t="shared" si="0"/>
-        <v>53001.591183074503</v>
+        <v>83797.452181829562</v>
       </c>
     </row>
     <row r="64" spans="3:8" x14ac:dyDescent="0.25">
@@ -14255,7 +14369,7 @@
       </c>
       <c r="H64" s="5">
         <f t="shared" si="0"/>
-        <v>53009.613444485462</v>
+        <v>83888.832566129247</v>
       </c>
     </row>
     <row r="65" spans="3:22" x14ac:dyDescent="0.25">
@@ -14264,7 +14378,7 @@
       </c>
       <c r="H65" s="5">
         <f t="shared" si="0"/>
-        <v>53015.636169841826</v>
+        <v>83961.194063558956</v>
       </c>
     </row>
     <row r="66" spans="3:22" x14ac:dyDescent="0.25">
@@ -14273,7 +14387,7 @@
       </c>
       <c r="H66" s="5">
         <f t="shared" si="0"/>
-        <v>53020.157441637435</v>
+        <v>84018.471681137642</v>
       </c>
     </row>
     <row r="67" spans="3:22" x14ac:dyDescent="0.25">
@@ -14282,7 +14396,7 @@
       </c>
       <c r="H67" s="5">
         <f t="shared" si="0"/>
-        <v>53023.551400945558</v>
+        <v>84063.79504180506</v>
       </c>
     </row>
     <row r="68" spans="3:22" x14ac:dyDescent="0.25">
@@ -14291,7 +14405,7 @@
       </c>
       <c r="H68" s="5">
         <f t="shared" si="0"/>
-        <v>53026.099031664846</v>
+        <v>84099.649923075151</v>
       </c>
     </row>
     <row r="69" spans="3:22" x14ac:dyDescent="0.25">
@@ -14300,7 +14414,7 @@
       </c>
       <c r="H69" s="5">
         <f t="shared" si="0"/>
-        <v>53028.011323563725</v>
+        <v>84128.008646616392</v>
       </c>
     </row>
     <row r="70" spans="3:22" x14ac:dyDescent="0.25">
@@ -14309,7 +14423,7 @@
       </c>
       <c r="H70" s="5">
         <f t="shared" si="0"/>
-        <v>53029.44668998674</v>
+        <v>84150.434843402894</v>
       </c>
     </row>
     <row r="71" spans="3:22" x14ac:dyDescent="0.25">
@@ -14318,7 +14432,7 @@
       </c>
       <c r="H71" s="5">
         <f t="shared" si="0"/>
-        <v>53030.524059151925</v>
+        <v>84168.167330967262</v>
       </c>
     </row>
     <row r="72" spans="3:22" x14ac:dyDescent="0.25">
@@ -14327,7 +14441,7 @@
       </c>
       <c r="H72" s="5">
         <f t="shared" si="0"/>
-        <v>53031.332710225921</v>
+        <v>84182.187081227676</v>
       </c>
       <c r="V72" s="5"/>
     </row>
@@ -14337,7 +14451,7 @@
       </c>
       <c r="H73" s="5">
         <f t="shared" si="0"/>
-        <v>53031.939661658762</v>
+        <v>84193.270571902263</v>
       </c>
     </row>
     <row r="74" spans="3:22" x14ac:dyDescent="0.25">
@@ -14346,7 +14460,7 @@
       </c>
       <c r="H74" s="5">
         <f t="shared" si="0"/>
-        <v>53032.395219810824</v>
+        <v>84202.032217901244</v>
       </c>
     </row>
     <row r="75" spans="3:22" x14ac:dyDescent="0.25">
@@ -14355,7 +14469,7 @@
       </c>
       <c r="H75" s="5">
         <f t="shared" si="0"/>
-        <v>53032.737145344749</v>
+        <v>84208.95807280502</v>
       </c>
     </row>
     <row r="76" spans="3:22" x14ac:dyDescent="0.25">
@@ -14364,7 +14478,7 @@
       </c>
       <c r="H76" s="5">
         <f t="shared" si="0"/>
-        <v>53032.993781367346</v>
+        <v>84214.432568462347</v>
       </c>
     </row>
   </sheetData>
@@ -14377,14 +14491,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA34C47C-1418-4979-B708-48EA867A2B48}">
   <dimension ref="A1:V76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V31" sqref="V31"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y44" sqref="Y44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.28515625" customWidth="1"/>
     <col min="11" max="11" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14442,7 +14557,7 @@
         <v>8</v>
       </c>
       <c r="B5" s="10">
-        <v>55884.123549401062</v>
+        <v>128611.92634076305</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>4</v>
@@ -14455,11 +14570,11 @@
         <v>18</v>
       </c>
       <c r="B6" s="10">
-        <v>4.9095537402815519E-6</v>
+        <v>1.3848878138816741E-6</v>
       </c>
       <c r="D6" s="8">
-        <f>SUM(K14:K40)</f>
-        <v>4087582.2734565753</v>
+        <f>SUM(K14:K44)</f>
+        <v>10925113.485261798</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -14469,7 +14584,7 @@
         <v>19</v>
       </c>
       <c r="B7" s="11">
-        <v>-18.958662725840405</v>
+        <v>-40.574222690328597</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
@@ -14477,7 +14592,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="7">
-        <v>27.725566588389558</v>
+        <v>261.41134120050532</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
@@ -14485,7 +14600,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="7">
-        <v>2.5028609409647861E-7</v>
+        <v>296.55289749734055</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -14523,22 +14638,22 @@
       </c>
       <c r="H14" s="5">
         <f xml:space="preserve"> $B$5 * 0.5 / ( 0.5 + ($B$5-0.5) * EXP(-$B$6 * $B$5 * (C14- $B$7))) - ($B$8 * C14 + $B$9)</f>
-        <v>90.636145428703131</v>
+        <v>387.69645273786119</v>
       </c>
       <c r="K14" s="5">
         <f>(H14   -F14) ^2</f>
-        <v>1416.4794427304917</v>
+        <v>112021.71547530736</v>
       </c>
       <c r="M14" s="1">
         <v>43889</v>
       </c>
       <c r="N14" s="5">
         <f>H16</f>
-        <v>101.25939558249988</v>
+        <v>155.46549942241768</v>
       </c>
       <c r="P14" s="5">
         <f>H18</f>
-        <v>159.81760974569073</v>
+        <v>45.306532597530804</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -14553,22 +14668,22 @@
       </c>
       <c r="H15" s="5">
         <f t="shared" ref="H15:H76" si="0" xml:space="preserve"> $B$5 * 0.5 / ( 0.5 + ($B$5-0.5) * EXP(-$B$6 * $B$5 * (C15- $B$7))) - ($B$8 * C15 + $B$9)</f>
-        <v>91.46305745816548</v>
+        <v>258.83945124451031</v>
       </c>
       <c r="K15" s="5">
-        <f t="shared" ref="K15:K40" si="1">(H15   -F15) ^2</f>
-        <v>648.36729511783665</v>
+        <f t="shared" ref="K15:K45" si="1">(H15   -F15) ^2</f>
+        <v>37187.053956283868</v>
       </c>
       <c r="M15" s="1">
         <v>43890</v>
       </c>
       <c r="N15" s="5">
         <f t="shared" ref="N15:N36" si="2">H17</f>
-        <v>122.82441084526189</v>
+        <v>82.390736393145971</v>
       </c>
       <c r="P15" s="5">
         <f t="shared" ref="P15:P34" si="3">H19</f>
-        <v>217.01344071940468</v>
+        <v>50.92378364832166</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -14583,22 +14698,22 @@
       </c>
       <c r="H16" s="5">
         <f t="shared" si="0"/>
-        <v>101.25939558249988</v>
+        <v>155.46549942241768</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" si="1"/>
-        <v>247.76662742822438</v>
+        <v>1479.5946458160147</v>
       </c>
       <c r="M16" s="1">
         <v>43891</v>
       </c>
       <c r="N16" s="5">
         <f t="shared" si="2"/>
-        <v>159.81760974569073</v>
+        <v>45.306532597530804</v>
       </c>
       <c r="P16" s="5">
         <f t="shared" si="3"/>
-        <v>300.62435699916819</v>
+        <v>107.13470032347141</v>
       </c>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
@@ -14613,22 +14728,22 @@
       </c>
       <c r="H17" s="5">
         <f t="shared" si="0"/>
-        <v>122.82441084526189</v>
+        <v>82.390736393145971</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" si="1"/>
-        <v>738.51264590711935</v>
+        <v>4571.0125254610766</v>
       </c>
       <c r="M17" s="1">
         <v>43892</v>
       </c>
       <c r="N17" s="5">
         <f t="shared" si="2"/>
-        <v>217.01344071940468</v>
+        <v>50.92378364832166</v>
       </c>
       <c r="P17" s="5">
         <f t="shared" si="3"/>
-        <v>418.70545253443061</v>
+        <v>223.1913854301547</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -14643,22 +14758,22 @@
       </c>
       <c r="H18" s="5">
         <f t="shared" si="0"/>
-        <v>159.81760974569073</v>
+        <v>45.306532597530804</v>
       </c>
       <c r="K18" s="5">
         <f t="shared" si="1"/>
-        <v>794.24712044618605</v>
+        <v>20361.425639339541</v>
       </c>
       <c r="M18" s="1">
         <v>43893</v>
       </c>
       <c r="N18" s="5">
         <f t="shared" si="2"/>
-        <v>300.62435699916819</v>
+        <v>107.13470032347141</v>
       </c>
       <c r="P18" s="5">
         <f t="shared" si="3"/>
-        <v>581.65239796990647</v>
+        <v>409.89887219632919</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
@@ -14673,22 +14788,22 @@
       </c>
       <c r="H19" s="5">
         <f t="shared" si="0"/>
-        <v>217.01344071940468</v>
+        <v>50.92378364832166</v>
       </c>
       <c r="K19" s="5">
         <f t="shared" si="1"/>
-        <v>528.38190756032259</v>
+        <v>35749.815589866674</v>
       </c>
       <c r="M19" s="1">
         <v>43894</v>
       </c>
       <c r="N19" s="5">
         <f t="shared" si="2"/>
-        <v>418.70545253443061</v>
+        <v>223.1913854301547</v>
       </c>
       <c r="P19" s="5">
         <f t="shared" si="3"/>
-        <v>802.79895140868052</v>
+        <v>679.81791829133772</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -14703,22 +14818,22 @@
       </c>
       <c r="H20" s="5">
         <f t="shared" si="0"/>
-        <v>300.62435699916819</v>
+        <v>107.13470032347141</v>
       </c>
       <c r="K20" s="5">
         <f t="shared" si="1"/>
-        <v>2340.2028357439281</v>
+        <v>58498.823187616981</v>
       </c>
       <c r="M20" s="1">
         <v>43895</v>
       </c>
       <c r="N20" s="5">
         <f t="shared" si="2"/>
-        <v>581.65239796990647</v>
+        <v>409.89887219632919</v>
       </c>
       <c r="P20" s="5">
         <f t="shared" si="3"/>
-        <v>1099.1077581784596</v>
+        <v>1047.4694745254906</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -14733,22 +14848,22 @@
       </c>
       <c r="H21" s="5">
         <f t="shared" si="0"/>
-        <v>418.70545253443061</v>
+        <v>223.1913854301547</v>
       </c>
       <c r="K21" s="5">
         <f t="shared" si="1"/>
-        <v>13292.832675290434</v>
+        <v>96601.994890826652</v>
       </c>
       <c r="M21" s="1">
         <v>43896</v>
       </c>
       <c r="N21" s="5">
         <f t="shared" si="2"/>
-        <v>802.79895140868052</v>
+        <v>679.81791829133772</v>
       </c>
       <c r="P21" s="5">
         <f t="shared" si="3"/>
-        <v>1491.9237867461243</v>
+        <v>1529.5281302091885</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -14763,22 +14878,22 @@
       </c>
       <c r="H22" s="5">
         <f t="shared" si="0"/>
-        <v>581.65239796990647</v>
+        <v>409.89887219632919</v>
       </c>
       <c r="K22" s="5">
         <f t="shared" si="1"/>
-        <v>10475.031641310405</v>
+        <v>75131.428263244277</v>
       </c>
       <c r="M22" s="1">
         <v>43897</v>
       </c>
       <c r="N22" s="5">
         <f t="shared" si="2"/>
-        <v>1099.1077581784596</v>
+        <v>1047.4694745254906</v>
       </c>
       <c r="P22" s="5">
         <f t="shared" si="3"/>
-        <v>2007.7171615497291</v>
+        <v>2144.9857503027552</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -14793,22 +14908,22 @@
       </c>
       <c r="H23" s="5">
         <f t="shared" si="0"/>
-        <v>802.79895140868052</v>
+        <v>679.81791829133772</v>
       </c>
       <c r="K23" s="5">
         <f t="shared" si="1"/>
-        <v>1953.7326965721854</v>
+        <v>27949.848444441832</v>
       </c>
       <c r="M23" s="1">
         <v>43898</v>
       </c>
       <c r="N23" s="5">
         <f t="shared" si="2"/>
-        <v>1491.9237867461243</v>
+        <v>1529.5281302091885</v>
       </c>
       <c r="P23" s="5">
         <f t="shared" si="3"/>
-        <v>2678.673935021362</v>
+        <v>2915.2588250648469</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
@@ -14823,22 +14938,22 @@
       </c>
       <c r="H24" s="5">
         <f t="shared" si="0"/>
-        <v>1099.1077581784596</v>
+        <v>1047.4694745254906</v>
       </c>
       <c r="K24" s="5">
         <f t="shared" si="1"/>
-        <v>166.2098991850763</v>
+        <v>4164.1887180163103</v>
       </c>
       <c r="M24" s="1">
         <v>43899</v>
       </c>
       <c r="N24" s="5">
         <f t="shared" si="2"/>
-        <v>2007.7171615497291</v>
+        <v>2144.9857503027552</v>
       </c>
       <c r="P24" s="5">
         <f t="shared" si="3"/>
-        <v>3542.8938465611386</v>
+        <v>3864.2038205801846</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
@@ -14853,22 +14968,22 @@
       </c>
       <c r="H25" s="5">
         <f t="shared" si="0"/>
-        <v>1491.9237867461243</v>
+        <v>1529.5281302091885</v>
       </c>
       <c r="K25" s="5">
         <f t="shared" si="1"/>
-        <v>5340.1329435259213</v>
+        <v>1258.2535464562873</v>
       </c>
       <c r="M25" s="1">
         <v>43900</v>
       </c>
       <c r="N25" s="5">
         <f t="shared" si="2"/>
-        <v>2678.673935021362</v>
+        <v>2915.2588250648469</v>
       </c>
       <c r="P25" s="5">
         <f t="shared" si="3"/>
-        <v>4643.8261897918283</v>
+        <v>5017.9945035789497</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
@@ -14883,22 +14998,22 @@
       </c>
       <c r="H26" s="5">
         <f t="shared" si="0"/>
-        <v>2007.7171615497291</v>
+        <v>2144.9857503027552</v>
       </c>
       <c r="K26" s="5">
         <f t="shared" si="1"/>
-        <v>1740.321567766196</v>
+        <v>32035.898811440216</v>
       </c>
       <c r="M26" s="1">
         <v>43901</v>
       </c>
       <c r="N26" s="5">
         <f t="shared" si="2"/>
-        <v>3542.8938465611386</v>
+        <v>3864.2038205801846</v>
       </c>
       <c r="P26" s="5">
         <f t="shared" si="3"/>
-        <v>6028.4425458745591</v>
+        <v>6404.8049003961269</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -14913,22 +15028,22 @@
       </c>
       <c r="H27" s="5">
         <f t="shared" si="0"/>
-        <v>2678.673935021362</v>
+        <v>2915.2588250648469</v>
       </c>
       <c r="K27" s="5">
         <f t="shared" si="1"/>
-        <v>4399.1468955505088</v>
+        <v>28988.067512462127</v>
       </c>
       <c r="M27" s="1">
         <v>43902</v>
       </c>
       <c r="N27" s="5">
         <f t="shared" si="2"/>
-        <v>4643.8261897918283</v>
+        <v>5017.9945035789497</v>
       </c>
       <c r="P27" s="5">
         <f t="shared" si="3"/>
-        <v>7743.571667643082</v>
+        <v>8054.2332394736932</v>
       </c>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
@@ -14943,22 +15058,22 @@
       </c>
       <c r="H28" s="5">
         <f t="shared" si="0"/>
-        <v>3542.8938465611386</v>
+        <v>3864.2038205801846</v>
       </c>
       <c r="K28" s="5">
         <f t="shared" si="1"/>
-        <v>17452.035776411987</v>
+        <v>35798.085722138676</v>
       </c>
       <c r="M28" s="1">
         <v>43903</v>
       </c>
       <c r="N28" s="5">
         <f t="shared" si="2"/>
-        <v>6028.4425458745591</v>
+        <v>6404.8049003961269</v>
       </c>
       <c r="P28" s="5">
         <f t="shared" si="3"/>
-        <v>9829.9249028294944</v>
+        <v>9996.399107451507</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -14973,22 +15088,22 @@
       </c>
       <c r="H29" s="5">
         <f t="shared" si="0"/>
-        <v>4643.8261897918283</v>
+        <v>5017.9945035789497</v>
       </c>
       <c r="K29" s="5">
         <f t="shared" si="1"/>
-        <v>3460.5206054241989</v>
+        <v>187484.24012958104</v>
       </c>
       <c r="M29" s="1">
         <v>43904</v>
       </c>
       <c r="N29" s="5">
         <f t="shared" si="2"/>
-        <v>7743.571667643082</v>
+        <v>8054.2332394736932</v>
       </c>
       <c r="P29" s="5">
         <f t="shared" si="3"/>
-        <v>12313.779276328774</v>
+        <v>12260.652602763241</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
@@ -15003,22 +15118,22 @@
       </c>
       <c r="H30" s="5">
         <f t="shared" si="0"/>
-        <v>6028.4425458745591</v>
+        <v>6404.8049003961269</v>
       </c>
       <c r="K30" s="5">
         <f t="shared" si="1"/>
-        <v>46415.490572911491</v>
+        <v>350233.04013286962</v>
       </c>
       <c r="M30" s="1">
         <v>43905</v>
       </c>
       <c r="N30" s="5">
         <f t="shared" si="2"/>
-        <v>9829.9249028294944</v>
+        <v>9996.399107451507</v>
       </c>
       <c r="P30" s="5">
         <f t="shared" si="3"/>
-        <v>15197.178474842767</v>
+        <v>14873.855987455525</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -15033,22 +15148,22 @@
       </c>
       <c r="H31" s="5">
         <f t="shared" si="0"/>
-        <v>7743.571667643082</v>
+        <v>8054.2332394736932</v>
       </c>
       <c r="K31" s="5">
         <f t="shared" si="1"/>
-        <v>222379.83772367742</v>
+        <v>611888.84093750827</v>
       </c>
       <c r="M31" s="1">
         <v>43906</v>
       </c>
       <c r="N31" s="5">
         <f t="shared" si="2"/>
-        <v>12313.779276328774</v>
+        <v>12260.652602763241</v>
       </c>
       <c r="P31" s="5">
         <f t="shared" si="3"/>
-        <v>18448.764081966692</v>
+        <v>17858.24072527419</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -15063,22 +15178,22 @@
       </c>
       <c r="H32" s="5">
         <f t="shared" si="0"/>
-        <v>9829.9249028294944</v>
+        <v>9996.399107451507</v>
       </c>
       <c r="K32" s="5">
         <f t="shared" si="1"/>
-        <v>220829.41429930975</v>
+        <v>405003.82396507479</v>
       </c>
       <c r="M32" s="1">
         <v>43907</v>
       </c>
       <c r="N32" s="5">
         <f t="shared" si="2"/>
-        <v>15197.178474842767</v>
+        <v>14873.855987455525</v>
       </c>
       <c r="P32" s="5">
         <f t="shared" si="3"/>
-        <v>21998.459416840924</v>
+        <v>21228.909403484842</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -15093,20 +15208,20 @@
       </c>
       <c r="H33" s="5">
         <f t="shared" si="0"/>
-        <v>12313.779276328774</v>
+        <v>12260.652602763241</v>
       </c>
       <c r="K33" s="5">
         <f t="shared" si="1"/>
-        <v>231.67042907580858</v>
+        <v>4671.3667090393601</v>
       </c>
       <c r="N33" s="5">
         <f t="shared" si="2"/>
-        <v>18448.764081966692</v>
+        <v>17858.24072527419</v>
       </c>
       <c r="O33" s="1"/>
       <c r="P33" s="5">
         <f t="shared" si="3"/>
-        <v>25739.318032988282</v>
+        <v>24991.141478772719</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -15121,20 +15236,20 @@
       </c>
       <c r="H34" s="5">
         <f t="shared" si="0"/>
-        <v>15197.178474842767</v>
+        <v>14873.855987455525</v>
       </c>
       <c r="K34" s="5">
         <f t="shared" si="1"/>
-        <v>15580.413142577707</v>
+        <v>200833.05597946266</v>
       </c>
       <c r="N34" s="5">
         <f t="shared" si="2"/>
-        <v>21998.459416840924</v>
+        <v>21228.909403484842</v>
       </c>
       <c r="O34" s="1"/>
       <c r="P34" s="5">
         <f t="shared" si="3"/>
-        <v>29538.172447073117</v>
+        <v>29137.764309066162</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -15149,15 +15264,15 @@
       </c>
       <c r="H35" s="5">
         <f t="shared" si="0"/>
-        <v>18448.764081966692</v>
+        <v>17858.24072527419</v>
       </c>
       <c r="K35" s="5">
         <f t="shared" si="1"/>
-        <v>1963462.0979866469</v>
+        <v>3967105.0084562828</v>
       </c>
       <c r="N35" s="5">
         <f t="shared" si="2"/>
-        <v>25739.318032988282</v>
+        <v>24991.141478772719</v>
       </c>
       <c r="O35" s="1"/>
       <c r="P35" s="5"/>
@@ -15174,15 +15289,15 @@
       </c>
       <c r="H36" s="5">
         <f t="shared" si="0"/>
-        <v>21998.459416840924</v>
+        <v>21228.909403484842</v>
       </c>
       <c r="K36" s="5">
         <f t="shared" si="1"/>
-        <v>135086.08026891371</v>
+        <v>1292975.0246831975</v>
       </c>
       <c r="N36" s="5">
         <f t="shared" si="2"/>
-        <v>29538.172447073117</v>
+        <v>29137.764309066162</v>
       </c>
       <c r="O36" s="1"/>
       <c r="P36" s="5"/>
@@ -15199,11 +15314,11 @@
       </c>
       <c r="H37" s="5">
         <f t="shared" si="0"/>
-        <v>25739.318032988282</v>
+        <v>24991.141478772719</v>
       </c>
       <c r="K37" s="5">
         <f t="shared" si="1"/>
-        <v>747045.66214873234</v>
+        <v>13488.843091513934</v>
       </c>
       <c r="N37" s="5"/>
       <c r="O37" s="1"/>
@@ -15220,11 +15335,11 @@
       </c>
       <c r="H38" s="5">
         <f t="shared" si="0"/>
-        <v>29538.172447073117</v>
+        <v>29137.764309066162</v>
       </c>
       <c r="K38" s="5">
         <f t="shared" si="1"/>
-        <v>232490.26871647773</v>
+        <v>6685.4022370669009</v>
       </c>
       <c r="N38" s="5"/>
       <c r="O38" s="1"/>
@@ -15238,11 +15353,11 @@
       </c>
       <c r="H39" s="5">
         <f t="shared" si="0"/>
-        <v>33253.503902870929</v>
+        <v>33646.946006973303</v>
       </c>
       <c r="K39" s="5">
         <f t="shared" si="1"/>
-        <v>117308.92348181868</v>
+        <v>541616.52517994912</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
@@ -15254,11 +15369,11 @@
       </c>
       <c r="H40" s="5">
         <f t="shared" si="0"/>
-        <v>36755.76240241812</v>
+        <v>38480.823871020941</v>
       </c>
       <c r="K40" s="5">
         <f t="shared" si="1"/>
-        <v>321758.49211046228</v>
+        <v>1340556.1163059159</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
@@ -15266,36 +15381,64 @@
       <c r="C41">
         <v>27</v>
       </c>
+      <c r="F41">
+        <v>43211</v>
+      </c>
       <c r="H41" s="5">
         <f t="shared" si="0"/>
-        <v>39944.196954618186</v>
+        <v>43585.367640592689</v>
+      </c>
+      <c r="K41" s="5">
+        <f t="shared" si="1"/>
+        <v>140151.13032293675</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C42">
         <v>28</v>
       </c>
+      <c r="F42">
+        <v>49039</v>
+      </c>
       <c r="H42" s="5">
         <f t="shared" si="0"/>
-        <v>42755.909075778647</v>
+        <v>48891.765556695129</v>
+      </c>
+      <c r="K42" s="5">
+        <f t="shared" si="1"/>
+        <v>21677.9812952953</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C43">
         <v>29</v>
       </c>
+      <c r="F43">
+        <v>54268</v>
+      </c>
       <c r="H43" s="5">
         <f t="shared" si="0"/>
-        <v>45166.196227668479</v>
+        <v>54319.411986313346</v>
+      </c>
+      <c r="K43" s="5">
+        <f t="shared" si="1"/>
+        <v>2643.1923366836304</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C44">
         <v>30</v>
       </c>
+      <c r="F44">
+        <v>58655</v>
+      </c>
       <c r="H44" s="5">
         <f t="shared" si="0"/>
-        <v>47182.266972676043</v>
+        <v>59780.301153723172</v>
+      </c>
+      <c r="K44" s="5">
+        <f t="shared" si="1"/>
+        <v>1266302.6865707026</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
@@ -15304,7 +15447,11 @@
       </c>
       <c r="H45" s="5">
         <f t="shared" si="0"/>
-        <v>48833.741449435525</v>
+        <v>65184.357015681235</v>
+      </c>
+      <c r="K45" s="5">
+        <f t="shared" si="1"/>
+        <v>4249000399.5477915</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
@@ -15313,7 +15460,7 @@
       </c>
       <c r="H46" s="5">
         <f t="shared" si="0"/>
-        <v>50163.004469400832</v>
+        <v>70445.032156266403</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
@@ -15322,7 +15469,7 @@
       </c>
       <c r="H47" s="5">
         <f t="shared" si="0"/>
-        <v>51217.28456904435</v>
+        <v>75484.450004784594</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
@@ -15331,7 +15478,7 @@
       </c>
       <c r="H48" s="5">
         <f t="shared" si="0"/>
-        <v>52043.122105219263</v>
+        <v>80237.463618263952</v>
       </c>
     </row>
     <row r="49" spans="3:8" x14ac:dyDescent="0.25">
@@ -15340,7 +15487,7 @@
       </c>
       <c r="H49" s="5">
         <f t="shared" si="0"/>
-        <v>52683.081391422958</v>
+        <v>84654.228941423469</v>
       </c>
     </row>
     <row r="50" spans="3:8" x14ac:dyDescent="0.25">
@@ -15349,7 +15496,7 @@
       </c>
       <c r="H50" s="5">
         <f t="shared" si="0"/>
-        <v>53174.196266760577</v>
+        <v>88701.172362658952</v>
       </c>
     </row>
     <row r="51" spans="3:8" x14ac:dyDescent="0.25">
@@ -15358,7 +15505,7 @@
       </c>
       <c r="H51" s="5">
         <f t="shared" si="0"/>
-        <v>53547.578842317911</v>
+        <v>92360.494677754701</v>
       </c>
     </row>
     <row r="52" spans="3:8" x14ac:dyDescent="0.25">
@@ -15367,7 +15514,7 @@
       </c>
       <c r="H52" s="5">
         <f t="shared" si="0"/>
-        <v>53828.712488193967</v>
+        <v>95628.538731991939</v>
       </c>
     </row>
     <row r="53" spans="3:8" x14ac:dyDescent="0.25">
@@ -15376,7 +15523,7 @@
       </c>
       <c r="H53" s="5">
         <f t="shared" si="0"/>
-        <v>54038.084983609333</v>
+        <v>98513.432469016174</v>
       </c>
     </row>
     <row r="54" spans="3:8" x14ac:dyDescent="0.25">
@@ -15385,7 +15532,7 @@
       </c>
       <c r="H54" s="5">
         <f t="shared" si="0"/>
-        <v>54191.941437103924</v>
+        <v>101032.41169433438</v>
       </c>
     </row>
     <row r="55" spans="3:8" x14ac:dyDescent="0.25">
@@ -15394,7 +15541,7 @@
       </c>
       <c r="H55" s="5">
         <f t="shared" si="0"/>
-        <v>54303.030200850721</v>
+        <v>103209.15635991676</v>
       </c>
     </row>
     <row r="56" spans="3:8" x14ac:dyDescent="0.25">
@@ -15403,7 +15550,7 @@
       </c>
       <c r="H56" s="5">
         <f t="shared" si="0"/>
-        <v>54381.278008387439</v>
+        <v>105071.37453459842</v>
       </c>
     </row>
     <row r="57" spans="3:8" x14ac:dyDescent="0.25">
@@ -15412,7 +15559,7 @@
       </c>
       <c r="H57" s="5">
         <f t="shared" si="0"/>
-        <v>54434.369280969018</v>
+        <v>106648.76761506648</v>
       </c>
     </row>
     <row r="58" spans="3:8" x14ac:dyDescent="0.25">
@@ -15421,7 +15568,7 @@
       </c>
       <c r="H58" s="5">
         <f t="shared" si="0"/>
-        <v>54468.22632919297</v>
+        <v>107971.42635255762</v>
       </c>
     </row>
     <row r="59" spans="3:8" x14ac:dyDescent="0.25">
@@ -15430,7 +15577,7 @@
       </c>
       <c r="H59" s="5">
         <f t="shared" si="0"/>
-        <v>54487.398139486926</v>
+        <v>109068.64716371786</v>
       </c>
     </row>
     <row r="60" spans="3:8" x14ac:dyDescent="0.25">
@@ -15439,7 +15586,7 @@
       </c>
       <c r="H60" s="5">
         <f t="shared" si="0"/>
-        <v>54495.369967410159</v>
+        <v>109968.12171665633</v>
       </c>
     </row>
     <row r="61" spans="3:8" x14ac:dyDescent="0.25">
@@ -15448,7 +15595,7 @@
       </c>
       <c r="H61" s="5">
         <f t="shared" si="0"/>
-        <v>54494.806940187475</v>
+        <v>110695.43561665383</v>
       </c>
     </row>
     <row r="62" spans="3:8" x14ac:dyDescent="0.25">
@@ -15457,7 +15604,7 @@
       </c>
       <c r="H62" s="5">
         <f t="shared" si="0"/>
-        <v>54487.744067601125</v>
+        <v>111273.80850978619</v>
       </c>
     </row>
     <row r="63" spans="3:8" x14ac:dyDescent="0.25">
@@ -15466,7 +15613,7 @@
       </c>
       <c r="H63" s="5">
         <f t="shared" si="0"/>
-        <v>54475.733498122783</v>
+        <v>111724.0127909053</v>
       </c>
     </row>
     <row r="64" spans="3:8" x14ac:dyDescent="0.25">
@@ -15475,7 +15622,7 @@
       </c>
       <c r="H64" s="5">
         <f t="shared" si="0"/>
-        <v>54459.958094101334</v>
+        <v>112064.41719683455</v>
       </c>
     </row>
     <row r="65" spans="3:22" x14ac:dyDescent="0.25">
@@ -15484,7 +15631,7 @@
       </c>
       <c r="H65" s="5">
         <f t="shared" si="0"/>
-        <v>54441.318715596499</v>
+        <v>112311.11203089969</v>
       </c>
     </row>
     <row r="66" spans="3:22" x14ac:dyDescent="0.25">
@@ -15493,7 +15640,7 @@
       </c>
       <c r="H66" s="5">
         <f t="shared" si="0"/>
-        <v>54420.501118300323</v>
+        <v>112478.08286949387</v>
       </c>
     </row>
     <row r="67" spans="3:22" x14ac:dyDescent="0.25">
@@ -15502,7 +15649,7 @@
       </c>
       <c r="H67" s="5">
         <f t="shared" si="0"/>
-        <v>54398.02712276802</v>
+        <v>112577.40845354805</v>
       </c>
     </row>
     <row r="68" spans="3:22" x14ac:dyDescent="0.25">
@@ -15511,7 +15658,7 @@
       </c>
       <c r="H68" s="5">
         <f t="shared" si="0"/>
-        <v>54374.293693003725</v>
+        <v>112619.46573477048</v>
       </c>
     </row>
     <row r="69" spans="3:22" x14ac:dyDescent="0.25">
@@ -15520,7 +15667,7 @@
       </c>
       <c r="H69" s="5">
         <f t="shared" si="0"/>
-        <v>54349.602746662436</v>
+        <v>112613.13072786326</v>
       </c>
     </row>
     <row r="70" spans="3:22" x14ac:dyDescent="0.25">
@@ -15529,7 +15676,7 @@
       </c>
       <c r="H70" s="5">
         <f t="shared" si="0"/>
-        <v>54324.183875110321</v>
+        <v>112565.96808629629</v>
       </c>
     </row>
     <row r="71" spans="3:22" x14ac:dyDescent="0.25">
@@ -15538,7 +15685,7 @@
       </c>
       <c r="H71" s="5">
         <f t="shared" si="0"/>
-        <v>54298.211648158132</v>
+        <v>112484.40540879617</v>
       </c>
     </row>
     <row r="72" spans="3:22" x14ac:dyDescent="0.25">
@@ -15547,7 +15694,7 @@
       </c>
       <c r="H72" s="5">
         <f t="shared" si="0"/>
-        <v>54271.818787558106</v>
+        <v>112373.89044197858</v>
       </c>
       <c r="V72" s="5"/>
     </row>
@@ -15557,7 +15704,7 @@
       </c>
       <c r="H73" s="5">
         <f t="shared" si="0"/>
-        <v>54245.106191691564</v>
+        <v>112239.03079358321</v>
       </c>
     </row>
     <row r="74" spans="3:22" x14ac:dyDescent="0.25">
@@ -15566,7 +15713,7 @@
       </c>
       <c r="H74" s="5">
         <f t="shared" si="0"/>
-        <v>54218.15056187669</v>
+        <v>112083.71669683857</v>
       </c>
     </row>
     <row r="75" spans="3:22" x14ac:dyDescent="0.25">
@@ -15575,7 +15722,7 @@
       </c>
       <c r="H75" s="5">
         <f t="shared" si="0"/>
-        <v>54191.010202821337</v>
+        <v>111911.22791812012</v>
       </c>
     </row>
     <row r="76" spans="3:22" x14ac:dyDescent="0.25">
@@ -15584,7 +15731,7 @@
       </c>
       <c r="H76" s="5">
         <f t="shared" si="0"/>
-        <v>54163.729433618711</v>
+        <v>111724.3261913434</v>
       </c>
     </row>
   </sheetData>

</xml_diff>